<commit_message>
Update listing des variables
</commit_message>
<xml_diff>
--- a/allvariables.xlsx
+++ b/allvariables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="13360" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25365" windowHeight="13365" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="nomenclature" sheetId="5" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="indexOfFunctions" sheetId="3" r:id="rId4"/>
     <sheet name="indexofArguments" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140001" iterate="1" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="212">
   <si>
     <t>name</t>
   </si>
@@ -607,6 +607,69 @@
   </si>
   <si>
     <t>incrementing function to apply</t>
+  </si>
+  <si>
+    <t>cCoefWaterstress</t>
+  </si>
+  <si>
+    <t>cPhotoDuration</t>
+  </si>
+  <si>
+    <t>sThermalUnite</t>
+  </si>
+  <si>
+    <t>sBiologicalDay</t>
+  </si>
+  <si>
+    <t>pCriticalPhotoPerdiod</t>
+  </si>
+  <si>
+    <t>pPhotoPeriodSensitivity</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>durée journalière ensoleillement</t>
+  </si>
+  <si>
+    <t>Nombre de jours dans le stade</t>
+  </si>
+  <si>
+    <t>Nombre de jours</t>
+  </si>
+  <si>
+    <t>Sensibilité de la plante à la photopériode</t>
+  </si>
+  <si>
+    <t>Seuil photopériode</t>
+  </si>
+  <si>
+    <t>pp</t>
+  </si>
+  <si>
+    <t>Photoperiod duration</t>
+  </si>
+  <si>
+    <t>Number of Daily temperature unit</t>
+  </si>
+  <si>
+    <t>Number of Biological day per calindar day</t>
+  </si>
+  <si>
+    <t>ppsen</t>
+  </si>
+  <si>
+    <t>cpp</t>
+  </si>
+  <si>
+    <t>Photoperiod sensitivity coefficient</t>
+  </si>
+  <si>
+    <t>Critical photoperiod</t>
   </si>
 </sst>
 </file>
@@ -649,7 +712,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -659,6 +722,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -689,7 +758,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -698,6 +767,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -1055,12 +1125,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="112.83203125" customWidth="1"/>
+    <col min="1" max="1" width="112.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="180">
+    <row r="1" spans="1:1" ht="189" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
@@ -1078,18 +1148,19 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1118,7 +1189,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1144,7 +1215,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1173,7 +1244,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1202,7 +1273,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1231,7 +1302,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1260,7 +1331,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1289,7 +1360,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1318,7 +1389,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -1347,7 +1418,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -1376,7 +1447,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -1405,7 +1476,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -1434,7 +1505,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -1463,7 +1534,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -1492,7 +1563,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>76</v>
       </c>
@@ -1521,9 +1592,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>191</v>
       </c>
       <c r="B16" t="s">
         <v>42</v>
@@ -1550,7 +1621,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>91</v>
       </c>
@@ -1579,7 +1650,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>101</v>
       </c>
@@ -1608,7 +1679,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>110</v>
       </c>
@@ -1637,7 +1708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>115</v>
       </c>
@@ -1666,7 +1737,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>116</v>
       </c>
@@ -1695,7 +1766,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>130</v>
       </c>
@@ -1724,7 +1795,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>105</v>
       </c>
@@ -1753,7 +1824,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -1782,7 +1853,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>139</v>
       </c>
@@ -1811,7 +1882,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>140</v>
       </c>
@@ -1840,7 +1911,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>141</v>
       </c>
@@ -1869,7 +1940,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>142</v>
       </c>
@@ -1898,7 +1969,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="4" customFormat="1">
+    <row r="29" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>155</v>
       </c>
@@ -1924,7 +1995,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>156</v>
       </c>
@@ -1950,7 +2021,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>166</v>
       </c>
@@ -1979,7 +2050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>172</v>
       </c>
@@ -2005,7 +2076,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>178</v>
       </c>
@@ -2024,8 +2095,11 @@
       <c r="F33" s="3" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="I33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>181</v>
       </c>
@@ -2044,8 +2118,11 @@
       <c r="F34" s="3" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="I34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>182</v>
       </c>
@@ -2064,8 +2141,11 @@
       <c r="F35" s="3" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="I35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>188</v>
       </c>
@@ -2084,9 +2164,154 @@
       <c r="F36" s="3" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="E37" s="4"/>
+      <c r="I36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>192</v>
+      </c>
+      <c r="B37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" t="s">
+        <v>98</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="G37" t="s">
+        <v>204</v>
+      </c>
+      <c r="H37" t="s">
+        <v>199</v>
+      </c>
+      <c r="I37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>193</v>
+      </c>
+      <c r="B38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" t="s">
+        <v>98</v>
+      </c>
+      <c r="E38" t="s">
+        <v>125</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="G38" t="s">
+        <v>79</v>
+      </c>
+      <c r="H38" t="s">
+        <v>200</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>194</v>
+      </c>
+      <c r="B39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" t="s">
+        <v>98</v>
+      </c>
+      <c r="E39" t="s">
+        <v>125</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G39" t="s">
+        <v>102</v>
+      </c>
+      <c r="H39" t="s">
+        <v>201</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" t="s">
+        <v>98</v>
+      </c>
+      <c r="E40" t="s">
+        <v>197</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="G40" t="s">
+        <v>209</v>
+      </c>
+      <c r="H40" t="s">
+        <v>203</v>
+      </c>
+      <c r="I40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="B41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" t="s">
+        <v>98</v>
+      </c>
+      <c r="E41" t="s">
+        <v>198</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H41" t="s">
+        <v>202</v>
+      </c>
+      <c r="I41" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2106,7 +2331,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -2126,9 +2351,9 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -2154,52 +2379,52 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>170</v>
       </c>
@@ -2223,14 +2448,14 @@
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -2241,7 +2466,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>81</v>
       </c>
@@ -2252,7 +2477,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -2263,7 +2488,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>81</v>
       </c>
@@ -2274,7 +2499,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>81</v>
       </c>
@@ -2285,7 +2510,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -2296,7 +2521,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -2307,7 +2532,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>82</v>
       </c>
@@ -2318,7 +2543,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -2329,7 +2554,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>109</v>
       </c>
@@ -2340,7 +2565,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>109</v>
       </c>
@@ -2351,7 +2576,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>109</v>
       </c>
@@ -2362,7 +2587,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>109</v>
       </c>
@@ -2373,7 +2598,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -2384,7 +2609,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -2395,7 +2620,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -2406,7 +2631,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>118</v>
       </c>
@@ -2417,7 +2642,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -2428,7 +2653,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>118</v>
       </c>
@@ -2439,7 +2664,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>117</v>
       </c>
@@ -2450,7 +2675,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>117</v>
       </c>
@@ -2461,7 +2686,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -2472,7 +2697,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -2483,7 +2708,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>135</v>
       </c>
@@ -2494,7 +2719,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>135</v>
       </c>
@@ -2505,7 +2730,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>165</v>
       </c>
@@ -2516,7 +2741,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>165</v>
       </c>
@@ -2527,7 +2752,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>165</v>
       </c>
@@ -2538,7 +2763,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>165</v>
       </c>
@@ -2549,7 +2774,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>165</v>
       </c>
@@ -2560,7 +2785,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>170</v>
       </c>
@@ -2571,7 +2796,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>170</v>
       </c>
@@ -2582,7 +2807,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>170</v>
       </c>

</xml_diff>

<commit_message>
merge from LAI Branch
</commit_message>
<xml_diff>
--- a/allvariables.xlsx
+++ b/allvariables.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="249">
   <si>
     <t>name</t>
   </si>
@@ -671,12 +671,123 @@
   <si>
     <t>Critical photoperiod</t>
   </si>
+  <si>
+    <t>sLAI</t>
+  </si>
+  <si>
+    <t>LAI</t>
+  </si>
+  <si>
+    <t>GLAI</t>
+  </si>
+  <si>
+    <t>DLAI</t>
+  </si>
+  <si>
+    <t>m2 m-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leaf area index </t>
+  </si>
+  <si>
+    <t>Index de surface foliaire</t>
+  </si>
+  <si>
+    <t>m2 m-2 d-1</t>
+  </si>
+  <si>
+    <t>Daily increase (growth) in leaf area index</t>
+  </si>
+  <si>
+    <t>cGrowthLAI</t>
+  </si>
+  <si>
+    <t>Daily decrease (death) in leaf area index</t>
+  </si>
+  <si>
+    <t>Croissance de la surface foliaire</t>
+  </si>
+  <si>
+    <t>Décroissance de la surface foliaire</t>
+  </si>
+  <si>
+    <t>cDecreaseLAI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily rate of nitrogen mobilized from leaves </t>
+  </si>
+  <si>
+    <t>g N m-2 d-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XNLF </t>
+  </si>
+  <si>
+    <t>Taux d'azote mobilisable depuis les feuilles</t>
+  </si>
+  <si>
+    <t>cDailyRateNfromLeave</t>
+  </si>
+  <si>
+    <t>Specific leaf nitrogen in green leaves (target)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLNG </t>
+  </si>
+  <si>
+    <t>g N m-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLNS </t>
+  </si>
+  <si>
+    <t>Specific leaf nitrogen in senesced leaves (minimum)</t>
+  </si>
+  <si>
+    <t>pSpecLeafNGreenLeaf</t>
+  </si>
+  <si>
+    <t>pSpecLeafNSenescenceLeaf</t>
+  </si>
+  <si>
+    <t>Azote spécifique des feuilles dans les feuilles vertes</t>
+  </si>
+  <si>
+    <t>Azote spécifique des feuilles dans les feuilles mortes</t>
+  </si>
+  <si>
+    <t>pFreezeThresholdTemp</t>
+  </si>
+  <si>
+    <t>Fraction leaf destruction below the critical by each degree centigrad</t>
+  </si>
+  <si>
+    <t>Critical minimum temp for leaf destruction due to frosts</t>
+  </si>
+  <si>
+    <t>Température seuil sous laquelle il y a destruction de feuille</t>
+  </si>
+  <si>
+    <t>Fraction de la feuille détruite par le gel par degré sous le seuil critique</t>
+  </si>
+  <si>
+    <t>m2 m-2 °C-1</t>
+  </si>
+  <si>
+    <t>pFreezeFracLeafDestruction</t>
+  </si>
+  <si>
+    <t>FRZTKIL</t>
+  </si>
+  <si>
+    <t>FRZLDR</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -711,8 +822,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -728,6 +845,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -758,7 +881,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -768,6 +891,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -1148,10 +1278,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2310,6 +2440,238 @@
         <v>202</v>
       </c>
       <c r="I41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>212</v>
+      </c>
+      <c r="B42" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" t="s">
+        <v>213</v>
+      </c>
+      <c r="E42" t="s">
+        <v>216</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="G42" t="s">
+        <v>213</v>
+      </c>
+      <c r="H42" t="s">
+        <v>218</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>221</v>
+      </c>
+      <c r="B43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" t="s">
+        <v>213</v>
+      </c>
+      <c r="E43" t="s">
+        <v>219</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="G43" t="s">
+        <v>214</v>
+      </c>
+      <c r="H43" t="s">
+        <v>223</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>225</v>
+      </c>
+      <c r="B44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" t="s">
+        <v>213</v>
+      </c>
+      <c r="E44" t="s">
+        <v>219</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="G44" t="s">
+        <v>215</v>
+      </c>
+      <c r="H44" t="s">
+        <v>224</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>230</v>
+      </c>
+      <c r="B45" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" t="s">
+        <v>213</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="H45" t="s">
+        <v>229</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>236</v>
+      </c>
+      <c r="B46" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" t="s">
+        <v>213</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H46" t="s">
+        <v>238</v>
+      </c>
+      <c r="I46" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>237</v>
+      </c>
+      <c r="B47" t="s">
+        <v>36</v>
+      </c>
+      <c r="C47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" t="s">
+        <v>213</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="H47" t="s">
+        <v>239</v>
+      </c>
+      <c r="I47" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>240</v>
+      </c>
+      <c r="B48" t="s">
+        <v>36</v>
+      </c>
+      <c r="C48" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" t="s">
+        <v>213</v>
+      </c>
+      <c r="E48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="G48" t="s">
+        <v>247</v>
+      </c>
+      <c r="H48" t="s">
+        <v>243</v>
+      </c>
+      <c r="I48" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>246</v>
+      </c>
+      <c r="B49" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" t="s">
+        <v>213</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="G49" t="s">
+        <v>248</v>
+      </c>
+      <c r="H49" t="s">
+        <v>244</v>
+      </c>
+      <c r="I49" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update of xls files
</commit_message>
<xml_diff>
--- a/allvariables.xlsx
+++ b/allvariables.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="246">
   <si>
     <t>name</t>
   </si>
@@ -568,15 +568,6 @@
   </si>
   <si>
     <t>character</t>
-  </si>
-  <si>
-    <t>sCumulatedPhenoCounts</t>
-  </si>
-  <si>
-    <t>arbitrary(depends on the counter)</t>
-  </si>
-  <si>
-    <t>cumulated "growth units" accumulated since the beginning of the stage</t>
   </si>
   <si>
     <t>sCrop</t>
@@ -1278,10 +1269,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1724,7 +1715,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B16" t="s">
         <v>42</v>
@@ -2211,19 +2202,19 @@
         <v>178</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>26</v>
+        <v>177</v>
       </c>
       <c r="D33" t="s">
-        <v>98</v>
+        <v>180</v>
       </c>
       <c r="E33" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="I33" t="s">
         <v>39</v>
@@ -2231,7 +2222,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B34" t="s">
         <v>5</v>
@@ -2240,13 +2231,13 @@
         <v>177</v>
       </c>
       <c r="D34" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E34" t="s">
+        <v>182</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>186</v>
       </c>
       <c r="I34" t="s">
         <v>39</v>
@@ -2254,19 +2245,19 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="C35" t="s">
         <v>177</v>
       </c>
       <c r="D35" t="s">
-        <v>183</v>
+        <v>98</v>
       </c>
       <c r="E35" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>187</v>
@@ -2277,22 +2268,28 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B36" t="s">
         <v>42</v>
       </c>
       <c r="C36" t="s">
-        <v>177</v>
+        <v>26</v>
       </c>
       <c r="D36" t="s">
         <v>98</v>
       </c>
-      <c r="E36" t="s">
-        <v>189</v>
+      <c r="E36" s="4" t="s">
+        <v>194</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>190</v>
+        <v>202</v>
+      </c>
+      <c r="G36" t="s">
+        <v>201</v>
+      </c>
+      <c r="H36" t="s">
+        <v>196</v>
       </c>
       <c r="I36" t="s">
         <v>39</v>
@@ -2300,7 +2297,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B37" t="s">
         <v>42</v>
@@ -2311,25 +2308,25 @@
       <c r="D37" t="s">
         <v>98</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" t="s">
+        <v>125</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="G37" t="s">
+        <v>79</v>
+      </c>
+      <c r="H37" t="s">
         <v>197</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="G37" t="s">
-        <v>204</v>
-      </c>
-      <c r="H37" t="s">
-        <v>199</v>
-      </c>
-      <c r="I37" t="s">
-        <v>39</v>
+      <c r="I37">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B38" t="s">
         <v>42</v>
@@ -2344,24 +2341,24 @@
         <v>125</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G38" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="H38" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I38">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>194</v>
+      <c r="A39" s="6" t="s">
+        <v>192</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C39" t="s">
         <v>26</v>
@@ -2370,24 +2367,24 @@
         <v>98</v>
       </c>
       <c r="E39" t="s">
-        <v>125</v>
+        <v>194</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G39" t="s">
-        <v>102</v>
+        <v>206</v>
       </c>
       <c r="H39" t="s">
-        <v>201</v>
-      </c>
-      <c r="I39">
-        <v>0</v>
+        <v>200</v>
+      </c>
+      <c r="I39" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B40" t="s">
         <v>36</v>
@@ -2399,53 +2396,53 @@
         <v>98</v>
       </c>
       <c r="E40" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="G40" t="s">
+        <v>207</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="H40" t="s">
+        <v>199</v>
+      </c>
+      <c r="I40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>209</v>
       </c>
-      <c r="H40" t="s">
-        <v>203</v>
-      </c>
-      <c r="I40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>196</v>
-      </c>
       <c r="B41" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C41" t="s">
         <v>26</v>
       </c>
       <c r="D41" t="s">
-        <v>98</v>
+        <v>210</v>
       </c>
       <c r="E41" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="F41" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="G41" t="s">
         <v>210</v>
       </c>
-      <c r="G41" s="3" t="s">
-        <v>208</v>
-      </c>
       <c r="H41" t="s">
-        <v>202</v>
-      </c>
-      <c r="I41" t="s">
-        <v>39</v>
+        <v>215</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="B42" t="s">
         <v>42</v>
@@ -2454,7 +2451,7 @@
         <v>26</v>
       </c>
       <c r="D42" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E42" t="s">
         <v>216</v>
@@ -2463,10 +2460,10 @@
         <v>217</v>
       </c>
       <c r="G42" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H42" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="I42">
         <v>0</v>
@@ -2474,7 +2471,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B43" t="s">
         <v>42</v>
@@ -2483,19 +2480,19 @@
         <v>26</v>
       </c>
       <c r="D43" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E43" t="s">
+        <v>216</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="F43" s="3" t="s">
-        <v>220</v>
-      </c>
       <c r="G43" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H43" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I43">
         <v>0</v>
@@ -2503,7 +2500,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B44" t="s">
         <v>42</v>
@@ -2512,19 +2509,19 @@
         <v>26</v>
       </c>
       <c r="D44" t="s">
-        <v>213</v>
-      </c>
-      <c r="E44" t="s">
-        <v>219</v>
+        <v>210</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>224</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="G44" t="s">
-        <v>215</v>
+        <v>223</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>225</v>
       </c>
       <c r="H44" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="I44">
         <v>0</v>
@@ -2532,36 +2529,36 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>233</v>
+      </c>
+      <c r="B45" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" t="s">
+        <v>210</v>
+      </c>
+      <c r="E45" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="B45" t="s">
-        <v>42</v>
-      </c>
-      <c r="C45" t="s">
-        <v>26</v>
-      </c>
-      <c r="D45" t="s">
-        <v>213</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>227</v>
-      </c>
       <c r="F45" s="3" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H45" t="s">
-        <v>229</v>
-      </c>
-      <c r="I45">
-        <v>0</v>
+        <v>235</v>
+      </c>
+      <c r="I45" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B46" t="s">
         <v>36</v>
@@ -2570,19 +2567,19 @@
         <v>26</v>
       </c>
       <c r="D46" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F46" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G46" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="G46" s="3" t="s">
-        <v>232</v>
-      </c>
       <c r="H46" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="I46" t="s">
         <v>39</v>
@@ -2599,19 +2596,19 @@
         <v>26</v>
       </c>
       <c r="D47" t="s">
-        <v>213</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>234</v>
+        <v>210</v>
+      </c>
+      <c r="E47" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="G47" t="s">
+        <v>244</v>
       </c>
       <c r="H47" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="I47" t="s">
         <v>39</v>
@@ -2619,7 +2616,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B48" t="s">
         <v>36</v>
@@ -2628,50 +2625,21 @@
         <v>26</v>
       </c>
       <c r="D48" t="s">
-        <v>213</v>
-      </c>
-      <c r="E48" t="s">
-        <v>15</v>
+        <v>210</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>242</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="G48" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H48" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I48" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>246</v>
-      </c>
-      <c r="B49" t="s">
-        <v>36</v>
-      </c>
-      <c r="C49" t="s">
-        <v>26</v>
-      </c>
-      <c r="D49" t="s">
-        <v>213</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="G49" t="s">
-        <v>248</v>
-      </c>
-      <c r="H49" t="s">
-        <v>244</v>
-      </c>
-      <c r="I49" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mise à jour de la liste des variables (prise en compte pour DM production et LAI)
</commit_message>
<xml_diff>
--- a/allvariables.xlsx
+++ b/allvariables.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="319">
   <si>
     <t>name</t>
   </si>
@@ -600,9 +600,6 @@
     <t>incrementing function to apply</t>
   </si>
   <si>
-    <t>cCoefWaterstress</t>
-  </si>
-  <si>
     <t>cPhotoDuration</t>
   </si>
   <si>
@@ -772,6 +769,228 @@
   </si>
   <si>
     <t>FRZLDR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phyllochron </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pPhyllochron </t>
+  </si>
+  <si>
+    <t xml:space="preserve">oC per leaf </t>
+  </si>
+  <si>
+    <t>PHYL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mainstem node number </t>
+  </si>
+  <si>
+    <t>MSNN</t>
+  </si>
+  <si>
+    <t>numéro du nœud de la tige principale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sMainstemNodeNumber </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLACON </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A coefficient (constant) in power relationship between plant leaf area and mainstem node number </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLAPOW </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A coefficient (exponent) in power relationship between plant leaf area and mainstem node number </t>
+  </si>
+  <si>
+    <t>pcoefPlantLeafNumberNode</t>
+  </si>
+  <si>
+    <t>pExpPlantLeafNumberNode</t>
+  </si>
+  <si>
+    <t>Coefficient d'une loi puissance entre le nombre de feuilles et le nombre de nœuds</t>
+  </si>
+  <si>
+    <t>Exposant d'une loi puissance entre le nombre de feuilles et le nombre de nœuds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDEN </t>
+  </si>
+  <si>
+    <t># m-2</t>
+  </si>
+  <si>
+    <t>Plant density</t>
+  </si>
+  <si>
+    <t>Densité de semis</t>
+  </si>
+  <si>
+    <t>pPlantdensity</t>
+  </si>
+  <si>
+    <t>cCoefWaterstressDevelopment</t>
+  </si>
+  <si>
+    <t>cCoefWaterstressLeaf</t>
+  </si>
+  <si>
+    <t>WSFL</t>
+  </si>
+  <si>
+    <t>Water stress factor for leaf</t>
+  </si>
+  <si>
+    <t>facteur limitant des feuilles lié au stress hydrique</t>
+  </si>
+  <si>
+    <t>Plant leaf area today</t>
+  </si>
+  <si>
+    <t>PLA2</t>
+  </si>
+  <si>
+    <t>cm2 per plant</t>
+  </si>
+  <si>
+    <t>Surface follière</t>
+  </si>
+  <si>
+    <t>cPlantLeafArea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLF </t>
+  </si>
+  <si>
+    <t>g m-2 d-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily increase (growth) in leaf weight </t>
+  </si>
+  <si>
+    <t>cDailyLeafWeight</t>
+  </si>
+  <si>
+    <t>poids des feuilles du jours</t>
+  </si>
+  <si>
+    <t>DMProduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specific leaf area </t>
+  </si>
+  <si>
+    <t>SLA</t>
+  </si>
+  <si>
+    <t>pSpecificLeafArea</t>
+  </si>
+  <si>
+    <t>m2 g-1</t>
+  </si>
+  <si>
+    <t>suface spécifique des feuilles</t>
+  </si>
+  <si>
+    <t>cEndCropCycle</t>
+  </si>
+  <si>
+    <t>Stage of the culture: in Progress, death, harvested</t>
+  </si>
+  <si>
+    <t>MATYP</t>
+  </si>
+  <si>
+    <t>Etat de la culture: en cours, morte, récoltée</t>
+  </si>
+  <si>
+    <t>PlantN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRUE </t>
+  </si>
+  <si>
+    <t>g MJ-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radiation use efficiency under optimal growth conditions </t>
+  </si>
+  <si>
+    <t>DMDistribution</t>
+  </si>
+  <si>
+    <t>pRadEffiencyOptimal</t>
+  </si>
+  <si>
+    <t>Efficacité d'utilisation des radiations dans des conditions de croissance optimales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCFRUE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">oC  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A correction factor of radiation use efficiency for daily temperature </t>
+  </si>
+  <si>
+    <t>facteur de correction de l'efficacité d'utilisation du rayonnement pour la température journalière</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUE </t>
+  </si>
+  <si>
+    <t>Radiation use efficiency adjusted for temperature and water stress</t>
+  </si>
+  <si>
+    <t>cRadiationUseEffiency</t>
+  </si>
+  <si>
+    <t>cCoefRadiationEffiency</t>
+  </si>
+  <si>
+    <t>Efficacité d'utilisation des radiations ajustée à la température et au stress hydrique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WSFG </t>
+  </si>
+  <si>
+    <t>Water stress factor for growth (dry matter production)</t>
+  </si>
+  <si>
+    <t>cCoefWaterstressDryMatter</t>
+  </si>
+  <si>
+    <t>SoiWater</t>
+  </si>
+  <si>
+    <t>Facteur de stress hydrique pour la croissance (production de matière sèche)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPAR </t>
+  </si>
+  <si>
+    <t>Extinction coefficient for photosyntheticaly active radiation (PAR)</t>
+  </si>
+  <si>
+    <t>Coefficient d'extinction pour le rayonnement actif photosynthétiquement (PAR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DDMP </t>
+  </si>
+  <si>
+    <t>Daily dry matter production</t>
+  </si>
+  <si>
+    <t>cDryMatterProduction</t>
+  </si>
+  <si>
+    <t>Production journalière de matière sèche</t>
   </si>
 </sst>
 </file>
@@ -1269,10 +1488,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1715,7 +1934,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>188</v>
+        <v>266</v>
       </c>
       <c r="B16" t="s">
         <v>42</v>
@@ -1724,7 +1943,7 @@
         <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>98</v>
+        <v>310</v>
       </c>
       <c r="E16" t="s">
         <v>174</v>
@@ -1738,8 +1957,8 @@
       <c r="H16" t="s">
         <v>97</v>
       </c>
-      <c r="I16" t="s">
-        <v>39</v>
+      <c r="I16">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2268,7 +2487,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B36" t="s">
         <v>42</v>
@@ -2280,16 +2499,16 @@
         <v>98</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G36" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H36" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I36" t="s">
         <v>39</v>
@@ -2297,7 +2516,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B37" t="s">
         <v>42</v>
@@ -2312,13 +2531,13 @@
         <v>125</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G37" t="s">
         <v>79</v>
       </c>
       <c r="H37" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -2326,7 +2545,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B38" t="s">
         <v>42</v>
@@ -2341,13 +2560,13 @@
         <v>125</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G38" t="s">
         <v>102</v>
       </c>
       <c r="H38" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I38">
         <v>0</v>
@@ -2355,7 +2574,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B39" t="s">
         <v>36</v>
@@ -2367,16 +2586,16 @@
         <v>98</v>
       </c>
       <c r="E39" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H39" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I39" t="s">
         <v>39</v>
@@ -2384,7 +2603,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B40" t="s">
         <v>36</v>
@@ -2396,16 +2615,16 @@
         <v>98</v>
       </c>
       <c r="E40" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H40" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I40" t="s">
         <v>39</v>
@@ -2413,7 +2632,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B41" t="s">
         <v>42</v>
@@ -2422,19 +2641,19 @@
         <v>26</v>
       </c>
       <c r="D41" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E41" t="s">
+        <v>212</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="G41" t="s">
+        <v>209</v>
+      </c>
+      <c r="H41" t="s">
         <v>214</v>
-      </c>
-      <c r="G41" t="s">
-        <v>210</v>
-      </c>
-      <c r="H41" t="s">
-        <v>215</v>
       </c>
       <c r="I41">
         <v>0</v>
@@ -2442,7 +2661,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B42" t="s">
         <v>42</v>
@@ -2451,19 +2670,19 @@
         <v>26</v>
       </c>
       <c r="D42" t="s">
+        <v>209</v>
+      </c>
+      <c r="E42" t="s">
+        <v>215</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="G42" t="s">
         <v>210</v>
       </c>
-      <c r="E42" t="s">
-        <v>216</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="G42" t="s">
-        <v>211</v>
-      </c>
       <c r="H42" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I42">
         <v>0</v>
@@ -2471,7 +2690,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B43" t="s">
         <v>42</v>
@@ -2480,19 +2699,19 @@
         <v>26</v>
       </c>
       <c r="D43" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E43" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G43" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H43" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I43">
         <v>0</v>
@@ -2500,7 +2719,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B44" t="s">
         <v>42</v>
@@ -2509,19 +2728,19 @@
         <v>26</v>
       </c>
       <c r="D44" t="s">
-        <v>210</v>
+        <v>291</v>
       </c>
       <c r="E44" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="G44" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="F44" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="G44" s="3" t="s">
+      <c r="H44" t="s">
         <v>225</v>
-      </c>
-      <c r="H44" t="s">
-        <v>226</v>
       </c>
       <c r="I44">
         <v>0</v>
@@ -2529,7 +2748,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B45" t="s">
         <v>36</v>
@@ -2538,19 +2757,19 @@
         <v>26</v>
       </c>
       <c r="D45" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F45" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G45" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="G45" s="3" t="s">
-        <v>229</v>
-      </c>
       <c r="H45" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I45" t="s">
         <v>39</v>
@@ -2558,7 +2777,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B46" t="s">
         <v>36</v>
@@ -2567,19 +2786,19 @@
         <v>26</v>
       </c>
       <c r="D46" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E46" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G46" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="F46" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>231</v>
-      </c>
       <c r="H46" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I46" t="s">
         <v>39</v>
@@ -2587,7 +2806,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B47" t="s">
         <v>36</v>
@@ -2596,19 +2815,19 @@
         <v>26</v>
       </c>
       <c r="D47" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E47" t="s">
         <v>15</v>
       </c>
       <c r="F47" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="G47" t="s">
+        <v>243</v>
+      </c>
+      <c r="H47" t="s">
         <v>239</v>
-      </c>
-      <c r="G47" t="s">
-        <v>244</v>
-      </c>
-      <c r="H47" t="s">
-        <v>240</v>
       </c>
       <c r="I47" t="s">
         <v>39</v>
@@ -2616,7 +2835,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B48" t="s">
         <v>36</v>
@@ -2625,21 +2844,482 @@
         <v>26</v>
       </c>
       <c r="D48" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G48" t="s">
+        <v>244</v>
+      </c>
+      <c r="H48" t="s">
+        <v>240</v>
+      </c>
+      <c r="I48" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>246</v>
+      </c>
+      <c r="B49" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" t="s">
+        <v>209</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="F49" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H48" t="s">
-        <v>241</v>
-      </c>
-      <c r="I48" t="s">
+      <c r="G49" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="I49" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>252</v>
+      </c>
+      <c r="B50" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" t="s">
+        <v>209</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="H50" t="s">
+        <v>251</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>257</v>
+      </c>
+      <c r="B51" t="s">
+        <v>36</v>
+      </c>
+      <c r="C51" t="s">
+        <v>26</v>
+      </c>
+      <c r="D51" t="s">
+        <v>209</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="H51" t="s">
+        <v>259</v>
+      </c>
+      <c r="I51" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>258</v>
+      </c>
+      <c r="B52" t="s">
+        <v>36</v>
+      </c>
+      <c r="C52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D52" t="s">
+        <v>209</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="H52" t="s">
+        <v>260</v>
+      </c>
+      <c r="I52" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>265</v>
+      </c>
+      <c r="B53" t="s">
+        <v>36</v>
+      </c>
+      <c r="C53" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" t="s">
+        <v>209</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="H53" t="s">
+        <v>264</v>
+      </c>
+      <c r="I53" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>267</v>
+      </c>
+      <c r="B54" t="s">
+        <v>42</v>
+      </c>
+      <c r="C54" t="s">
+        <v>26</v>
+      </c>
+      <c r="D54" t="s">
+        <v>310</v>
+      </c>
+      <c r="E54" t="s">
+        <v>174</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="G54" t="s">
+        <v>268</v>
+      </c>
+      <c r="H54" t="s">
+        <v>270</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B55" t="s">
+        <v>42</v>
+      </c>
+      <c r="C55" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55" t="s">
+        <v>209</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="H55" t="s">
+        <v>274</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>279</v>
+      </c>
+      <c r="B56" t="s">
+        <v>42</v>
+      </c>
+      <c r="C56" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56" t="s">
+        <v>295</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="H56" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>284</v>
+      </c>
+      <c r="B57" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57" t="s">
+        <v>26</v>
+      </c>
+      <c r="D57" t="s">
+        <v>209</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="H57" t="s">
+        <v>286</v>
+      </c>
+      <c r="I57" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>287</v>
+      </c>
+      <c r="B58" t="s">
+        <v>42</v>
+      </c>
+      <c r="C58" t="s">
+        <v>26</v>
+      </c>
+      <c r="D58" t="s">
+        <v>32</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="H58" t="s">
+        <v>290</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>296</v>
+      </c>
+      <c r="B59" t="s">
+        <v>36</v>
+      </c>
+      <c r="C59" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" t="s">
+        <v>281</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="H59" t="s">
+        <v>297</v>
+      </c>
+      <c r="I59" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>305</v>
+      </c>
+      <c r="B60" t="s">
+        <v>42</v>
+      </c>
+      <c r="C60" t="s">
+        <v>26</v>
+      </c>
+      <c r="D60" t="s">
+        <v>281</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="H60" t="s">
+        <v>301</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>304</v>
+      </c>
+      <c r="B61" t="s">
+        <v>42</v>
+      </c>
+      <c r="C61" t="s">
+        <v>26</v>
+      </c>
+      <c r="D61" t="s">
+        <v>281</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="H61" t="s">
+        <v>306</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>309</v>
+      </c>
+      <c r="B62" t="s">
+        <v>42</v>
+      </c>
+      <c r="C62" t="s">
+        <v>26</v>
+      </c>
+      <c r="D62" t="s">
+        <v>310</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="H62" t="s">
+        <v>311</v>
+      </c>
+      <c r="I62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="B63" t="s">
+        <v>36</v>
+      </c>
+      <c r="C63" t="s">
+        <v>26</v>
+      </c>
+      <c r="D63" t="s">
+        <v>281</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="H63" t="s">
+        <v>314</v>
+      </c>
+      <c r="I63" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>317</v>
+      </c>
+      <c r="B64" t="s">
+        <v>42</v>
+      </c>
+      <c r="C64" t="s">
+        <v>26</v>
+      </c>
+      <c r="D64" t="s">
+        <v>281</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="H64" t="s">
+        <v>318</v>
+      </c>
+      <c r="I64" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
progress on water balance (TEP etc..)
</commit_message>
<xml_diff>
--- a/allvariables.xlsx
+++ b/allvariables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7760" yWindow="0" windowWidth="24720" windowHeight="18900" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="11660" yWindow="1740" windowWidth="24720" windowHeight="18900" tabRatio="652" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="nomenclature" sheetId="5" r:id="rId1"/>
@@ -12,8 +12,9 @@
     <sheet name="other" sheetId="2" r:id="rId3"/>
     <sheet name="indexOfFunctions" sheetId="3" r:id="rId4"/>
     <sheet name="indexofArguments" sheetId="4" r:id="rId5"/>
+    <sheet name="generalPhysicalParameters" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="491">
   <si>
     <t>name</t>
   </si>
@@ -1290,9 +1291,6 @@
     <t>SoilParameter</t>
   </si>
   <si>
-    <t>residual water content when the soil is dryed by evaporation in layer 10</t>
-  </si>
-  <si>
     <t>eau résiduelle du sol sec couche 10</t>
   </si>
   <si>
@@ -1314,15 +1312,6 @@
     <t>SAT(L)</t>
   </si>
   <si>
-    <t>water content at wilting point layer 10</t>
-  </si>
-  <si>
-    <t>water content at field capacity later 10</t>
-  </si>
-  <si>
-    <t>water content at full saturation layer 10</t>
-  </si>
-  <si>
     <t>saturation couche 10</t>
   </si>
   <si>
@@ -1338,9 +1327,6 @@
     <t xml:space="preserve">Potential daily increase (growth) in root depth </t>
   </si>
   <si>
-    <t>thickness soil layer 1</t>
-  </si>
-  <si>
     <t>GRTDP</t>
   </si>
   <si>
@@ -1414,6 +1400,114 @@
   </si>
   <si>
     <t>pKPAR</t>
+  </si>
+  <si>
+    <t>EOSMIN</t>
+  </si>
+  <si>
+    <t>pMinimalSoilEvaporation</t>
+  </si>
+  <si>
+    <t>Minimal Soil Evaporation</t>
+  </si>
+  <si>
+    <t>evaporation minimale du sol</t>
+  </si>
+  <si>
+    <t>WETWAT</t>
+  </si>
+  <si>
+    <t>KET</t>
+  </si>
+  <si>
+    <t>CALB</t>
+  </si>
+  <si>
+    <t>canopy extinction coefficient</t>
+  </si>
+  <si>
+    <t>pCanopyExtinctionCoefficient</t>
+  </si>
+  <si>
+    <t>pCropAlbedo</t>
+  </si>
+  <si>
+    <t>Crop albedo</t>
+  </si>
+  <si>
+    <t>amount of rainfall and/or irrigation required to wet the top soil layer to return soil evaporation from Stage II to Stage I</t>
+  </si>
+  <si>
+    <t>pSoilAlbedo</t>
+  </si>
+  <si>
+    <t>SALB</t>
+  </si>
+  <si>
+    <t>Soil Albedo</t>
+  </si>
+  <si>
+    <t>albedo du sol</t>
+  </si>
+  <si>
+    <t>STBLW</t>
+  </si>
+  <si>
+    <t>pStubleWeight</t>
+  </si>
+  <si>
+    <t>stubble weight left on the soil (has an impact on soil evaporation)</t>
+  </si>
+  <si>
+    <t>ITKParameter</t>
+  </si>
+  <si>
+    <t>t.ha-1</t>
+  </si>
+  <si>
+    <t>poids du mulch laissé en surface</t>
+  </si>
+  <si>
+    <t>thickness soil layer (columns = cases, rows: layers)</t>
+  </si>
+  <si>
+    <t>water content at full saturation  (columns = cases, rows: layers)</t>
+  </si>
+  <si>
+    <t>water content at field capacity  (columns = cases, rows: layers)</t>
+  </si>
+  <si>
+    <t>water content at wilting point  (columns = cases, rows: layers)</t>
+  </si>
+  <si>
+    <t>residual water content when the soil is dryed by evaporation  (columns = cases, rows: layers)</t>
+  </si>
+  <si>
+    <t>pSoilWettingWaterQuantity</t>
+  </si>
+  <si>
+    <t>sDaysSinceSoilWettingWater</t>
+  </si>
+  <si>
+    <t>days since the last sufficient water amount to wet the soil (to go from stage II soil evaporation to stage I soil evaporation</t>
+  </si>
+  <si>
+    <t>DYSE</t>
+  </si>
+  <si>
+    <t>nombre de jours depuis la dernière arrivée d'eau suffisante pour mouiller le sol (passer de stade II à stade I pour l'évaporation)</t>
+  </si>
+  <si>
+    <t>cSoilEvaporation</t>
+  </si>
+  <si>
+    <t>soil evaporation</t>
+  </si>
+  <si>
+    <t>SEVP</t>
+  </si>
+  <si>
+    <t>évaporation du sol</t>
   </si>
 </sst>
 </file>
@@ -1518,8 +1612,60 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="165">
+  <cellStyleXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1713,7 +1859,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="165">
+  <cellStyles count="217">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -1796,6 +1942,32 @@
     <cellStyle name="Lien hypertexte" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="215" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -1878,6 +2050,32 @@
     <cellStyle name="Lien hypertexte visité" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="216" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2242,13 +2440,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:I97"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A49" sqref="A49"/>
+      <selection pane="bottomRight" activeCell="I99" sqref="I99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3603,7 +3801,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="3" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="B48" t="s">
         <v>143</v>
@@ -4597,29 +4795,28 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>34</v>
+        <v>251</v>
       </c>
       <c r="B83" t="s">
-        <v>36</v>
+        <v>474</v>
       </c>
       <c r="C83" t="s">
         <v>26</v>
       </c>
       <c r="D83" t="s">
-        <v>37</v>
-      </c>
-      <c r="E83" t="s">
-        <v>168</v>
-      </c>
-      <c r="F83" t="s">
-        <v>38</v>
-      </c>
-      <c r="G83" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+        <v>203</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>382</v>
       </c>
       <c r="H83" t="s">
-        <v>39</v>
+        <v>250</v>
       </c>
       <c r="I83" t="e">
         <f>NA()</f>
@@ -4628,28 +4825,28 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>251</v>
+        <v>383</v>
       </c>
       <c r="B84" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C84" t="s">
         <v>26</v>
       </c>
       <c r="D84" t="s">
-        <v>203</v>
-      </c>
-      <c r="E84" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>382</v>
+        <v>393</v>
+      </c>
+      <c r="E84" t="s">
+        <v>394</v>
+      </c>
+      <c r="F84" t="s">
+        <v>395</v>
+      </c>
+      <c r="G84" t="s">
+        <v>405</v>
       </c>
       <c r="H84" t="s">
-        <v>250</v>
+        <v>406</v>
       </c>
       <c r="I84" t="e">
         <f>NA()</f>
@@ -4658,7 +4855,7 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B85" t="s">
         <v>41</v>
@@ -4673,13 +4870,13 @@
         <v>394</v>
       </c>
       <c r="F85" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="G85" t="s">
         <v>405</v>
       </c>
       <c r="H85" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="I85" t="e">
         <f>NA()</f>
@@ -4688,7 +4885,7 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B86" t="s">
         <v>41</v>
@@ -4703,13 +4900,13 @@
         <v>394</v>
       </c>
       <c r="F86" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="G86" t="s">
         <v>405</v>
       </c>
       <c r="H86" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="I86" t="e">
         <f>NA()</f>
@@ -4718,7 +4915,7 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B87" t="s">
         <v>41</v>
@@ -4733,13 +4930,13 @@
         <v>394</v>
       </c>
       <c r="F87" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="G87" t="s">
         <v>405</v>
       </c>
       <c r="H87" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="I87" t="e">
         <f>NA()</f>
@@ -4748,7 +4945,7 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B88" t="s">
         <v>41</v>
@@ -4763,13 +4960,13 @@
         <v>394</v>
       </c>
       <c r="F88" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="G88" t="s">
         <v>405</v>
       </c>
       <c r="H88" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="I88" t="e">
         <f>NA()</f>
@@ -4778,7 +4975,7 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B89" t="s">
         <v>41</v>
@@ -4793,13 +4990,13 @@
         <v>394</v>
       </c>
       <c r="F89" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="G89" t="s">
         <v>405</v>
       </c>
       <c r="H89" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="I89" t="e">
         <f>NA()</f>
@@ -4808,7 +5005,7 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B90" t="s">
         <v>41</v>
@@ -4823,13 +5020,13 @@
         <v>394</v>
       </c>
       <c r="F90" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="G90" t="s">
         <v>405</v>
       </c>
       <c r="H90" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="I90" t="e">
         <f>NA()</f>
@@ -4838,7 +5035,7 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B91" t="s">
         <v>41</v>
@@ -4853,13 +5050,13 @@
         <v>394</v>
       </c>
       <c r="F91" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="G91" t="s">
         <v>405</v>
       </c>
       <c r="H91" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="I91" t="e">
         <f>NA()</f>
@@ -4868,7 +5065,7 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B92" t="s">
         <v>41</v>
@@ -4883,13 +5080,13 @@
         <v>394</v>
       </c>
       <c r="F92" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="G92" t="s">
         <v>405</v>
       </c>
       <c r="H92" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="I92" t="e">
         <f>NA()</f>
@@ -4898,7 +5095,7 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B93" t="s">
         <v>41</v>
@@ -4913,13 +5110,13 @@
         <v>394</v>
       </c>
       <c r="F93" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="G93" t="s">
         <v>405</v>
       </c>
       <c r="H93" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="I93" t="e">
         <f>NA()</f>
@@ -4928,28 +5125,28 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>392</v>
+        <v>431</v>
       </c>
       <c r="B94" t="s">
-        <v>41</v>
+        <v>143</v>
       </c>
       <c r="C94" t="s">
         <v>26</v>
       </c>
       <c r="D94" t="s">
-        <v>393</v>
-      </c>
-      <c r="E94" t="s">
-        <v>394</v>
+        <v>432</v>
+      </c>
+      <c r="E94" s="7" t="s">
+        <v>433</v>
       </c>
       <c r="F94" t="s">
-        <v>404</v>
+        <v>429</v>
       </c>
       <c r="G94" t="s">
-        <v>405</v>
+        <v>430</v>
       </c>
       <c r="H94" t="s">
-        <v>415</v>
+        <v>434</v>
       </c>
       <c r="I94" t="e">
         <f>NA()</f>
@@ -4961,25 +5158,25 @@
         <v>436</v>
       </c>
       <c r="B95" t="s">
-        <v>143</v>
+        <v>41</v>
       </c>
       <c r="C95" t="s">
         <v>26</v>
       </c>
       <c r="D95" t="s">
+        <v>432</v>
+      </c>
+      <c r="E95" t="s">
+        <v>118</v>
+      </c>
+      <c r="F95" t="s">
         <v>437</v>
-      </c>
-      <c r="E95" s="7" t="s">
-        <v>438</v>
-      </c>
-      <c r="F95" t="s">
-        <v>433</v>
       </c>
       <c r="G95" t="s">
         <v>435</v>
       </c>
       <c r="H95" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="I95" t="e">
         <f>NA()</f>
@@ -4991,25 +5188,25 @@
         <v>441</v>
       </c>
       <c r="B96" t="s">
-        <v>41</v>
+        <v>143</v>
       </c>
       <c r="C96" t="s">
         <v>26</v>
       </c>
       <c r="D96" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="E96" t="s">
         <v>118</v>
       </c>
-      <c r="F96" t="s">
+      <c r="F96" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="H96" t="s">
         <v>442</v>
-      </c>
-      <c r="G96" t="s">
-        <v>440</v>
-      </c>
-      <c r="H96" t="s">
-        <v>443</v>
       </c>
       <c r="I96" t="e">
         <f>NA()</f>
@@ -5018,30 +5215,90 @@
     </row>
     <row r="97" spans="1:9">
       <c r="A97" t="s">
-        <v>446</v>
+        <v>472</v>
       </c>
       <c r="B97" t="s">
-        <v>143</v>
+        <v>474</v>
       </c>
       <c r="C97" t="s">
         <v>26</v>
       </c>
       <c r="D97" t="s">
-        <v>437</v>
+        <v>444</v>
       </c>
       <c r="E97" t="s">
+        <v>475</v>
+      </c>
+      <c r="F97" t="s">
+        <v>473</v>
+      </c>
+      <c r="G97" t="s">
+        <v>471</v>
+      </c>
+      <c r="H97" t="s">
+        <v>476</v>
+      </c>
+      <c r="I97" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" t="s">
+        <v>483</v>
+      </c>
+      <c r="B98" t="s">
+        <v>41</v>
+      </c>
+      <c r="C98" t="s">
+        <v>26</v>
+      </c>
+      <c r="D98" t="s">
+        <v>444</v>
+      </c>
+      <c r="E98" t="s">
+        <v>188</v>
+      </c>
+      <c r="F98" t="s">
+        <v>484</v>
+      </c>
+      <c r="G98" t="s">
+        <v>485</v>
+      </c>
+      <c r="H98" t="s">
+        <v>486</v>
+      </c>
+      <c r="I98" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
+      <c r="A99" t="s">
+        <v>487</v>
+      </c>
+      <c r="B99" t="s">
+        <v>41</v>
+      </c>
+      <c r="C99" t="s">
+        <v>26</v>
+      </c>
+      <c r="D99" t="s">
+        <v>444</v>
+      </c>
+      <c r="E99" t="s">
         <v>118</v>
       </c>
-      <c r="F97" s="3" t="s">
-        <v>444</v>
-      </c>
-      <c r="G97" s="3" t="s">
-        <v>445</v>
-      </c>
-      <c r="H97" t="s">
-        <v>447</v>
-      </c>
-      <c r="I97" t="e">
+      <c r="F99" t="s">
+        <v>488</v>
+      </c>
+      <c r="G99" t="s">
+        <v>489</v>
+      </c>
+      <c r="H99" t="s">
+        <v>490</v>
+      </c>
+      <c r="I99" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
@@ -5065,10 +5322,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil3" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5107,7 +5364,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="B2" t="s">
         <v>417</v>
@@ -5116,149 +5373,175 @@
         <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="E2" t="s">
         <v>188</v>
       </c>
       <c r="F2" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="G2" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="H2" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="B3" t="s">
         <v>417</v>
       </c>
       <c r="C3" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="D3" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="E3" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="F3" t="s">
-        <v>434</v>
+        <v>477</v>
       </c>
       <c r="G3" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="H3" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="B4" t="s">
         <v>417</v>
       </c>
       <c r="C4" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="D4" t="s">
-        <v>393</v>
+        <v>444</v>
       </c>
       <c r="E4" t="s">
+        <v>423</v>
+      </c>
+      <c r="F4" t="s">
+        <v>478</v>
+      </c>
+      <c r="G4" t="s">
         <v>424</v>
       </c>
-      <c r="F4" t="s">
-        <v>428</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>425</v>
-      </c>
-      <c r="H4" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="B5" t="s">
         <v>417</v>
       </c>
       <c r="C5" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="D5" t="s">
-        <v>393</v>
+        <v>444</v>
       </c>
       <c r="E5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F5" t="s">
-        <v>427</v>
+        <v>479</v>
       </c>
       <c r="G5" t="s">
+        <v>421</v>
+      </c>
+      <c r="H5" t="s">
         <v>422</v>
-      </c>
-      <c r="H5" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="B6" t="s">
         <v>417</v>
       </c>
       <c r="C6" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="D6" t="s">
-        <v>393</v>
+        <v>444</v>
       </c>
       <c r="E6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F6" t="s">
-        <v>426</v>
+        <v>480</v>
       </c>
       <c r="G6" t="s">
+        <v>419</v>
+      </c>
+      <c r="H6" t="s">
         <v>420</v>
-      </c>
-      <c r="H6" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="B7" t="s">
         <v>417</v>
       </c>
       <c r="C7" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="D7" t="s">
-        <v>393</v>
+        <v>444</v>
       </c>
       <c r="E7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F7" t="s">
-        <v>418</v>
+        <v>481</v>
       </c>
       <c r="G7" t="s">
         <v>416</v>
       </c>
       <c r="H7" t="s">
-        <v>419</v>
+        <v>418</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>467</v>
+      </c>
+      <c r="B8" t="s">
+        <v>417</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>444</v>
+      </c>
+      <c r="E8" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" t="s">
+        <v>469</v>
+      </c>
+      <c r="G8" t="s">
+        <v>468</v>
+      </c>
+      <c r="H8" t="s">
+        <v>470</v>
       </c>
     </row>
   </sheetData>
@@ -5757,4 +6040,192 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil6" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>456</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>444</v>
+      </c>
+      <c r="E2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" t="s">
+        <v>457</v>
+      </c>
+      <c r="G2" t="s">
+        <v>455</v>
+      </c>
+      <c r="H2" t="s">
+        <v>458</v>
+      </c>
+      <c r="I2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>482</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>444</v>
+      </c>
+      <c r="E3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" t="s">
+        <v>466</v>
+      </c>
+      <c r="G3" t="s">
+        <v>459</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="45">
+      <c r="A4" t="s">
+        <v>463</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>444</v>
+      </c>
+      <c r="E4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="G4" t="s">
+        <v>460</v>
+      </c>
+      <c r="I4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>464</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>444</v>
+      </c>
+      <c r="E5" t="s">
+        <v>188</v>
+      </c>
+      <c r="F5" t="s">
+        <v>465</v>
+      </c>
+      <c r="G5" t="s">
+        <v>461</v>
+      </c>
+      <c r="I5">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>168</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6">
+        <v>0.48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
end coding plant transpiration
</commit_message>
<xml_diff>
--- a/allvariables.xlsx
+++ b/allvariables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11660" yWindow="1740" windowWidth="24720" windowHeight="18900" tabRatio="652" activeTab="1"/>
+    <workbookView xWindow="12380" yWindow="840" windowWidth="25600" windowHeight="16060" tabRatio="652" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="nomenclature" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="510">
   <si>
     <t>name</t>
   </si>
@@ -1508,6 +1508,63 @@
   </si>
   <si>
     <t>évaporation du sol</t>
+  </si>
+  <si>
+    <t>A coefficient to calculate VPD; 0.65 for humid and subhumid climates and 0.75 for arid and semi-arid climates</t>
+  </si>
+  <si>
+    <t>VPDF</t>
+  </si>
+  <si>
+    <t>pVPDcoef</t>
+  </si>
+  <si>
+    <t>coefficient pour calculer le VPD, 0.65 pour les climats humides et subhumides, 0.75 pour les climats arides et semiarides</t>
+  </si>
+  <si>
+    <t>Transpiration efficiency coefficient at CO2 concentration 350 ppm</t>
+  </si>
+  <si>
+    <t>TEC350</t>
+  </si>
+  <si>
+    <t>pTranspirationEfficiencyLinkedToCO2</t>
+  </si>
+  <si>
+    <t>coefficient d'efficacité de la transpiration lié à la teneur en CO2</t>
+  </si>
+  <si>
+    <t>FLOUT</t>
+  </si>
+  <si>
+    <t>cDownwardWaterFlux.1</t>
+  </si>
+  <si>
+    <t>cDownwardWaterFlux.2</t>
+  </si>
+  <si>
+    <t>cDownwardWaterFlux.3</t>
+  </si>
+  <si>
+    <t>cDownwardWaterFlux.4</t>
+  </si>
+  <si>
+    <t>cDownwardWaterFlux.5</t>
+  </si>
+  <si>
+    <t>cDownwardWaterFlux.6</t>
+  </si>
+  <si>
+    <t>cDownwardWaterFlux.7</t>
+  </si>
+  <si>
+    <t>cDownwardWaterFlux.8</t>
+  </si>
+  <si>
+    <t>cDownwardWaterFlux.9</t>
+  </si>
+  <si>
+    <t>cDownwardWaterFlux.10</t>
   </si>
 </sst>
 </file>
@@ -1612,8 +1669,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="217">
+  <cellStyleXfs count="231">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1859,7 +1930,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="217">
+  <cellStyles count="231">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -1968,6 +2039,13 @@
     <cellStyle name="Lien hypertexte" xfId="211" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="213" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="229" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -2076,6 +2154,13 @@
     <cellStyle name="Lien hypertexte visité" xfId="212" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="214" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="230" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2440,13 +2525,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:I99"/>
+  <dimension ref="A1:I110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B63" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I99" sqref="I99"/>
+      <selection pane="bottomRight" activeCell="F101" sqref="F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5301,6 +5386,209 @@
       <c r="I99" t="e">
         <f>NA()</f>
         <v>#N/A</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100" t="s">
+        <v>497</v>
+      </c>
+      <c r="B100" t="s">
+        <v>143</v>
+      </c>
+      <c r="C100" t="s">
+        <v>26</v>
+      </c>
+      <c r="D100" t="s">
+        <v>444</v>
+      </c>
+      <c r="E100" t="s">
+        <v>188</v>
+      </c>
+      <c r="F100" t="s">
+        <v>495</v>
+      </c>
+      <c r="G100" t="s">
+        <v>496</v>
+      </c>
+      <c r="H100" t="s">
+        <v>498</v>
+      </c>
+      <c r="I100" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="A101" t="s">
+        <v>500</v>
+      </c>
+      <c r="B101" t="s">
+        <v>41</v>
+      </c>
+      <c r="C101" t="s">
+        <v>26</v>
+      </c>
+      <c r="D101" t="s">
+        <v>444</v>
+      </c>
+      <c r="E101" t="s">
+        <v>118</v>
+      </c>
+      <c r="G101" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
+      <c r="A102" t="s">
+        <v>501</v>
+      </c>
+      <c r="B102" t="s">
+        <v>41</v>
+      </c>
+      <c r="C102" t="s">
+        <v>26</v>
+      </c>
+      <c r="D102" t="s">
+        <v>444</v>
+      </c>
+      <c r="E102" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
+      <c r="A103" t="s">
+        <v>502</v>
+      </c>
+      <c r="B103" t="s">
+        <v>41</v>
+      </c>
+      <c r="C103" t="s">
+        <v>26</v>
+      </c>
+      <c r="D103" t="s">
+        <v>444</v>
+      </c>
+      <c r="E103" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104" t="s">
+        <v>503</v>
+      </c>
+      <c r="B104" t="s">
+        <v>41</v>
+      </c>
+      <c r="C104" t="s">
+        <v>26</v>
+      </c>
+      <c r="D104" t="s">
+        <v>444</v>
+      </c>
+      <c r="E104" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105" t="s">
+        <v>504</v>
+      </c>
+      <c r="B105" t="s">
+        <v>41</v>
+      </c>
+      <c r="C105" t="s">
+        <v>26</v>
+      </c>
+      <c r="D105" t="s">
+        <v>444</v>
+      </c>
+      <c r="E105" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106" t="s">
+        <v>505</v>
+      </c>
+      <c r="B106" t="s">
+        <v>41</v>
+      </c>
+      <c r="C106" t="s">
+        <v>26</v>
+      </c>
+      <c r="D106" t="s">
+        <v>444</v>
+      </c>
+      <c r="E106" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
+      <c r="A107" t="s">
+        <v>506</v>
+      </c>
+      <c r="B107" t="s">
+        <v>41</v>
+      </c>
+      <c r="C107" t="s">
+        <v>26</v>
+      </c>
+      <c r="D107" t="s">
+        <v>444</v>
+      </c>
+      <c r="E107" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
+      <c r="A108" t="s">
+        <v>507</v>
+      </c>
+      <c r="B108" t="s">
+        <v>41</v>
+      </c>
+      <c r="C108" t="s">
+        <v>26</v>
+      </c>
+      <c r="D108" t="s">
+        <v>444</v>
+      </c>
+      <c r="E108" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
+      <c r="A109" t="s">
+        <v>508</v>
+      </c>
+      <c r="B109" t="s">
+        <v>41</v>
+      </c>
+      <c r="C109" t="s">
+        <v>26</v>
+      </c>
+      <c r="D109" t="s">
+        <v>444</v>
+      </c>
+      <c r="E109" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
+      <c r="A110" t="s">
+        <v>509</v>
+      </c>
+      <c r="B110" t="s">
+        <v>41</v>
+      </c>
+      <c r="C110" t="s">
+        <v>26</v>
+      </c>
+      <c r="D110" t="s">
+        <v>444</v>
+      </c>
+      <c r="E110" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -5322,10 +5610,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil3" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5542,6 +5830,29 @@
       </c>
       <c r="H8" t="s">
         <v>470</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>493</v>
+      </c>
+      <c r="B9" t="s">
+        <v>417</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>444</v>
+      </c>
+      <c r="F9" t="s">
+        <v>491</v>
+      </c>
+      <c r="G9" t="s">
+        <v>492</v>
+      </c>
+      <c r="H9" t="s">
+        <v>494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
simplified the format of ALLCROPS
now ALLCROPS is a data.frame with crop.cultivar as rownames.
Also changed the way the crop parameter file is read: now read from format where all crops are on the same sheet (names allcrops)
</commit_message>
<xml_diff>
--- a/allvariables.xlsx
+++ b/allvariables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13600" tabRatio="652" activeTab="1"/>
+    <workbookView xWindow="2780" yWindow="0" windowWidth="25120" windowHeight="13120" tabRatio="652" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="nomenclature" sheetId="5" r:id="rId1"/>
@@ -739,12 +739,6 @@
     <t>pFreezeFracLeafDestruction</t>
   </si>
   <si>
-    <t>FRZTKIL</t>
-  </si>
-  <si>
-    <t>FRZLDR</t>
-  </si>
-  <si>
     <t xml:space="preserve">Phyllochron </t>
   </si>
   <si>
@@ -1153,9 +1147,6 @@
     <t>PLACON</t>
   </si>
   <si>
-    <t>PLAPOW</t>
-  </si>
-  <si>
     <t>HtLDR</t>
   </si>
   <si>
@@ -1598,6 +1589,15 @@
   </si>
   <si>
     <t>stade de développement en chiffre</t>
+  </si>
+  <si>
+    <t>PLAPOW300</t>
+  </si>
+  <si>
+    <t>FrzLDR</t>
+  </si>
+  <si>
+    <t>FrzTh</t>
   </si>
 </sst>
 </file>
@@ -1709,7 +1709,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="255">
+  <cellStyleXfs count="259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1965,8 +1965,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1995,8 +1999,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="255">
+  <cellStyles count="259">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -2124,6 +2129,8 @@
     <cellStyle name="Lien hypertexte" xfId="249" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="251" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="257" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -2251,6 +2258,8 @@
     <cellStyle name="Lien hypertexte visité" xfId="250" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="252" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="258" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2618,10 +2627,10 @@
   <dimension ref="A1:I113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomRight" activeCell="G72" sqref="G72:G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2663,28 +2672,28 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B2" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="H2" t="s">
         <v>295</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="H2" t="s">
-        <v>297</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2692,28 +2701,28 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B3" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2721,28 +2730,28 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B4" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -2753,7 +2762,7 @@
         <v>202</v>
       </c>
       <c r="B5" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>26</v>
@@ -2779,10 +2788,10 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B6" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C6" t="s">
         <v>26</v>
@@ -2794,13 +2803,13 @@
         <v>188</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="H6" t="s">
         <v>238</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="H6" t="s">
-        <v>240</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -2808,10 +2817,10 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="B7" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
@@ -2820,16 +2829,16 @@
         <v>203</v>
       </c>
       <c r="E7" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="H7" t="s">
         <v>247</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="H7" t="s">
-        <v>249</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -2840,7 +2849,7 @@
         <v>172</v>
       </c>
       <c r="B8" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C8" t="s">
         <v>171</v>
@@ -2863,7 +2872,7 @@
         <v>173</v>
       </c>
       <c r="B9" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C9" t="s">
         <v>171</v>
@@ -2886,7 +2895,7 @@
         <v>184</v>
       </c>
       <c r="B10" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C10" t="s">
         <v>26</v>
@@ -2915,7 +2924,7 @@
         <v>166</v>
       </c>
       <c r="B11" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C11" t="s">
         <v>171</v>
@@ -2938,10 +2947,10 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B12" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C12" t="s">
         <v>26</v>
@@ -2953,10 +2962,10 @@
         <v>188</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="H12" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -2964,7 +2973,7 @@
         <v>183</v>
       </c>
       <c r="B13" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -2990,28 +2999,28 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C14" t="s">
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="E14" t="s">
         <v>118</v>
       </c>
       <c r="F14" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="G14" t="s">
+        <v>427</v>
+      </c>
+      <c r="H14" t="s">
         <v>430</v>
-      </c>
-      <c r="H14" t="s">
-        <v>433</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -3019,26 +3028,26 @@
     </row>
     <row r="15" spans="1:9" s="14" customFormat="1">
       <c r="A15" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B15" t="s">
+        <v>502</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
         <v>505</v>
       </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
+        <v>506</v>
+      </c>
+      <c r="F15" t="s">
         <v>508</v>
-      </c>
-      <c r="E15" t="s">
-        <v>509</v>
-      </c>
-      <c r="F15" t="s">
-        <v>511</v>
       </c>
       <c r="G15"/>
       <c r="H15" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -3046,25 +3055,25 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
+        <v>503</v>
+      </c>
+      <c r="B16" t="s">
+        <v>502</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>505</v>
+      </c>
+      <c r="E16" t="s">
         <v>506</v>
       </c>
-      <c r="B16" t="s">
-        <v>505</v>
-      </c>
-      <c r="C16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" t="s">
-        <v>508</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
+        <v>507</v>
+      </c>
+      <c r="H16" t="s">
         <v>509</v>
-      </c>
-      <c r="F16" t="s">
-        <v>510</v>
-      </c>
-      <c r="H16" t="s">
-        <v>512</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -3072,28 +3081,28 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C17" t="s">
         <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E17" t="s">
         <v>188</v>
       </c>
       <c r="F17" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="G17" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="H17" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -3101,28 +3110,28 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="B18" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E18" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="F18" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="G18" t="s">
+        <v>463</v>
+      </c>
+      <c r="H18" t="s">
         <v>466</v>
-      </c>
-      <c r="H18" t="s">
-        <v>469</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -3130,28 +3139,28 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B19" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E19" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F19" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="G19" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="H19" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -3159,28 +3168,28 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B20" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C20" t="s">
         <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E20" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F20" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="G20" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="H20" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -3188,28 +3197,28 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B21" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C21" t="s">
         <v>26</v>
       </c>
       <c r="D21" t="s">
+        <v>385</v>
+      </c>
+      <c r="E21" t="s">
+        <v>386</v>
+      </c>
+      <c r="F21" t="s">
         <v>388</v>
       </c>
-      <c r="E21" t="s">
-        <v>389</v>
-      </c>
-      <c r="F21" t="s">
-        <v>391</v>
-      </c>
       <c r="G21" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="H21" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -3217,28 +3226,28 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B22" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C22" t="s">
         <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E22" t="s">
+        <v>386</v>
+      </c>
+      <c r="F22" t="s">
         <v>389</v>
       </c>
-      <c r="F22" t="s">
-        <v>392</v>
-      </c>
       <c r="G22" t="s">
+        <v>397</v>
+      </c>
+      <c r="H22" t="s">
         <v>400</v>
-      </c>
-      <c r="H22" t="s">
-        <v>403</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -3246,28 +3255,28 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B23" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C23" t="s">
         <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E23" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F23" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="G23" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="H23" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -3275,28 +3284,28 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B24" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C24" t="s">
         <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E24" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F24" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G24" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="H24" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -3304,28 +3313,28 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B25" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C25" t="s">
         <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E25" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F25" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="G25" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="H25" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -3333,28 +3342,28 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B26" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C26" t="s">
         <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E26" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F26" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="G26" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="H26" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -3362,28 +3371,28 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
+        <v>382</v>
+      </c>
+      <c r="B27" t="s">
+        <v>502</v>
+      </c>
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" t="s">
         <v>385</v>
       </c>
-      <c r="B27" t="s">
-        <v>505</v>
-      </c>
-      <c r="C27" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" t="s">
-        <v>388</v>
-      </c>
       <c r="E27" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F27" t="s">
+        <v>394</v>
+      </c>
+      <c r="G27" t="s">
         <v>397</v>
       </c>
-      <c r="G27" t="s">
-        <v>400</v>
-      </c>
       <c r="H27" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -3391,28 +3400,28 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
+        <v>383</v>
+      </c>
+      <c r="B28" t="s">
+        <v>502</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" t="s">
+        <v>385</v>
+      </c>
+      <c r="E28" t="s">
         <v>386</v>
       </c>
-      <c r="B28" t="s">
-        <v>505</v>
-      </c>
-      <c r="C28" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" t="s">
-        <v>388</v>
-      </c>
-      <c r="E28" t="s">
-        <v>389</v>
-      </c>
       <c r="F28" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="G28" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="H28" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -3423,13 +3432,13 @@
         <v>160</v>
       </c>
       <c r="B29" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C29" t="s">
         <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E29" t="s">
         <v>124</v>
@@ -3452,7 +3461,7 @@
         <v>109</v>
       </c>
       <c r="B30" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C30" t="s">
         <v>26</v>
@@ -3625,7 +3634,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B36" t="s">
         <v>143</v>
@@ -3634,16 +3643,16 @@
         <v>26</v>
       </c>
       <c r="D36" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G36" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="I36" t="e">
         <f>NA()</f>
@@ -3652,7 +3661,7 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B37" t="s">
         <v>143</v>
@@ -3661,16 +3670,16 @@
         <v>26</v>
       </c>
       <c r="D37" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G37" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="I37" t="e">
         <f>NA()</f>
@@ -3679,7 +3688,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B38" t="s">
         <v>143</v>
@@ -3688,16 +3697,16 @@
         <v>26</v>
       </c>
       <c r="D38" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G38" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="I38" t="e">
         <f>NA()</f>
@@ -3706,7 +3715,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B39" t="s">
         <v>143</v>
@@ -3715,16 +3724,16 @@
         <v>26</v>
       </c>
       <c r="D39" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G39" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="I39" t="e">
         <f>NA()</f>
@@ -3733,7 +3742,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B40" t="s">
         <v>143</v>
@@ -3742,16 +3751,16 @@
         <v>26</v>
       </c>
       <c r="D40" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G40" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="I40" t="e">
         <f>NA()</f>
@@ -3760,7 +3769,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B41" t="s">
         <v>143</v>
@@ -3769,16 +3778,16 @@
         <v>26</v>
       </c>
       <c r="D41" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G41" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="I41" t="e">
         <f>NA()</f>
@@ -3787,7 +3796,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B42" t="s">
         <v>143</v>
@@ -3796,16 +3805,16 @@
         <v>26</v>
       </c>
       <c r="D42" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G42" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="I42" t="e">
         <f>NA()</f>
@@ -3814,7 +3823,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B43" t="s">
         <v>143</v>
@@ -3823,16 +3832,16 @@
         <v>26</v>
       </c>
       <c r="D43" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G43" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="I43" t="e">
         <f>NA()</f>
@@ -3841,7 +3850,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B44" t="s">
         <v>143</v>
@@ -3850,16 +3859,16 @@
         <v>26</v>
       </c>
       <c r="D44" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G44" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="I44" t="e">
         <f>NA()</f>
@@ -3868,7 +3877,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B45" t="s">
         <v>143</v>
@@ -3877,16 +3886,16 @@
         <v>26</v>
       </c>
       <c r="D45" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G45" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I45" t="e">
         <f>NA()</f>
@@ -3895,7 +3904,7 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B46" t="s">
         <v>143</v>
@@ -3904,16 +3913,16 @@
         <v>26</v>
       </c>
       <c r="D46" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G46" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I46" t="e">
         <f>NA()</f>
@@ -3922,7 +3931,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B47" t="s">
         <v>143</v>
@@ -3931,19 +3940,19 @@
         <v>26</v>
       </c>
       <c r="D47" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>188</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="H47" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="I47" t="e">
         <f>NA()</f>
@@ -3952,7 +3961,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B48" t="s">
         <v>143</v>
@@ -3961,13 +3970,13 @@
         <v>26</v>
       </c>
       <c r="D48" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="I48" t="e">
         <f>NA()</f>
@@ -3976,7 +3985,7 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B49" t="s">
         <v>143</v>
@@ -3985,19 +3994,19 @@
         <v>26</v>
       </c>
       <c r="D49" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="H49" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I49" t="e">
         <f>NA()</f>
@@ -4006,7 +4015,7 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B50" t="s">
         <v>143</v>
@@ -4015,13 +4024,13 @@
         <v>26</v>
       </c>
       <c r="D50" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="I50" t="e">
         <f>NA()</f>
@@ -4030,7 +4039,7 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B51" t="s">
         <v>143</v>
@@ -4039,13 +4048,13 @@
         <v>26</v>
       </c>
       <c r="D51" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="I51" t="e">
         <f>NA()</f>
@@ -4054,7 +4063,7 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B52" t="s">
         <v>143</v>
@@ -4063,13 +4072,13 @@
         <v>26</v>
       </c>
       <c r="D52" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I52" t="e">
         <f>NA()</f>
@@ -4078,7 +4087,7 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B53" t="s">
         <v>143</v>
@@ -4087,19 +4096,19 @@
         <v>26</v>
       </c>
       <c r="D53" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E53" s="7" t="s">
         <v>188</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="H53" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="I53" t="e">
         <f>NA()</f>
@@ -4108,7 +4117,7 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B54" t="s">
         <v>143</v>
@@ -4117,19 +4126,19 @@
         <v>26</v>
       </c>
       <c r="D54" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E54" s="7" t="s">
         <v>188</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>372</v>
+        <v>518</v>
       </c>
       <c r="H54" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I54" t="e">
         <f>NA()</f>
@@ -4138,7 +4147,7 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B55" t="s">
         <v>143</v>
@@ -4147,19 +4156,19 @@
         <v>26</v>
       </c>
       <c r="D55" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I55" t="e">
         <f>NA()</f>
@@ -4168,7 +4177,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B56" t="s">
         <v>143</v>
@@ -4177,19 +4186,19 @@
         <v>26</v>
       </c>
       <c r="D56" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="H56" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I56" t="e">
         <f>NA()</f>
@@ -4207,7 +4216,7 @@
         <v>26</v>
       </c>
       <c r="D57" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E57" s="9" t="s">
         <v>232</v>
@@ -4215,8 +4224,8 @@
       <c r="F57" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="G57" t="s">
-        <v>235</v>
+      <c r="G57" s="18" t="s">
+        <v>519</v>
       </c>
       <c r="H57" t="s">
         <v>231</v>
@@ -4237,7 +4246,7 @@
         <v>26</v>
       </c>
       <c r="D58" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E58" t="s">
         <v>15</v>
@@ -4245,8 +4254,8 @@
       <c r="F58" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="G58" t="s">
-        <v>234</v>
+      <c r="G58" s="11" t="s">
+        <v>520</v>
       </c>
       <c r="H58" t="s">
         <v>230</v>
@@ -4258,7 +4267,7 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B59" t="s">
         <v>143</v>
@@ -4267,13 +4276,13 @@
         <v>26</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="I59" t="e">
         <f>NA()</f>
@@ -4282,7 +4291,7 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B60" t="s">
         <v>143</v>
@@ -4291,13 +4300,13 @@
         <v>26</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="I60" t="e">
         <f>NA()</f>
@@ -4315,7 +4324,7 @@
         <v>26</v>
       </c>
       <c r="D61" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E61" s="7" t="s">
         <v>221</v>
@@ -4324,7 +4333,7 @@
         <v>220</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="H61" t="s">
         <v>225</v>
@@ -4345,7 +4354,7 @@
         <v>26</v>
       </c>
       <c r="D62" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E62" s="7" t="s">
         <v>221</v>
@@ -4354,7 +4363,7 @@
         <v>222</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="H62" t="s">
         <v>226</v>
@@ -4456,7 +4465,7 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B66" t="s">
         <v>143</v>
@@ -4495,7 +4504,7 @@
         <v>26</v>
       </c>
       <c r="D67" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E67" t="s">
         <v>187</v>
@@ -4525,7 +4534,7 @@
         <v>26</v>
       </c>
       <c r="D68" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E68" t="s">
         <v>188</v>
@@ -4546,7 +4555,7 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B69" t="s">
         <v>143</v>
@@ -4555,19 +4564,19 @@
         <v>26</v>
       </c>
       <c r="D69" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="E69" t="s">
         <v>118</v>
       </c>
       <c r="F69" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="H69" t="s">
         <v>434</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="H69" t="s">
-        <v>437</v>
       </c>
       <c r="I69" t="e">
         <f>NA()</f>
@@ -4576,7 +4585,7 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B70" t="s">
         <v>143</v>
@@ -4585,19 +4594,19 @@
         <v>26</v>
       </c>
       <c r="D70" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="F70" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="G70" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="H70" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="I70" t="e">
         <f>NA()</f>
@@ -4606,7 +4615,7 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B71" t="s">
         <v>143</v>
@@ -4615,27 +4624,27 @@
         <v>26</v>
       </c>
       <c r="D71" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E71" t="s">
         <v>188</v>
       </c>
       <c r="F71" t="s">
+        <v>485</v>
+      </c>
+      <c r="G71" t="s">
+        <v>486</v>
+      </c>
+      <c r="H71" t="s">
         <v>488</v>
       </c>
-      <c r="G71" t="s">
-        <v>489</v>
-      </c>
-      <c r="H71" t="s">
-        <v>491</v>
-      </c>
       <c r="I71" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="72" spans="1:9">
-      <c r="A72" t="s">
+      <c r="A72" s="16" t="s">
         <v>138</v>
       </c>
       <c r="B72" t="s">
@@ -4645,7 +4654,7 @@
         <v>26</v>
       </c>
       <c r="D72" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E72" t="s">
         <v>15</v>
@@ -4653,8 +4662,8 @@
       <c r="F72" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="G72" t="s">
-        <v>338</v>
+      <c r="G72" s="16" t="s">
+        <v>336</v>
       </c>
       <c r="H72" t="s">
         <v>156</v>
@@ -4665,7 +4674,7 @@
       </c>
     </row>
     <row r="73" spans="1:9">
-      <c r="A73" t="s">
+      <c r="A73" s="16" t="s">
         <v>141</v>
       </c>
       <c r="B73" t="s">
@@ -4675,7 +4684,7 @@
         <v>26</v>
       </c>
       <c r="D73" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E73" t="s">
         <v>15</v>
@@ -4683,8 +4692,8 @@
       <c r="F73" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="G73" t="s">
-        <v>336</v>
+      <c r="G73" s="16" t="s">
+        <v>334</v>
       </c>
       <c r="H73" t="s">
         <v>154</v>
@@ -4695,7 +4704,7 @@
       </c>
     </row>
     <row r="74" spans="1:9">
-      <c r="A74" t="s">
+      <c r="A74" s="16" t="s">
         <v>139</v>
       </c>
       <c r="B74" t="s">
@@ -4705,7 +4714,7 @@
         <v>26</v>
       </c>
       <c r="D74" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E74" t="s">
         <v>15</v>
@@ -4713,8 +4722,8 @@
       <c r="F74" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G74" t="s">
-        <v>339</v>
+      <c r="G74" s="16" t="s">
+        <v>337</v>
       </c>
       <c r="H74" t="s">
         <v>157</v>
@@ -4725,8 +4734,8 @@
       </c>
     </row>
     <row r="75" spans="1:9">
-      <c r="A75" t="s">
-        <v>503</v>
+      <c r="A75" s="16" t="s">
+        <v>500</v>
       </c>
       <c r="B75" t="s">
         <v>143</v>
@@ -4735,7 +4744,7 @@
         <v>26</v>
       </c>
       <c r="D75" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E75" t="s">
         <v>15</v>
@@ -4743,8 +4752,8 @@
       <c r="F75" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="G75" t="s">
-        <v>335</v>
+      <c r="G75" s="16" t="s">
+        <v>333</v>
       </c>
       <c r="H75" t="s">
         <v>158</v>
@@ -4756,7 +4765,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B76" t="s">
         <v>143</v>
@@ -4765,14 +4774,14 @@
         <v>26</v>
       </c>
       <c r="D76" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E76" s="4"/>
       <c r="F76" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="G76" s="4" t="s">
-        <v>337</v>
+      <c r="G76" s="16" t="s">
+        <v>335</v>
       </c>
       <c r="H76" s="4" t="s">
         <v>153</v>
@@ -4793,7 +4802,7 @@
         <v>26</v>
       </c>
       <c r="D77" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>147</v>
@@ -4841,7 +4850,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B79" t="s">
         <v>41</v>
@@ -4850,19 +4859,19 @@
         <v>26</v>
       </c>
       <c r="D79" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F79" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="H79" t="s">
         <v>261</v>
-      </c>
-      <c r="G79" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="H79" t="s">
-        <v>263</v>
       </c>
       <c r="I79" t="e">
         <f>NA()</f>
@@ -4871,7 +4880,7 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B80" t="s">
         <v>41</v>
@@ -4880,19 +4889,19 @@
         <v>26</v>
       </c>
       <c r="D80" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E80" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="H80" t="s">
         <v>280</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="G80" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="H80" t="s">
-        <v>282</v>
       </c>
       <c r="I80" t="e">
         <f>NA()</f>
@@ -4901,7 +4910,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B81" t="s">
         <v>41</v>
@@ -4910,19 +4919,19 @@
         <v>26</v>
       </c>
       <c r="D81" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F81" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="H81" t="s">
         <v>292</v>
-      </c>
-      <c r="G81" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="H81" t="s">
-        <v>294</v>
       </c>
       <c r="I81" t="e">
         <f>NA()</f>
@@ -4931,7 +4940,7 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B82" t="s">
         <v>41</v>
@@ -4940,19 +4949,19 @@
         <v>26</v>
       </c>
       <c r="D82" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E82" s="7" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F82" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="H82" t="s">
         <v>283</v>
-      </c>
-      <c r="G82" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="H82" t="s">
-        <v>285</v>
       </c>
       <c r="I82" t="e">
         <f>NA()</f>
@@ -4961,7 +4970,7 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B83" t="s">
         <v>41</v>
@@ -4976,13 +4985,13 @@
         <v>188</v>
       </c>
       <c r="F83" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="H83" t="s">
         <v>271</v>
-      </c>
-      <c r="G83" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="H83" t="s">
-        <v>273</v>
       </c>
       <c r="I83" t="e">
         <f>NA()</f>
@@ -5051,7 +5060,7 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B86" t="s">
         <v>41</v>
@@ -5063,16 +5072,16 @@
         <v>203</v>
       </c>
       <c r="E86" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G86" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="H86" t="s">
         <v>256</v>
-      </c>
-      <c r="H86" t="s">
-        <v>258</v>
       </c>
       <c r="I86" t="e">
         <f>NA()</f>
@@ -5296,7 +5305,7 @@
         <v>26</v>
       </c>
       <c r="D94" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E94" s="7" t="s">
         <v>217</v>
@@ -5305,7 +5314,7 @@
         <v>216</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="H94" t="s">
         <v>218</v>
@@ -5317,7 +5326,7 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B95" t="s">
         <v>41</v>
@@ -5326,13 +5335,13 @@
         <v>26</v>
       </c>
       <c r="D95" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E95" t="s">
         <v>118</v>
       </c>
       <c r="G95" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="I95" t="e">
         <f>NA()</f>
@@ -5341,7 +5350,7 @@
     </row>
     <row r="96" spans="1:9">
       <c r="A96" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="B96" t="s">
         <v>41</v>
@@ -5350,7 +5359,7 @@
         <v>26</v>
       </c>
       <c r="D96" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E96" t="s">
         <v>118</v>
@@ -5362,7 +5371,7 @@
     </row>
     <row r="97" spans="1:9">
       <c r="A97" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B97" t="s">
         <v>41</v>
@@ -5371,7 +5380,7 @@
         <v>26</v>
       </c>
       <c r="D97" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E97" t="s">
         <v>118</v>
@@ -5383,7 +5392,7 @@
     </row>
     <row r="98" spans="1:9">
       <c r="A98" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B98" t="s">
         <v>41</v>
@@ -5392,7 +5401,7 @@
         <v>26</v>
       </c>
       <c r="D98" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E98" t="s">
         <v>118</v>
@@ -5404,7 +5413,7 @@
     </row>
     <row r="99" spans="1:9">
       <c r="A99" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B99" t="s">
         <v>41</v>
@@ -5413,7 +5422,7 @@
         <v>26</v>
       </c>
       <c r="D99" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E99" t="s">
         <v>118</v>
@@ -5425,7 +5434,7 @@
     </row>
     <row r="100" spans="1:9">
       <c r="A100" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B100" t="s">
         <v>41</v>
@@ -5434,7 +5443,7 @@
         <v>26</v>
       </c>
       <c r="D100" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E100" t="s">
         <v>118</v>
@@ -5446,7 +5455,7 @@
     </row>
     <row r="101" spans="1:9">
       <c r="A101" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B101" t="s">
         <v>41</v>
@@ -5455,7 +5464,7 @@
         <v>26</v>
       </c>
       <c r="D101" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E101" t="s">
         <v>118</v>
@@ -5467,7 +5476,7 @@
     </row>
     <row r="102" spans="1:9">
       <c r="A102" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B102" t="s">
         <v>41</v>
@@ -5476,7 +5485,7 @@
         <v>26</v>
       </c>
       <c r="D102" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E102" t="s">
         <v>118</v>
@@ -5488,7 +5497,7 @@
     </row>
     <row r="103" spans="1:9">
       <c r="A103" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B103" t="s">
         <v>41</v>
@@ -5497,7 +5506,7 @@
         <v>26</v>
       </c>
       <c r="D103" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E103" t="s">
         <v>118</v>
@@ -5509,7 +5518,7 @@
     </row>
     <row r="104" spans="1:9">
       <c r="A104" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B104" t="s">
         <v>41</v>
@@ -5518,7 +5527,7 @@
         <v>26</v>
       </c>
       <c r="D104" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E104" t="s">
         <v>118</v>
@@ -5530,7 +5539,7 @@
     </row>
     <row r="105" spans="1:9">
       <c r="A105" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B105" t="s">
         <v>41</v>
@@ -5539,19 +5548,19 @@
         <v>26</v>
       </c>
       <c r="D105" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E105" t="s">
         <v>118</v>
       </c>
       <c r="F105" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="G105" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="H105" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="I105" t="e">
         <f>NA()</f>
@@ -5560,7 +5569,7 @@
     </row>
     <row r="106" spans="1:9">
       <c r="A106" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B106" t="s">
         <v>41</v>
@@ -5569,7 +5578,7 @@
         <v>26</v>
       </c>
       <c r="D106" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E106" t="s">
         <v>168</v>
@@ -5590,7 +5599,7 @@
     </row>
     <row r="107" spans="1:9">
       <c r="A107" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B107" t="s">
         <v>41</v>
@@ -5599,19 +5608,19 @@
         <v>26</v>
       </c>
       <c r="D107" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E107" s="7" t="s">
         <v>188</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="H107" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I107" t="e">
         <f>NA()</f>
@@ -5620,7 +5629,7 @@
     </row>
     <row r="108" spans="1:9">
       <c r="A108" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B108" t="s">
         <v>41</v>
@@ -5629,19 +5638,19 @@
         <v>26</v>
       </c>
       <c r="D108" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E108" t="s">
         <v>168</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G108" t="s">
+        <v>250</v>
+      </c>
+      <c r="H108" t="s">
         <v>252</v>
-      </c>
-      <c r="H108" t="s">
-        <v>254</v>
       </c>
       <c r="I108" t="e">
         <f>NA()</f>
@@ -5859,207 +5868,207 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B2" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E2" t="s">
         <v>188</v>
       </c>
       <c r="F2" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="G2" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="H2" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B3" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C3" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D3" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="E3" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="F3" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="G3" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="H3" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B4" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C4" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D4" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E4" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="F4" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="G4" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="H4" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B5" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C5" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D5" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E5" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="F5" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="G5" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="H5" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B6" t="s">
+        <v>409</v>
+      </c>
+      <c r="C6" t="s">
+        <v>441</v>
+      </c>
+      <c r="D6" t="s">
+        <v>436</v>
+      </c>
+      <c r="E6" t="s">
+        <v>415</v>
+      </c>
+      <c r="F6" t="s">
+        <v>470</v>
+      </c>
+      <c r="G6" t="s">
+        <v>411</v>
+      </c>
+      <c r="H6" t="s">
         <v>412</v>
-      </c>
-      <c r="C6" t="s">
-        <v>444</v>
-      </c>
-      <c r="D6" t="s">
-        <v>439</v>
-      </c>
-      <c r="E6" t="s">
-        <v>418</v>
-      </c>
-      <c r="F6" t="s">
-        <v>473</v>
-      </c>
-      <c r="G6" t="s">
-        <v>414</v>
-      </c>
-      <c r="H6" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B7" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C7" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D7" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E7" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="F7" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="G7" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="H7" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B8" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C8" t="s">
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E8" t="s">
         <v>188</v>
       </c>
       <c r="F8" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="G8" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H8" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B9" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C9" t="s">
         <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="F9" t="s">
+        <v>481</v>
+      </c>
+      <c r="G9" t="s">
+        <v>482</v>
+      </c>
+      <c r="H9" t="s">
         <v>484</v>
-      </c>
-      <c r="G9" t="s">
-        <v>485</v>
-      </c>
-      <c r="H9" t="s">
-        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -6602,7 +6611,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
@@ -6611,19 +6620,19 @@
         <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E2" t="s">
         <v>118</v>
       </c>
       <c r="F2" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="G2" t="s">
+        <v>447</v>
+      </c>
+      <c r="H2" t="s">
         <v>450</v>
-      </c>
-      <c r="H2" t="s">
-        <v>453</v>
       </c>
       <c r="I2">
         <v>1.5</v>
@@ -6631,7 +6640,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
@@ -6640,16 +6649,16 @@
         <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E3" t="s">
         <v>118</v>
       </c>
       <c r="F3" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="G3" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="I3">
         <v>10</v>
@@ -6657,7 +6666,7 @@
     </row>
     <row r="4" spans="1:9" ht="45">
       <c r="A4" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B4" t="s">
         <v>36</v>
@@ -6666,16 +6675,16 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E4" t="s">
         <v>188</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="G4" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="I4">
         <v>0.5</v>
@@ -6683,7 +6692,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B5" t="s">
         <v>36</v>
@@ -6692,16 +6701,16 @@
         <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E5" t="s">
         <v>188</v>
       </c>
       <c r="F5" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="G5" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="I5">
         <v>0.23</v>

</xml_diff>

<commit_message>
added LAI without N (except effect of frost and heat)
now LAI decreases from BLS to MAT with a constant rate per biological day. But I had to comment out the effect of frost and heat because they led to NA... I will investigate this.
</commit_message>
<xml_diff>
--- a/allvariables.xlsx
+++ b/allvariables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13600" tabRatio="652" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13680" tabRatio="652" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="nomenclature" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="538">
   <si>
     <t>name</t>
   </si>
@@ -1637,6 +1637,18 @@
   </si>
   <si>
     <t>not really a state variable, but sometimes computed on-the-fly at stage change and must remain the same for the whole stage</t>
+  </si>
+  <si>
+    <t>sDecreaseLAIperBD</t>
+  </si>
+  <si>
+    <t>m2 m-2 bd-1</t>
+  </si>
+  <si>
+    <t>rate of decrease (death) in leaf area index per biologicalday</t>
+  </si>
+  <si>
+    <t>not really a state variable, but sometimes computed on-the-fly at beginning of LAI senescence and must remain the same until the end of the crop</t>
   </si>
 </sst>
 </file>
@@ -1747,8 +1759,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="289">
+  <cellStyleXfs count="301">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2070,7 +2094,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="289">
+  <cellStyles count="301">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -2215,6 +2239,12 @@
     <cellStyle name="Lien hypertexte" xfId="283" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="285" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="299" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -2359,6 +2389,12 @@
     <cellStyle name="Lien hypertexte visité" xfId="284" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="286" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="300" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2723,13 +2759,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:J115"/>
+  <dimension ref="A1:J116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A75" sqref="A75"/>
+      <selection pane="bottomRight" activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5335,7 +5371,7 @@
         <v>26</v>
       </c>
       <c r="D91" t="s">
-        <v>194</v>
+        <v>309</v>
       </c>
       <c r="E91" t="s">
         <v>200</v>
@@ -5893,7 +5929,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:10">
       <c r="A113" t="s">
         <v>130</v>
       </c>
@@ -5923,7 +5959,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:10">
       <c r="A114" t="s">
         <v>110</v>
       </c>
@@ -5953,7 +5989,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:10">
       <c r="A115" t="s">
         <v>109</v>
       </c>
@@ -5981,6 +6017,38 @@
       <c r="I115" t="e">
         <f>NA()</f>
         <v>#N/A</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10">
+      <c r="A116" t="s">
+        <v>534</v>
+      </c>
+      <c r="B116" t="s">
+        <v>483</v>
+      </c>
+      <c r="C116" t="s">
+        <v>26</v>
+      </c>
+      <c r="D116" t="s">
+        <v>309</v>
+      </c>
+      <c r="E116" t="s">
+        <v>535</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="G116" t="s">
+        <v>196</v>
+      </c>
+      <c r="H116" t="s">
+        <v>205</v>
+      </c>
+      <c r="I116">
+        <v>0</v>
+      </c>
+      <c r="J116" t="s">
+        <v>537</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added effect of frost and heat on LAI decrease
</commit_message>
<xml_diff>
--- a/allvariables.xlsx
+++ b/allvariables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13680" tabRatio="652" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13600" tabRatio="652" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="nomenclature" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="549">
   <si>
     <t>name</t>
   </si>
@@ -1649,6 +1649,39 @@
   </si>
   <si>
     <t>not really a state variable, but sometimes computed on-the-fly at beginning of LAI senescence and must remain the same until the end of the crop</t>
+  </si>
+  <si>
+    <t>in the code this is called FRZLDR</t>
+  </si>
+  <si>
+    <t>in the code this is called FRZTKIL</t>
+  </si>
+  <si>
+    <t>in the code this is called HtLTH</t>
+  </si>
+  <si>
+    <t>cFrost</t>
+  </si>
+  <si>
+    <t>cHeat</t>
+  </si>
+  <si>
+    <t>decrease of LAI due to frost</t>
+  </si>
+  <si>
+    <t>decrease of LAI due to heat</t>
+  </si>
+  <si>
+    <t>DLAIF</t>
+  </si>
+  <si>
+    <t>DLAIH</t>
+  </si>
+  <si>
+    <t>décroissance du LAI à cause du froid</t>
+  </si>
+  <si>
+    <t>décroissance du LAI à cause de la chaleur</t>
   </si>
 </sst>
 </file>
@@ -1759,8 +1792,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="301">
+  <cellStyleXfs count="307">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2094,7 +2133,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="301">
+  <cellStyles count="307">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -2245,6 +2284,9 @@
     <cellStyle name="Lien hypertexte" xfId="295" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="297" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="305" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -2395,6 +2437,9 @@
     <cellStyle name="Lien hypertexte visité" xfId="296" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="298" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="306" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2759,13 +2804,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:J116"/>
+  <dimension ref="A1:J118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B89" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A92" sqref="A92"/>
+      <selection pane="bottomRight" activeCell="J113" sqref="J113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4162,7 +4207,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
         <v>324</v>
       </c>
@@ -4189,7 +4234,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:10">
       <c r="A50" t="s">
         <v>300</v>
       </c>
@@ -4216,7 +4261,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:10">
       <c r="A51" t="s">
         <v>301</v>
       </c>
@@ -4243,7 +4288,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:10">
       <c r="A52" t="s">
         <v>302</v>
       </c>
@@ -4270,7 +4315,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:10">
       <c r="A53" t="s">
         <v>296</v>
       </c>
@@ -4297,7 +4342,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:10">
       <c r="A54" s="3" t="s">
         <v>427</v>
       </c>
@@ -4327,7 +4372,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:10">
       <c r="A55" t="s">
         <v>308</v>
       </c>
@@ -4351,7 +4396,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:10">
       <c r="A56" t="s">
         <v>259</v>
       </c>
@@ -4381,7 +4426,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:10">
       <c r="A57" t="s">
         <v>305</v>
       </c>
@@ -4405,7 +4450,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:10">
       <c r="A58" t="s">
         <v>306</v>
       </c>
@@ -4429,7 +4474,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:10">
       <c r="A59" t="s">
         <v>307</v>
       </c>
@@ -4453,7 +4498,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:10">
       <c r="A60" t="s">
         <v>231</v>
       </c>
@@ -4483,7 +4528,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:10">
       <c r="A61" t="s">
         <v>232</v>
       </c>
@@ -4513,7 +4558,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:10">
       <c r="A62" t="s">
         <v>312</v>
       </c>
@@ -4543,7 +4588,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:10">
       <c r="A63" t="s">
         <v>248</v>
       </c>
@@ -4573,7 +4618,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:10">
       <c r="A64" t="s">
         <v>223</v>
       </c>
@@ -4602,8 +4647,11 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="65" spans="1:9">
+      <c r="J64" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65" t="s">
         <v>217</v>
       </c>
@@ -4632,8 +4680,11 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="66" spans="1:9">
+      <c r="J65" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66" t="s">
         <v>310</v>
       </c>
@@ -4657,7 +4708,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:10">
       <c r="A67" t="s">
         <v>311</v>
       </c>
@@ -4680,8 +4731,11 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="68" spans="1:9">
+      <c r="J67" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68" t="s">
         <v>213</v>
       </c>
@@ -4711,7 +4765,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:10">
       <c r="A69" t="s">
         <v>214</v>
       </c>
@@ -4741,7 +4795,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:10">
       <c r="A70" s="6" t="s">
         <v>517</v>
       </c>
@@ -4771,7 +4825,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:10">
       <c r="A71" t="s">
         <v>515</v>
       </c>
@@ -4795,7 +4849,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:10">
       <c r="A72" s="6" t="s">
         <v>179</v>
       </c>
@@ -4825,7 +4879,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:10">
       <c r="A73" t="s">
         <v>61</v>
       </c>
@@ -4855,7 +4909,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:10">
       <c r="A74" t="s">
         <v>60</v>
       </c>
@@ -4885,7 +4939,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:10">
       <c r="A75" t="s">
         <v>58</v>
       </c>
@@ -4915,7 +4969,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:10">
       <c r="A76" t="s">
         <v>482</v>
       </c>
@@ -4945,7 +4999,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:10">
       <c r="A77" t="s">
         <v>414</v>
       </c>
@@ -4975,7 +5029,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:10">
       <c r="A78" t="s">
         <v>404</v>
       </c>
@@ -5005,7 +5059,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:10">
       <c r="A79" t="s">
         <v>468</v>
       </c>
@@ -5035,7 +5089,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:10">
       <c r="A80" s="16" t="s">
         <v>133</v>
       </c>
@@ -6038,9 +6092,6 @@
       <c r="F116" s="3" t="s">
         <v>536</v>
       </c>
-      <c r="G116" t="s">
-        <v>196</v>
-      </c>
       <c r="H116" t="s">
         <v>205</v>
       </c>
@@ -6049,6 +6100,66 @@
       </c>
       <c r="J116" t="s">
         <v>537</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10">
+      <c r="A117" t="s">
+        <v>541</v>
+      </c>
+      <c r="B117" t="s">
+        <v>41</v>
+      </c>
+      <c r="C117" t="s">
+        <v>26</v>
+      </c>
+      <c r="D117" t="s">
+        <v>309</v>
+      </c>
+      <c r="E117" t="s">
+        <v>197</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="G117" t="s">
+        <v>545</v>
+      </c>
+      <c r="H117" t="s">
+        <v>547</v>
+      </c>
+      <c r="I117" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10">
+      <c r="A118" t="s">
+        <v>542</v>
+      </c>
+      <c r="B118" t="s">
+        <v>41</v>
+      </c>
+      <c r="C118" t="s">
+        <v>26</v>
+      </c>
+      <c r="D118" t="s">
+        <v>309</v>
+      </c>
+      <c r="E118" t="s">
+        <v>197</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="G118" t="s">
+        <v>546</v>
+      </c>
+      <c r="H118" t="s">
+        <v>548</v>
+      </c>
+      <c r="I118" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected dry matter production
now I think I corrected all the code left by Dimitri!
</commit_message>
<xml_diff>
--- a/allvariables.xlsx
+++ b/allvariables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13600" tabRatio="652" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21260" windowHeight="12480" tabRatio="652" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="nomenclature" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="560">
   <si>
     <t>name</t>
   </si>
@@ -832,9 +832,6 @@
     <t>Radiation use efficiency adjusted for temperature and water stress</t>
   </si>
   <si>
-    <t>cRadiationUseEffiency</t>
-  </si>
-  <si>
     <t>Efficacité d'utilisation des radiations ajustée à la température et au stress hydrique</t>
   </si>
   <si>
@@ -1513,9 +1510,6 @@
     <t>pas de temps de la dernière récolte</t>
   </si>
   <si>
-    <t>cCoefRadiationEfficiency</t>
-  </si>
-  <si>
     <t>sPlantdensity</t>
   </si>
   <si>
@@ -1558,12 +1552,6 @@
     <t>remark</t>
   </si>
   <si>
-    <t>sCoefWaterstressLeaf</t>
-  </si>
-  <si>
-    <t>not really a state variable, but value from last time step is used by module LAI (which is before water module, which computes it)</t>
-  </si>
-  <si>
     <t>sDailyLeafWeightIncrease</t>
   </si>
   <si>
@@ -1630,12 +1618,6 @@
     <t>incrément journalier de temps thermal</t>
   </si>
   <si>
-    <t>sCoefWaterstressDevelopment</t>
-  </si>
-  <si>
-    <t>sCoefWaterstressDryMatter</t>
-  </si>
-  <si>
     <t>not really a state variable, but sometimes computed on-the-fly at stage change and must remain the same for the whole stage</t>
   </si>
   <si>
@@ -1682,6 +1664,57 @@
   </si>
   <si>
     <t>décroissance du LAI à cause de la chaleur</t>
+  </si>
+  <si>
+    <t>cCoefWaterstressDryMatter</t>
+  </si>
+  <si>
+    <t>cCoefTemperatureRUE</t>
+  </si>
+  <si>
+    <t>cRUE</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>pCoefPAR</t>
+  </si>
+  <si>
+    <t>cCoefWaterstressDevelopment</t>
+  </si>
+  <si>
+    <t>cCoefWaterstressLeaf</t>
+  </si>
+  <si>
+    <t>because computewaterstress functions not coded yet</t>
+  </si>
+  <si>
+    <t>because it should be 0 when there is no vernalization</t>
+  </si>
+  <si>
+    <t>because it should be 1 when there is no vernalization</t>
+  </si>
+  <si>
+    <t>because it sould be 1 outside of temperature sensibility stages</t>
+  </si>
+  <si>
+    <t>because it should be 1 outside of photoperiod sensitivity stages</t>
+  </si>
+  <si>
+    <t>cCoefDrySoilSurface</t>
+  </si>
+  <si>
+    <t>coeficient to stop germination if soil surface is dry</t>
+  </si>
+  <si>
+    <t>arrêt de la germination si le sol est sec en surface</t>
+  </si>
+  <si>
+    <t>because it should be 1 after germination ; I haven't been able to find where in the original model this is used so I don't have the SSM translation</t>
+  </si>
+  <si>
+    <t>because it should be 1 outside of any modifications</t>
   </si>
 </sst>
 </file>
@@ -1792,8 +1825,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="307">
+  <cellStyleXfs count="337">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2133,7 +2196,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="307">
+  <cellStyles count="337">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -2287,6 +2350,21 @@
     <cellStyle name="Lien hypertexte" xfId="301" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="303" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="335" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -2440,6 +2518,21 @@
     <cellStyle name="Lien hypertexte visité" xfId="302" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="304" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="336" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2804,13 +2897,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:J118"/>
+  <dimension ref="A1:J119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B89" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E78" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J113" sqref="J113"/>
+      <selection pane="bottomRight" activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2819,6 +2912,7 @@
     <col min="2" max="2" width="33.6640625" customWidth="1"/>
     <col min="4" max="4" width="26.6640625" customWidth="1"/>
     <col min="6" max="6" width="42.6640625" customWidth="1"/>
+    <col min="8" max="8" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2850,15 +2944,15 @@
         <v>160</v>
       </c>
       <c r="J1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
@@ -2867,16 +2961,16 @@
         <v>258</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="H2" t="s">
         <v>276</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="H2" t="s">
-        <v>277</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2884,10 +2978,10 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
@@ -2896,16 +2990,16 @@
         <v>258</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2913,10 +3007,10 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
@@ -2925,16 +3019,16 @@
         <v>258</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -2942,10 +3036,10 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C5" t="s">
         <v>26</v>
@@ -2960,16 +3054,16 @@
         <v>244</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H5" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2977,7 +3071,7 @@
         <v>193</v>
       </c>
       <c r="B6" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>26</v>
@@ -3003,10 +3097,10 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B7" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
@@ -3032,10 +3126,10 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B8" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C8" t="s">
         <v>26</v>
@@ -3050,7 +3144,7 @@
         <v>236</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H8" t="s">
         <v>237</v>
@@ -3061,10 +3155,10 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="3" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C9" t="s">
         <v>26</v>
@@ -3076,19 +3170,19 @@
         <v>242</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>241</v>
       </c>
       <c r="H9" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -3096,7 +3190,7 @@
         <v>167</v>
       </c>
       <c r="B10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C10" t="s">
         <v>166</v>
@@ -3110,8 +3204,8 @@
       <c r="F10" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="I10">
-        <v>0</v>
+      <c r="I10" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3119,7 +3213,7 @@
         <v>168</v>
       </c>
       <c r="B11" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C11" t="s">
         <v>166</v>
@@ -3133,8 +3227,8 @@
       <c r="F11" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="I11">
-        <v>0</v>
+      <c r="I11" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -3142,7 +3236,7 @@
         <v>178</v>
       </c>
       <c r="B12" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C12" t="s">
         <v>26</v>
@@ -3154,13 +3248,13 @@
         <v>98</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G12" t="s">
         <v>98</v>
       </c>
       <c r="H12" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -3168,10 +3262,10 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B13" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -3183,19 +3277,19 @@
         <v>98</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="G13" t="s">
         <v>98</v>
       </c>
       <c r="H13" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="I13" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="J13" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -3203,7 +3297,7 @@
         <v>161</v>
       </c>
       <c r="B14" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C14" t="s">
         <v>166</v>
@@ -3220,16 +3314,16 @@
       <c r="H14" t="s">
         <v>165</v>
       </c>
-      <c r="I14">
-        <v>0</v>
+      <c r="I14" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C15" t="s">
         <v>26</v>
@@ -3241,10 +3335,10 @@
         <v>181</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H15" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -3252,10 +3346,10 @@
     </row>
     <row r="16" spans="1:10" s="14" customFormat="1">
       <c r="A16" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="B16" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C16" t="s">
         <v>26</v>
@@ -3282,10 +3376,10 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="B17" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C17" t="s">
         <v>26</v>
@@ -3300,7 +3394,7 @@
         <v>207</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H17" t="s">
         <v>209</v>
@@ -3309,33 +3403,33 @@
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E18" t="s">
         <v>113</v>
       </c>
       <c r="F18" t="s">
+        <v>409</v>
+      </c>
+      <c r="G18" t="s">
+        <v>407</v>
+      </c>
+      <c r="H18" t="s">
         <v>410</v>
-      </c>
-      <c r="G18" t="s">
-        <v>408</v>
-      </c>
-      <c r="H18" t="s">
-        <v>411</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -3343,81 +3437,81 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
+        <v>484</v>
+      </c>
+      <c r="B19" t="s">
+        <v>482</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
         <v>485</v>
       </c>
-      <c r="B19" t="s">
-        <v>483</v>
-      </c>
-      <c r="C19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>486</v>
       </c>
-      <c r="E19" t="s">
-        <v>487</v>
-      </c>
       <c r="F19" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H19" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="J19" s="14"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B20" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C20" t="s">
         <v>26</v>
       </c>
       <c r="D20" t="s">
+        <v>485</v>
+      </c>
+      <c r="E20" t="s">
         <v>486</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>487</v>
       </c>
-      <c r="F20" t="s">
-        <v>488</v>
-      </c>
       <c r="H20" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I20" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C21" t="s">
         <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E21" t="s">
         <v>181</v>
       </c>
       <c r="F21" t="s">
+        <v>454</v>
+      </c>
+      <c r="G21" t="s">
         <v>455</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>456</v>
-      </c>
-      <c r="H21" t="s">
-        <v>457</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -3425,28 +3519,28 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B22" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C22" t="s">
         <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E22" t="s">
+        <v>445</v>
+      </c>
+      <c r="F22" t="s">
+        <v>444</v>
+      </c>
+      <c r="G22" t="s">
+        <v>443</v>
+      </c>
+      <c r="H22" t="s">
         <v>446</v>
-      </c>
-      <c r="F22" t="s">
-        <v>445</v>
-      </c>
-      <c r="G22" t="s">
-        <v>444</v>
-      </c>
-      <c r="H22" t="s">
-        <v>447</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -3454,28 +3548,28 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B23" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C23" t="s">
         <v>26</v>
       </c>
       <c r="D23" t="s">
+        <v>365</v>
+      </c>
+      <c r="E23" t="s">
         <v>366</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>367</v>
       </c>
-      <c r="F23" t="s">
-        <v>368</v>
-      </c>
       <c r="G23" t="s">
+        <v>377</v>
+      </c>
+      <c r="H23" t="s">
         <v>378</v>
-      </c>
-      <c r="H23" t="s">
-        <v>379</v>
       </c>
       <c r="I23">
         <v>0.5</v>
@@ -3483,28 +3577,28 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
+        <v>364</v>
+      </c>
+      <c r="B24" t="s">
+        <v>482</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" t="s">
         <v>365</v>
       </c>
-      <c r="B24" t="s">
-        <v>483</v>
-      </c>
-      <c r="C24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>366</v>
       </c>
-      <c r="E24" t="s">
-        <v>367</v>
-      </c>
       <c r="F24" t="s">
+        <v>376</v>
+      </c>
+      <c r="G24" t="s">
         <v>377</v>
       </c>
-      <c r="G24" t="s">
-        <v>378</v>
-      </c>
       <c r="H24" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I24">
         <v>0.5</v>
@@ -3512,28 +3606,28 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B25" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C25" t="s">
         <v>26</v>
       </c>
       <c r="D25" t="s">
+        <v>365</v>
+      </c>
+      <c r="E25" t="s">
         <v>366</v>
       </c>
-      <c r="E25" t="s">
-        <v>367</v>
-      </c>
       <c r="F25" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G25" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I25">
         <v>0.5</v>
@@ -3541,28 +3635,28 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B26" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C26" t="s">
         <v>26</v>
       </c>
       <c r="D26" t="s">
+        <v>365</v>
+      </c>
+      <c r="E26" t="s">
         <v>366</v>
       </c>
-      <c r="E26" t="s">
-        <v>367</v>
-      </c>
       <c r="F26" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G26" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H26" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I26">
         <v>0.5</v>
@@ -3570,28 +3664,28 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B27" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C27" t="s">
         <v>26</v>
       </c>
       <c r="D27" t="s">
+        <v>365</v>
+      </c>
+      <c r="E27" t="s">
         <v>366</v>
       </c>
-      <c r="E27" t="s">
-        <v>367</v>
-      </c>
       <c r="F27" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G27" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H27" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I27">
         <v>0.5</v>
@@ -3599,28 +3693,28 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B28" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C28" t="s">
         <v>26</v>
       </c>
       <c r="D28" t="s">
+        <v>365</v>
+      </c>
+      <c r="E28" t="s">
         <v>366</v>
       </c>
-      <c r="E28" t="s">
-        <v>367</v>
-      </c>
       <c r="F28" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G28" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H28" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I28">
         <v>0.5</v>
@@ -3628,28 +3722,28 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B29" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C29" t="s">
         <v>26</v>
       </c>
       <c r="D29" t="s">
+        <v>365</v>
+      </c>
+      <c r="E29" t="s">
         <v>366</v>
       </c>
-      <c r="E29" t="s">
-        <v>367</v>
-      </c>
       <c r="F29" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G29" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H29" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I29">
         <v>0.5</v>
@@ -3657,28 +3751,28 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B30" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C30" t="s">
         <v>26</v>
       </c>
       <c r="D30" t="s">
+        <v>365</v>
+      </c>
+      <c r="E30" t="s">
         <v>366</v>
       </c>
-      <c r="E30" t="s">
-        <v>367</v>
-      </c>
       <c r="F30" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G30" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H30" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I30">
         <v>0.5</v>
@@ -3686,28 +3780,28 @@
     </row>
     <row r="31" spans="1:10" s="4" customFormat="1">
       <c r="A31" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B31" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C31" t="s">
         <v>26</v>
       </c>
       <c r="D31" t="s">
+        <v>365</v>
+      </c>
+      <c r="E31" t="s">
         <v>366</v>
       </c>
-      <c r="E31" t="s">
-        <v>367</v>
-      </c>
       <c r="F31" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G31" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H31" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I31">
         <v>0.5</v>
@@ -3716,28 +3810,28 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B32" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C32" t="s">
         <v>26</v>
       </c>
       <c r="D32" t="s">
+        <v>365</v>
+      </c>
+      <c r="E32" t="s">
         <v>366</v>
       </c>
-      <c r="E32" t="s">
-        <v>367</v>
-      </c>
       <c r="F32" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G32" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H32" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I32">
         <v>0.5</v>
@@ -3745,16 +3839,16 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>531</v>
+        <v>548</v>
       </c>
       <c r="B33" t="s">
-        <v>483</v>
+        <v>41</v>
       </c>
       <c r="C33" t="s">
         <v>26</v>
       </c>
       <c r="D33" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E33" t="s">
         <v>163</v>
@@ -3772,53 +3866,53 @@
         <v>1</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>508</v>
+        <v>550</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>532</v>
+        <v>543</v>
       </c>
       <c r="B34" t="s">
-        <v>483</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
         <v>26</v>
       </c>
       <c r="D34" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>181</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H34" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I34">
         <v>1</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>508</v>
+        <v>550</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>507</v>
+        <v>549</v>
       </c>
       <c r="B35" t="s">
-        <v>483</v>
+        <v>41</v>
       </c>
       <c r="C35" t="s">
         <v>26</v>
       </c>
       <c r="D35" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E35" t="s">
         <v>163</v>
@@ -3836,7 +3930,7 @@
         <v>1</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>508</v>
+        <v>550</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -3844,13 +3938,13 @@
         <v>155</v>
       </c>
       <c r="B36" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C36" t="s">
         <v>26</v>
       </c>
       <c r="D36" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E36" t="s">
         <v>119</v>
@@ -3873,7 +3967,7 @@
         <v>104</v>
       </c>
       <c r="B37" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C37" t="s">
         <v>26</v>
@@ -4047,7 +4141,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B43" t="s">
         <v>138</v>
@@ -4059,13 +4153,13 @@
         <v>258</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I43" t="e">
         <f>NA()</f>
@@ -4074,7 +4168,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B44" t="s">
         <v>138</v>
@@ -4086,13 +4180,13 @@
         <v>258</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G44" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I44" t="e">
         <f>NA()</f>
@@ -4101,7 +4195,7 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B45" t="s">
         <v>138</v>
@@ -4113,13 +4207,13 @@
         <v>258</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G45" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I45" t="e">
         <f>NA()</f>
@@ -4128,7 +4222,7 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B46" t="s">
         <v>138</v>
@@ -4140,13 +4234,13 @@
         <v>258</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G46" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I46" t="e">
         <f>NA()</f>
@@ -4155,7 +4249,7 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B47" t="s">
         <v>138</v>
@@ -4167,13 +4261,13 @@
         <v>258</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G47" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I47" t="e">
         <f>NA()</f>
@@ -4182,7 +4276,7 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B48" t="s">
         <v>138</v>
@@ -4194,13 +4288,13 @@
         <v>258</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G48" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I48" t="e">
         <f>NA()</f>
@@ -4209,7 +4303,7 @@
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B49" t="s">
         <v>138</v>
@@ -4221,13 +4315,13 @@
         <v>258</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G49" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I49" t="e">
         <f>NA()</f>
@@ -4236,7 +4330,7 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B50" t="s">
         <v>138</v>
@@ -4248,13 +4342,13 @@
         <v>258</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G50" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I50" t="e">
         <f>NA()</f>
@@ -4263,7 +4357,7 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B51" t="s">
         <v>138</v>
@@ -4275,13 +4369,13 @@
         <v>258</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G51" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I51" t="e">
         <f>NA()</f>
@@ -4290,7 +4384,7 @@
     </row>
     <row r="52" spans="1:10">
       <c r="A52" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B52" t="s">
         <v>138</v>
@@ -4302,13 +4396,13 @@
         <v>258</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G52" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I52" t="e">
         <f>NA()</f>
@@ -4317,7 +4411,7 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B53" t="s">
         <v>138</v>
@@ -4329,13 +4423,13 @@
         <v>258</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G53" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I53" t="e">
         <f>NA()</f>
@@ -4344,7 +4438,7 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B54" t="s">
         <v>138</v>
@@ -4359,13 +4453,13 @@
         <v>181</v>
       </c>
       <c r="F54" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="H54" t="s">
         <v>270</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="H54" t="s">
-        <v>271</v>
       </c>
       <c r="I54" t="e">
         <f>NA()</f>
@@ -4374,7 +4468,7 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B55" t="s">
         <v>138</v>
@@ -4386,10 +4480,10 @@
         <v>245</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I55" t="e">
         <f>NA()</f>
@@ -4416,7 +4510,7 @@
         <v>257</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H56" t="s">
         <v>260</v>
@@ -4428,7 +4522,7 @@
     </row>
     <row r="57" spans="1:10">
       <c r="A57" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B57" t="s">
         <v>138</v>
@@ -4440,10 +4534,10 @@
         <v>245</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I57" t="e">
         <f>NA()</f>
@@ -4452,7 +4546,7 @@
     </row>
     <row r="58" spans="1:10">
       <c r="A58" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B58" t="s">
         <v>138</v>
@@ -4464,10 +4558,10 @@
         <v>245</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I58" t="e">
         <f>NA()</f>
@@ -4476,7 +4570,7 @@
     </row>
     <row r="59" spans="1:10">
       <c r="A59" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B59" t="s">
         <v>138</v>
@@ -4488,10 +4582,10 @@
         <v>245</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I59" t="e">
         <f>NA()</f>
@@ -4509,7 +4603,7 @@
         <v>26</v>
       </c>
       <c r="D60" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E60" s="7" t="s">
         <v>181</v>
@@ -4518,7 +4612,7 @@
         <v>229</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H60" t="s">
         <v>233</v>
@@ -4539,7 +4633,7 @@
         <v>26</v>
       </c>
       <c r="D61" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E61" s="7" t="s">
         <v>181</v>
@@ -4548,7 +4642,7 @@
         <v>230</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="H61" t="s">
         <v>234</v>
@@ -4560,7 +4654,7 @@
     </row>
     <row r="62" spans="1:10">
       <c r="A62" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B62" t="s">
         <v>138</v>
@@ -4569,7 +4663,7 @@
         <v>26</v>
       </c>
       <c r="D62" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E62" s="7" t="s">
         <v>225</v>
@@ -4578,7 +4672,7 @@
         <v>224</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>224</v>
@@ -4599,7 +4693,7 @@
         <v>26</v>
       </c>
       <c r="D63" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E63" s="7" t="s">
         <v>249</v>
@@ -4629,7 +4723,7 @@
         <v>26</v>
       </c>
       <c r="D64" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E64" s="9" t="s">
         <v>222</v>
@@ -4638,7 +4732,7 @@
         <v>218</v>
       </c>
       <c r="G64" s="18" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H64" t="s">
         <v>221</v>
@@ -4648,7 +4742,7 @@
         <v>#N/A</v>
       </c>
       <c r="J64" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -4662,7 +4756,7 @@
         <v>26</v>
       </c>
       <c r="D65" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E65" t="s">
         <v>15</v>
@@ -4671,7 +4765,7 @@
         <v>219</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="H65" t="s">
         <v>220</v>
@@ -4681,12 +4775,12 @@
         <v>#N/A</v>
       </c>
       <c r="J65" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B66" t="s">
         <v>138</v>
@@ -4695,13 +4789,13 @@
         <v>26</v>
       </c>
       <c r="D66" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I66" t="e">
         <f>NA()</f>
@@ -4710,7 +4804,7 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B67" t="s">
         <v>138</v>
@@ -4719,20 +4813,20 @@
         <v>26</v>
       </c>
       <c r="D67" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E67" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I67" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
       <c r="J67" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -4746,7 +4840,7 @@
         <v>26</v>
       </c>
       <c r="D68" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E68" s="7" t="s">
         <v>211</v>
@@ -4755,7 +4849,7 @@
         <v>210</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H68" t="s">
         <v>215</v>
@@ -4776,7 +4870,7 @@
         <v>26</v>
       </c>
       <c r="D69" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E69" s="7" t="s">
         <v>211</v>
@@ -4785,7 +4879,7 @@
         <v>212</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H69" t="s">
         <v>216</v>
@@ -4797,7 +4891,7 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="6" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B70" t="s">
         <v>138</v>
@@ -4827,7 +4921,7 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="B71" t="s">
         <v>138</v>
@@ -4839,10 +4933,10 @@
         <v>95</v>
       </c>
       <c r="F71" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="H71" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="I71" t="e">
         <f>NA()</f>
@@ -4971,7 +5065,7 @@
     </row>
     <row r="76" spans="1:10">
       <c r="A76" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B76" t="s">
         <v>138</v>
@@ -5001,7 +5095,7 @@
     </row>
     <row r="77" spans="1:10">
       <c r="A77" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B77" t="s">
         <v>138</v>
@@ -5010,19 +5104,19 @@
         <v>26</v>
       </c>
       <c r="D77" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E77" t="s">
         <v>113</v>
       </c>
       <c r="F77" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="G77" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="G77" s="3" t="s">
-        <v>413</v>
-      </c>
       <c r="H77" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I77" t="e">
         <f>NA()</f>
@@ -5031,7 +5125,7 @@
     </row>
     <row r="78" spans="1:10">
       <c r="A78" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B78" t="s">
         <v>138</v>
@@ -5040,19 +5134,19 @@
         <v>26</v>
       </c>
       <c r="D78" t="s">
+        <v>404</v>
+      </c>
+      <c r="E78" s="7" t="s">
         <v>405</v>
       </c>
-      <c r="E78" s="7" t="s">
+      <c r="F78" t="s">
+        <v>401</v>
+      </c>
+      <c r="G78" t="s">
+        <v>402</v>
+      </c>
+      <c r="H78" t="s">
         <v>406</v>
-      </c>
-      <c r="F78" t="s">
-        <v>402</v>
-      </c>
-      <c r="G78" t="s">
-        <v>403</v>
-      </c>
-      <c r="H78" t="s">
-        <v>407</v>
       </c>
       <c r="I78" t="e">
         <f>NA()</f>
@@ -5061,7 +5155,7 @@
     </row>
     <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B79" t="s">
         <v>138</v>
@@ -5070,19 +5164,19 @@
         <v>26</v>
       </c>
       <c r="D79" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E79" t="s">
         <v>181</v>
       </c>
       <c r="F79" t="s">
+        <v>465</v>
+      </c>
+      <c r="G79" t="s">
         <v>466</v>
       </c>
-      <c r="G79" t="s">
-        <v>467</v>
-      </c>
       <c r="H79" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I79" t="e">
         <f>NA()</f>
@@ -5100,7 +5194,7 @@
         <v>26</v>
       </c>
       <c r="D80" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E80" t="s">
         <v>15</v>
@@ -5109,7 +5203,7 @@
         <v>141</v>
       </c>
       <c r="G80" s="16" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H80" t="s">
         <v>151</v>
@@ -5119,7 +5213,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:10">
       <c r="A81" s="16" t="s">
         <v>136</v>
       </c>
@@ -5130,7 +5224,7 @@
         <v>26</v>
       </c>
       <c r="D81" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E81" t="s">
         <v>15</v>
@@ -5139,7 +5233,7 @@
         <v>137</v>
       </c>
       <c r="G81" s="16" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H81" t="s">
         <v>149</v>
@@ -5149,7 +5243,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:10">
       <c r="A82" s="16" t="s">
         <v>134</v>
       </c>
@@ -5160,7 +5254,7 @@
         <v>26</v>
       </c>
       <c r="D82" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E82" t="s">
         <v>15</v>
@@ -5169,7 +5263,7 @@
         <v>131</v>
       </c>
       <c r="G82" s="16" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H82" t="s">
         <v>152</v>
@@ -5179,9 +5273,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:10">
       <c r="A83" s="16" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B83" t="s">
         <v>138</v>
@@ -5190,7 +5284,7 @@
         <v>26</v>
       </c>
       <c r="D83" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E83" t="s">
         <v>15</v>
@@ -5199,7 +5293,7 @@
         <v>132</v>
       </c>
       <c r="G83" s="16" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H83" t="s">
         <v>153</v>
@@ -5209,9 +5303,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:10">
       <c r="A84" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B84" t="s">
         <v>138</v>
@@ -5220,14 +5314,14 @@
         <v>26</v>
       </c>
       <c r="D84" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="5" t="s">
         <v>143</v>
       </c>
       <c r="G84" s="16" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H84" s="4" t="s">
         <v>148</v>
@@ -5237,7 +5331,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:10">
       <c r="A85" t="s">
         <v>145</v>
       </c>
@@ -5248,7 +5342,7 @@
         <v>26</v>
       </c>
       <c r="D85" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F85" s="3" t="s">
         <v>142</v>
@@ -5264,7 +5358,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:10">
       <c r="A86" t="s">
         <v>35</v>
       </c>
@@ -5294,9 +5388,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:10">
       <c r="A87" t="s">
-        <v>492</v>
+        <v>544</v>
       </c>
       <c r="B87" t="s">
         <v>41</v>
@@ -5314,7 +5408,7 @@
         <v>262</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H87" t="s">
         <v>263</v>
@@ -5324,9 +5418,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:10">
       <c r="A88" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B88" t="s">
         <v>41</v>
@@ -5341,22 +5435,22 @@
         <v>243</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H88" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I88" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:10">
       <c r="A89" t="s">
-        <v>265</v>
+        <v>545</v>
       </c>
       <c r="B89" t="s">
         <v>41</v>
@@ -5374,17 +5468,17 @@
         <v>264</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H89" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I89" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:10">
       <c r="A90" t="s">
         <v>251</v>
       </c>
@@ -5414,7 +5508,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:10">
       <c r="A91" t="s">
         <v>206</v>
       </c>
@@ -5425,7 +5519,7 @@
         <v>26</v>
       </c>
       <c r="D91" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E91" t="s">
         <v>200</v>
@@ -5444,7 +5538,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:10">
       <c r="A92" t="s">
         <v>202</v>
       </c>
@@ -5474,7 +5568,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:10">
       <c r="A93" t="s">
         <v>88</v>
       </c>
@@ -5499,12 +5593,14 @@
       <c r="H93" t="s">
         <v>97</v>
       </c>
-      <c r="I93" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9">
+      <c r="I93">
+        <v>1</v>
+      </c>
+      <c r="J93" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
       <c r="A94" t="s">
         <v>71</v>
       </c>
@@ -5529,14 +5625,16 @@
       <c r="H94" t="s">
         <v>74</v>
       </c>
-      <c r="I94" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9">
+      <c r="I94">
+        <v>1</v>
+      </c>
+      <c r="J94" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
       <c r="A95" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="B95" t="s">
         <v>41</v>
@@ -5551,20 +5649,22 @@
         <v>15</v>
       </c>
       <c r="F95" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="G95" t="s">
         <v>98</v>
       </c>
       <c r="H95" t="s">
-        <v>528</v>
-      </c>
-      <c r="I95" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9">
+        <v>524</v>
+      </c>
+      <c r="I95">
+        <v>1</v>
+      </c>
+      <c r="J95" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
       <c r="A96" t="s">
         <v>75</v>
       </c>
@@ -5581,20 +5681,20 @@
         <v>15</v>
       </c>
       <c r="F96" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="G96" t="s">
         <v>77</v>
       </c>
       <c r="H96" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="I96" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:10">
       <c r="A97" s="16" t="s">
         <v>174</v>
       </c>
@@ -5620,7 +5720,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:10">
       <c r="A98" t="s">
         <v>177</v>
       </c>
@@ -5650,7 +5750,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:10">
       <c r="A99" t="s">
         <v>53</v>
       </c>
@@ -5680,9 +5780,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:10">
       <c r="A100" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B100" t="s">
         <v>41</v>
@@ -5691,22 +5791,22 @@
         <v>26</v>
       </c>
       <c r="D100" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E100" t="s">
         <v>113</v>
       </c>
       <c r="G100" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I100" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:10">
       <c r="A101" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B101" t="s">
         <v>41</v>
@@ -5715,7 +5815,7 @@
         <v>26</v>
       </c>
       <c r="D101" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E101" t="s">
         <v>113</v>
@@ -5725,9 +5825,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:10">
       <c r="A102" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B102" t="s">
         <v>41</v>
@@ -5736,7 +5836,7 @@
         <v>26</v>
       </c>
       <c r="D102" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E102" t="s">
         <v>113</v>
@@ -5746,9 +5846,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:10">
       <c r="A103" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B103" t="s">
         <v>41</v>
@@ -5757,7 +5857,7 @@
         <v>26</v>
       </c>
       <c r="D103" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E103" t="s">
         <v>113</v>
@@ -5767,9 +5867,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:10">
       <c r="A104" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B104" t="s">
         <v>41</v>
@@ -5778,7 +5878,7 @@
         <v>26</v>
       </c>
       <c r="D104" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E104" t="s">
         <v>113</v>
@@ -5788,9 +5888,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:10">
       <c r="A105" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B105" t="s">
         <v>41</v>
@@ -5799,7 +5899,7 @@
         <v>26</v>
       </c>
       <c r="D105" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E105" t="s">
         <v>113</v>
@@ -5809,9 +5909,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:10">
       <c r="A106" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B106" t="s">
         <v>41</v>
@@ -5820,7 +5920,7 @@
         <v>26</v>
       </c>
       <c r="D106" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E106" t="s">
         <v>113</v>
@@ -5830,9 +5930,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:10">
       <c r="A107" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B107" t="s">
         <v>41</v>
@@ -5841,7 +5941,7 @@
         <v>26</v>
       </c>
       <c r="D107" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E107" t="s">
         <v>113</v>
@@ -5851,9 +5951,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:10">
       <c r="A108" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B108" t="s">
         <v>41</v>
@@ -5862,7 +5962,7 @@
         <v>26</v>
       </c>
       <c r="D108" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E108" t="s">
         <v>113</v>
@@ -5872,9 +5972,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:10">
       <c r="A109" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B109" t="s">
         <v>41</v>
@@ -5883,7 +5983,7 @@
         <v>26</v>
       </c>
       <c r="D109" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E109" t="s">
         <v>113</v>
@@ -5893,9 +5993,9 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:10">
       <c r="A110" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B110" t="s">
         <v>41</v>
@@ -5904,26 +6004,26 @@
         <v>26</v>
       </c>
       <c r="D110" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E110" t="s">
         <v>113</v>
       </c>
       <c r="F110" t="s">
+        <v>458</v>
+      </c>
+      <c r="G110" t="s">
         <v>459</v>
       </c>
-      <c r="G110" t="s">
+      <c r="H110" t="s">
         <v>460</v>
       </c>
-      <c r="H110" t="s">
-        <v>461</v>
-      </c>
       <c r="I110" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:10">
       <c r="A111" t="s">
         <v>99</v>
       </c>
@@ -5948,12 +6048,14 @@
       <c r="H111" t="s">
         <v>102</v>
       </c>
-      <c r="I111" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9">
+      <c r="I111">
+        <v>1</v>
+      </c>
+      <c r="J111" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10">
       <c r="A112" t="s">
         <v>124</v>
       </c>
@@ -6008,9 +6110,11 @@
       <c r="H113" t="s">
         <v>150</v>
       </c>
-      <c r="I113" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="I113">
+        <v>0</v>
+      </c>
+      <c r="J113" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="114" spans="1:10">
@@ -6075,22 +6179,22 @@
     </row>
     <row r="116" spans="1:10">
       <c r="A116" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="B116" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C116" t="s">
         <v>26</v>
       </c>
       <c r="D116" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E116" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="H116" t="s">
         <v>205</v>
@@ -6099,12 +6203,12 @@
         <v>0</v>
       </c>
       <c r="J116" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
     </row>
     <row r="117" spans="1:10">
       <c r="A117" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="B117" t="s">
         <v>41</v>
@@ -6113,19 +6217,19 @@
         <v>26</v>
       </c>
       <c r="D117" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E117" t="s">
         <v>197</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="G117" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="H117" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="I117" t="e">
         <f>NA()</f>
@@ -6134,7 +6238,7 @@
     </row>
     <row r="118" spans="1:10">
       <c r="A118" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="B118" t="s">
         <v>41</v>
@@ -6143,23 +6247,52 @@
         <v>26</v>
       </c>
       <c r="D118" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E118" t="s">
         <v>197</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="G118" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="H118" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="I118" t="e">
         <f>NA()</f>
         <v>#N/A</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
+      <c r="A119" t="s">
+        <v>555</v>
+      </c>
+      <c r="B119" t="s">
+        <v>41</v>
+      </c>
+      <c r="C119" t="s">
+        <v>26</v>
+      </c>
+      <c r="D119" t="s">
+        <v>95</v>
+      </c>
+      <c r="E119" t="s">
+        <v>163</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="H119" t="s">
+        <v>557</v>
+      </c>
+      <c r="I119">
+        <v>1</v>
+      </c>
+      <c r="J119" t="s">
+        <v>558</v>
       </c>
     </row>
   </sheetData>
@@ -6223,207 +6356,207 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
         <v>416</v>
-      </c>
-      <c r="B2" t="s">
-        <v>390</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>417</v>
       </c>
       <c r="E2" t="s">
         <v>181</v>
       </c>
       <c r="F2" t="s">
+        <v>417</v>
+      </c>
+      <c r="G2" t="s">
         <v>418</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>419</v>
-      </c>
-      <c r="H2" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
+        <v>420</v>
+      </c>
+      <c r="B3" t="s">
+        <v>389</v>
+      </c>
+      <c r="C3" t="s">
         <v>421</v>
       </c>
-      <c r="B3" t="s">
-        <v>390</v>
-      </c>
-      <c r="C3" t="s">
-        <v>422</v>
-      </c>
       <c r="D3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E3" t="s">
+        <v>398</v>
+      </c>
+      <c r="F3" t="s">
+        <v>447</v>
+      </c>
+      <c r="G3" t="s">
+        <v>400</v>
+      </c>
+      <c r="H3" t="s">
         <v>399</v>
-      </c>
-      <c r="F3" t="s">
-        <v>448</v>
-      </c>
-      <c r="G3" t="s">
-        <v>401</v>
-      </c>
-      <c r="H3" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E4" t="s">
+        <v>395</v>
+      </c>
+      <c r="F4" t="s">
+        <v>448</v>
+      </c>
+      <c r="G4" t="s">
         <v>396</v>
       </c>
-      <c r="F4" t="s">
-        <v>449</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>397</v>
-      </c>
-      <c r="H4" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G5" t="s">
+        <v>393</v>
+      </c>
+      <c r="H5" t="s">
         <v>394</v>
-      </c>
-      <c r="H5" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G6" t="s">
+        <v>391</v>
+      </c>
+      <c r="H6" t="s">
         <v>392</v>
-      </c>
-      <c r="H6" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B7" t="s">
+        <v>389</v>
+      </c>
+      <c r="C7" t="s">
+        <v>421</v>
+      </c>
+      <c r="D7" t="s">
+        <v>416</v>
+      </c>
+      <c r="E7" t="s">
+        <v>395</v>
+      </c>
+      <c r="F7" t="s">
+        <v>451</v>
+      </c>
+      <c r="G7" t="s">
+        <v>388</v>
+      </c>
+      <c r="H7" t="s">
         <v>390</v>
-      </c>
-      <c r="C7" t="s">
-        <v>422</v>
-      </c>
-      <c r="D7" t="s">
-        <v>417</v>
-      </c>
-      <c r="E7" t="s">
-        <v>396</v>
-      </c>
-      <c r="F7" t="s">
-        <v>452</v>
-      </c>
-      <c r="G7" t="s">
-        <v>389</v>
-      </c>
-      <c r="H7" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C8" t="s">
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E8" t="s">
         <v>181</v>
       </c>
       <c r="F8" t="s">
+        <v>441</v>
+      </c>
+      <c r="G8" t="s">
+        <v>440</v>
+      </c>
+      <c r="H8" t="s">
         <v>442</v>
-      </c>
-      <c r="G8" t="s">
-        <v>441</v>
-      </c>
-      <c r="H8" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
+        <v>463</v>
+      </c>
+      <c r="B9" t="s">
+        <v>389</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>416</v>
+      </c>
+      <c r="F9" t="s">
+        <v>461</v>
+      </c>
+      <c r="G9" t="s">
+        <v>462</v>
+      </c>
+      <c r="H9" t="s">
         <v>464</v>
-      </c>
-      <c r="B9" t="s">
-        <v>390</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>417</v>
-      </c>
-      <c r="F9" t="s">
-        <v>462</v>
-      </c>
-      <c r="G9" t="s">
-        <v>463</v>
-      </c>
-      <c r="H9" t="s">
-        <v>465</v>
       </c>
     </row>
   </sheetData>
@@ -6930,7 +7063,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6966,7 +7099,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
@@ -6975,19 +7108,19 @@
         <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E2" t="s">
         <v>113</v>
       </c>
       <c r="F2" t="s">
+        <v>429</v>
+      </c>
+      <c r="G2" t="s">
+        <v>427</v>
+      </c>
+      <c r="H2" t="s">
         <v>430</v>
-      </c>
-      <c r="G2" t="s">
-        <v>428</v>
-      </c>
-      <c r="H2" t="s">
-        <v>431</v>
       </c>
       <c r="I2">
         <v>1.5</v>
@@ -6995,7 +7128,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
@@ -7004,16 +7137,16 @@
         <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E3" t="s">
         <v>113</v>
       </c>
       <c r="F3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="I3">
         <v>10</v>
@@ -7021,7 +7154,7 @@
     </row>
     <row r="4" spans="1:9" ht="45">
       <c r="A4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B4" t="s">
         <v>36</v>
@@ -7030,16 +7163,16 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E4" t="s">
         <v>181</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I4">
         <v>0.5</v>
@@ -7047,7 +7180,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B5" t="s">
         <v>36</v>
@@ -7056,16 +7189,16 @@
         <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E5" t="s">
         <v>181</v>
       </c>
       <c r="F5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I5">
         <v>0.23</v>
@@ -7073,7 +7206,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>547</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
started including soil water module
reading of excel soils file added,
root depth growth included
the rest hasn't been adapted to the model yet
</commit_message>
<xml_diff>
--- a/allvariables.xlsx
+++ b/allvariables.xlsx
@@ -1964,14 +1964,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2077,395 +2070,395 @@
   </borders>
   <cellStyleXfs count="359">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3196,10 +3189,10 @@
   <dimension ref="A1:J132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B95" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A92" sqref="A92"/>
+      <selection pane="bottomRight" activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
just added export of drainage
</commit_message>
<xml_diff>
--- a/allvariables.xlsx
+++ b/allvariables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="715">
   <si>
     <t>name</t>
   </si>
@@ -2228,6 +2228,18 @@
   </si>
   <si>
     <t>ruissellement</t>
+  </si>
+  <si>
+    <t>cDrain</t>
+  </si>
+  <si>
+    <t>DRAIN</t>
+  </si>
+  <si>
+    <t>amount of water drained below the drain layer</t>
+  </si>
+  <si>
+    <t>drainage sortant</t>
   </si>
 </sst>
 </file>
@@ -3647,13 +3659,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:J145"/>
+  <dimension ref="A1:J146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B132" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="I145" sqref="I145:I146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7678,6 +7690,9 @@
       <c r="D141" t="s">
         <v>373</v>
       </c>
+      <c r="E141" t="s">
+        <v>112</v>
+      </c>
       <c r="F141" t="s">
         <v>703</v>
       </c>
@@ -7705,6 +7720,9 @@
       <c r="D142" t="s">
         <v>373</v>
       </c>
+      <c r="E142" t="s">
+        <v>112</v>
+      </c>
       <c r="F142" t="s">
         <v>700</v>
       </c>
@@ -7732,6 +7750,9 @@
       <c r="D143" t="s">
         <v>373</v>
       </c>
+      <c r="E143" t="s">
+        <v>112</v>
+      </c>
       <c r="F143" t="s">
         <v>705</v>
       </c>
@@ -7759,6 +7780,9 @@
       <c r="D144" t="s">
         <v>373</v>
       </c>
+      <c r="E144" t="s">
+        <v>112</v>
+      </c>
       <c r="F144" t="s">
         <v>706</v>
       </c>
@@ -7786,6 +7810,9 @@
       <c r="D145" t="s">
         <v>373</v>
       </c>
+      <c r="E145" t="s">
+        <v>112</v>
+      </c>
       <c r="F145" t="s">
         <v>707</v>
       </c>
@@ -7796,6 +7823,36 @@
         <v>707</v>
       </c>
       <c r="I145" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9">
+      <c r="A146" t="s">
+        <v>711</v>
+      </c>
+      <c r="B146" t="s">
+        <v>41</v>
+      </c>
+      <c r="C146" t="s">
+        <v>26</v>
+      </c>
+      <c r="D146" t="s">
+        <v>373</v>
+      </c>
+      <c r="E146" t="s">
+        <v>112</v>
+      </c>
+      <c r="F146" t="s">
+        <v>713</v>
+      </c>
+      <c r="G146" t="s">
+        <v>712</v>
+      </c>
+      <c r="H146" t="s">
+        <v>714</v>
+      </c>
+      <c r="I146" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>

</xml_diff>

<commit_message>
corrected bug on harvest
reinitialize state variables at harvest
changed sCycleEndType to computed variable rather than state variable
</commit_message>
<xml_diff>
--- a/allvariables.xlsx
+++ b/allvariables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="751">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1499" uniqueCount="749">
   <si>
     <t>name</t>
   </si>
@@ -2317,12 +2317,6 @@
     <t>code de fin de culture</t>
   </si>
   <si>
-    <t>sCycleEndType</t>
-  </si>
-  <si>
-    <t>not really a state variable, but just to keep the levels of the factor</t>
-  </si>
-  <si>
     <t>factor</t>
   </si>
   <si>
@@ -2347,7 +2341,7 @@
     <t>facteur de stress hydrique par excès d'eau</t>
   </si>
   <si>
-    <t>"not yet"</t>
+    <t>cCycleEndType</t>
   </si>
 </sst>
 </file>
@@ -2463,8 +2457,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="479">
+  <cellStyleXfs count="481">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2980,7 +2976,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="479">
+  <cellStyles count="481">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -3220,6 +3216,7 @@
     <cellStyle name="Lien hypertexte" xfId="473" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="475" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="477" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="479" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -3459,6 +3456,7 @@
     <cellStyle name="Lien hypertexte visité" xfId="474" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="476" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="478" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="480" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3826,10 +3824,10 @@
   <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3875,68 +3873,58 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>740</v>
+        <v>164</v>
       </c>
       <c r="B2" t="s">
         <v>423</v>
       </c>
       <c r="C2" t="s">
-        <v>742</v>
+        <v>163</v>
       </c>
       <c r="D2" t="s">
         <v>426</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="F2" t="s">
-        <v>738</v>
-      </c>
-      <c r="G2" t="s">
-        <v>246</v>
-      </c>
-      <c r="H2" t="s">
-        <v>739</v>
-      </c>
-      <c r="I2" t="s">
-        <v>750</v>
-      </c>
-      <c r="J2" t="s">
-        <v>741</v>
+      <c r="E2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>425</v>
+        <v>699</v>
       </c>
       <c r="B3" t="s">
         <v>423</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>163</v>
       </c>
       <c r="D3" t="s">
         <v>426</v>
       </c>
-      <c r="E3" t="s">
-        <v>427</v>
+      <c r="E3" s="7" t="s">
+        <v>177</v>
       </c>
       <c r="F3" t="s">
-        <v>429</v>
+        <v>701</v>
       </c>
       <c r="H3" t="s">
-        <v>431</v>
-      </c>
-      <c r="I3" s="19">
-        <v>-5</v>
-      </c>
-      <c r="J3" s="20" t="s">
-        <v>697</v>
+        <v>702</v>
+      </c>
+      <c r="I3" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>424</v>
+        <v>741</v>
       </c>
       <c r="B4" t="s">
         <v>423</v>
@@ -3947,225 +3935,221 @@
       <c r="D4" t="s">
         <v>426</v>
       </c>
-      <c r="E4" t="s">
-        <v>427</v>
+      <c r="E4" s="7" t="s">
+        <v>177</v>
       </c>
       <c r="F4" t="s">
-        <v>428</v>
+        <v>742</v>
       </c>
       <c r="H4" t="s">
-        <v>430</v>
+        <v>743</v>
       </c>
       <c r="I4">
-        <v>-10</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>698</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>447</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
         <v>423</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>163</v>
       </c>
       <c r="D5" t="s">
+        <v>426</v>
+      </c>
+      <c r="E5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="I5" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>748</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>740</v>
+      </c>
+      <c r="D6" t="s">
+        <v>426</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="F6" t="s">
+        <v>738</v>
+      </c>
+      <c r="G6" t="s">
+        <v>246</v>
+      </c>
+      <c r="H6" t="s">
+        <v>739</v>
+      </c>
+      <c r="I6" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>425</v>
+      </c>
+      <c r="B7" t="s">
+        <v>423</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>426</v>
+      </c>
+      <c r="E7" t="s">
+        <v>427</v>
+      </c>
+      <c r="F7" t="s">
+        <v>429</v>
+      </c>
+      <c r="H7" t="s">
+        <v>431</v>
+      </c>
+      <c r="I7" s="19">
+        <v>-5</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>424</v>
+      </c>
+      <c r="B8" t="s">
+        <v>423</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>426</v>
+      </c>
+      <c r="E8" t="s">
+        <v>427</v>
+      </c>
+      <c r="F8" t="s">
+        <v>428</v>
+      </c>
+      <c r="H8" t="s">
+        <v>430</v>
+      </c>
+      <c r="I8">
+        <v>-10</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>700</v>
+      </c>
+      <c r="B9" t="s">
+        <v>423</v>
+      </c>
+      <c r="C9" t="s">
+        <v>163</v>
+      </c>
+      <c r="D9" t="s">
+        <v>426</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="F9" t="s">
+        <v>703</v>
+      </c>
+      <c r="H9" t="s">
+        <v>704</v>
+      </c>
+      <c r="I9" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>433</v>
+      </c>
+      <c r="B10" t="s">
+        <v>423</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>426</v>
+      </c>
+      <c r="E10" t="s">
+        <v>390</v>
+      </c>
+      <c r="F10" t="s">
+        <v>389</v>
+      </c>
+      <c r="G10" t="s">
+        <v>388</v>
+      </c>
+      <c r="H10" t="s">
+        <v>391</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>447</v>
+      </c>
+      <c r="B11" t="s">
+        <v>423</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
         <v>248</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H11" t="s">
         <v>204</v>
       </c>
-      <c r="I5">
+      <c r="I11">
         <v>0</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J11" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="20" t="s">
-        <v>543</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>423</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>707</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>534</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>544</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>545</v>
-      </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20">
-        <v>0</v>
-      </c>
-      <c r="J6" s="20"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="20" t="s">
-        <v>540</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>423</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>707</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>534</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>541</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>542</v>
-      </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20">
-        <v>0</v>
-      </c>
-      <c r="J7" s="20"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="20" t="s">
-        <v>279</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>423</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>707</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>534</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>535</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20">
-        <v>0</v>
-      </c>
-      <c r="J8" s="20"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>423</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>707</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>534</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>536</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>537</v>
-      </c>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20">
-        <v>0</v>
-      </c>
-      <c r="J9" s="20"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="20" t="s">
-        <v>538</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>423</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>707</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>534</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>539</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>265</v>
-      </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20">
-        <v>0</v>
-      </c>
-      <c r="J10" s="20"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="20" t="s">
-        <v>574</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>423</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>707</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>575</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>576</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>577</v>
-      </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20">
-        <v>0</v>
-      </c>
-      <c r="J11" s="20"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="20" t="s">
-        <v>562</v>
+        <v>543</v>
       </c>
       <c r="B12" s="20" t="s">
         <v>423</v>
@@ -4179,11 +4163,11 @@
       <c r="E12" s="20" t="s">
         <v>534</v>
       </c>
-      <c r="F12" s="20" t="s">
-        <v>563</v>
+      <c r="F12" s="21" t="s">
+        <v>544</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>564</v>
+        <v>545</v>
       </c>
       <c r="H12" s="20"/>
       <c r="I12" s="20">
@@ -4193,7 +4177,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="20" t="s">
-        <v>578</v>
+        <v>540</v>
       </c>
       <c r="B13" s="20" t="s">
         <v>423</v>
@@ -4204,14 +4188,14 @@
       <c r="D13" s="20" t="s">
         <v>707</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>177</v>
+      <c r="E13" s="20" t="s">
+        <v>534</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>579</v>
+        <v>541</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>580</v>
+        <v>542</v>
       </c>
       <c r="H13" s="20"/>
       <c r="I13" s="20">
@@ -4221,7 +4205,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="20" t="s">
-        <v>565</v>
+        <v>279</v>
       </c>
       <c r="B14" s="20" t="s">
         <v>423</v>
@@ -4236,10 +4220,10 @@
         <v>534</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>566</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>567</v>
+        <v>535</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>284</v>
       </c>
       <c r="H14" s="20"/>
       <c r="I14" s="20">
@@ -4248,314 +4232,321 @@
       <c r="J14" s="20"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" t="s">
-        <v>465</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="A15" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>423</v>
       </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>705</v>
-      </c>
-      <c r="E15" t="s">
-        <v>466</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>467</v>
-      </c>
-      <c r="H15" t="s">
-        <v>200</v>
-      </c>
-      <c r="I15">
+      <c r="C15" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>707</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>534</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>536</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20">
         <v>0</v>
       </c>
-      <c r="J15" t="s">
-        <v>468</v>
-      </c>
+      <c r="J15" s="20"/>
     </row>
     <row r="16" spans="1:10" s="14" customFormat="1">
-      <c r="A16" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="A16" s="20" t="s">
+        <v>538</v>
+      </c>
+      <c r="B16" s="20" t="s">
         <v>423</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>705</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>641</v>
-      </c>
-      <c r="I16">
+      <c r="C16" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>707</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>534</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>539</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>265</v>
+      </c>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20">
         <v>0</v>
       </c>
-      <c r="J16"/>
+      <c r="J16" s="20"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="14" t="s">
-        <v>642</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="A17" s="20" t="s">
+        <v>574</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>423</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>705</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>644</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>643</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>645</v>
-      </c>
-      <c r="I17">
+      <c r="C17" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>707</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>575</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>576</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>577</v>
+      </c>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20">
         <v>0</v>
       </c>
+      <c r="J17" s="20"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" t="s">
-        <v>281</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="A18" s="20" t="s">
+        <v>562</v>
+      </c>
+      <c r="B18" s="20" t="s">
         <v>423</v>
       </c>
-      <c r="C18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>705</v>
-      </c>
-      <c r="E18" s="7" t="s">
+      <c r="C18" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>707</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>534</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>563</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>564</v>
+      </c>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20">
+        <v>0</v>
+      </c>
+      <c r="J18" s="20"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="20" t="s">
+        <v>578</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>423</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>707</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="H18" t="s">
-        <v>223</v>
-      </c>
-      <c r="I18">
+      <c r="F19" s="20" t="s">
+        <v>579</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>580</v>
+      </c>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" t="s">
-        <v>432</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="J19" s="20"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="20" t="s">
+        <v>565</v>
+      </c>
+      <c r="B20" s="20" t="s">
         <v>423</v>
       </c>
-      <c r="C19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>705</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="H19" t="s">
-        <v>232</v>
-      </c>
-      <c r="I19">
+      <c r="C20" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>707</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>534</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>566</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>567</v>
+      </c>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="3" t="s">
-        <v>441</v>
-      </c>
-      <c r="B20" t="s">
-        <v>423</v>
-      </c>
-      <c r="C20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>705</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="H20" t="s">
-        <v>443</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20" t="s">
-        <v>444</v>
-      </c>
+      <c r="J20" s="20"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>164</v>
+        <v>465</v>
       </c>
       <c r="B21" t="s">
         <v>423</v>
       </c>
       <c r="C21" t="s">
-        <v>163</v>
-      </c>
-      <c r="D21" t="s">
-        <v>426</v>
+        <v>26</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>705</v>
       </c>
       <c r="E21" t="s">
-        <v>166</v>
+        <v>466</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="I21" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+        <v>467</v>
+      </c>
+      <c r="H21" t="s">
+        <v>200</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" t="s">
-        <v>699</v>
+      <c r="A22" s="14" t="s">
+        <v>189</v>
       </c>
       <c r="B22" t="s">
         <v>423</v>
       </c>
-      <c r="C22" t="s">
-        <v>163</v>
-      </c>
-      <c r="D22" t="s">
-        <v>426</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="F22" t="s">
-        <v>701</v>
-      </c>
-      <c r="H22" t="s">
-        <v>702</v>
-      </c>
-      <c r="I22" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="C22" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>705</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>641</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" t="s">
-        <v>743</v>
+      <c r="A23" s="14" t="s">
+        <v>642</v>
       </c>
       <c r="B23" t="s">
         <v>423</v>
       </c>
-      <c r="C23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" t="s">
-        <v>426</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="F23" t="s">
-        <v>744</v>
-      </c>
-      <c r="H23" t="s">
-        <v>745</v>
+      <c r="C23" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>705</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>644</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>643</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>645</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>165</v>
+        <v>281</v>
       </c>
       <c r="B24" t="s">
         <v>423</v>
       </c>
       <c r="C24" t="s">
-        <v>163</v>
-      </c>
-      <c r="D24" t="s">
-        <v>426</v>
-      </c>
-      <c r="E24" t="s">
-        <v>167</v>
+        <v>26</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>705</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>177</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="I24" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+        <v>221</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H24" t="s">
+        <v>223</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>700</v>
+        <v>432</v>
       </c>
       <c r="B25" t="s">
         <v>423</v>
       </c>
       <c r="C25" t="s">
-        <v>163</v>
-      </c>
-      <c r="D25" t="s">
-        <v>426</v>
+        <v>26</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>705</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="F25" t="s">
-        <v>703</v>
+        <v>230</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>311</v>
       </c>
       <c r="H25" t="s">
-        <v>704</v>
-      </c>
-      <c r="I25" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+        <v>232</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" t="s">
-        <v>433</v>
+      <c r="A26" s="3" t="s">
+        <v>441</v>
       </c>
       <c r="B26" t="s">
         <v>423</v>
@@ -4563,23 +4554,26 @@
       <c r="C26" t="s">
         <v>26</v>
       </c>
-      <c r="D26" t="s">
-        <v>426</v>
-      </c>
-      <c r="E26" t="s">
-        <v>390</v>
-      </c>
-      <c r="F26" t="s">
-        <v>389</v>
-      </c>
-      <c r="G26" t="s">
-        <v>388</v>
+      <c r="D26" s="14" t="s">
+        <v>705</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>236</v>
       </c>
       <c r="H26" t="s">
-        <v>391</v>
+        <v>443</v>
       </c>
       <c r="I26">
         <v>0</v>
+      </c>
+      <c r="J26" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -5339,34 +5333,37 @@
       </c>
     </row>
     <row r="53" spans="1:10">
-      <c r="A53" s="20" t="s">
-        <v>516</v>
-      </c>
-      <c r="B53" s="20" t="s">
+      <c r="A53" t="s">
+        <v>735</v>
+      </c>
+      <c r="B53" t="s">
         <v>135</v>
       </c>
-      <c r="C53" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D53" s="20" t="s">
-        <v>707</v>
-      </c>
-      <c r="E53" s="20" t="s">
-        <v>517</v>
-      </c>
-      <c r="F53" s="20" t="s">
-        <v>518</v>
-      </c>
-      <c r="G53" s="20" t="s">
-        <v>296</v>
-      </c>
-      <c r="H53" s="20"/>
-      <c r="I53" s="20"/>
-      <c r="J53" s="20"/>
+      <c r="C53" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" t="s">
+        <v>426</v>
+      </c>
+      <c r="E53" t="s">
+        <v>716</v>
+      </c>
+      <c r="F53" t="s">
+        <v>736</v>
+      </c>
+      <c r="G53" t="s">
+        <v>734</v>
+      </c>
+      <c r="H53" t="s">
+        <v>737</v>
+      </c>
+      <c r="I53" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="20" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="B54" s="20" t="s">
         <v>135</v>
@@ -5378,13 +5375,13 @@
         <v>707</v>
       </c>
       <c r="E54" s="20" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="F54" s="20" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="G54" s="20" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H54" s="20"/>
       <c r="I54" s="20"/>
@@ -5392,7 +5389,7 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="20" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B55" s="20" t="s">
         <v>135</v>
@@ -5404,13 +5401,13 @@
         <v>707</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="F55" s="20" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="G55" s="20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H55" s="20"/>
       <c r="I55" s="20"/>
@@ -5418,7 +5415,7 @@
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="20" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="B56" s="20" t="s">
         <v>135</v>
@@ -5430,13 +5427,13 @@
         <v>707</v>
       </c>
       <c r="E56" s="20" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="G56" s="20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H56" s="20"/>
       <c r="I56" s="20"/>
@@ -5444,7 +5441,7 @@
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="20" t="s">
-        <v>502</v>
+        <v>525</v>
       </c>
       <c r="B57" s="20" t="s">
         <v>135</v>
@@ -5456,13 +5453,13 @@
         <v>707</v>
       </c>
       <c r="E57" s="20" t="s">
-        <v>503</v>
+        <v>526</v>
       </c>
       <c r="F57" s="20" t="s">
-        <v>504</v>
+        <v>527</v>
       </c>
       <c r="G57" s="20" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="H57" s="20"/>
       <c r="I57" s="20"/>
@@ -5470,7 +5467,7 @@
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="20" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="B58" s="20" t="s">
         <v>135</v>
@@ -5482,13 +5479,13 @@
         <v>707</v>
       </c>
       <c r="E58" s="20" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="F58" s="20" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="G58" s="20" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="H58" s="20"/>
       <c r="I58" s="20"/>
@@ -5496,7 +5493,7 @@
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="20" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="B59" s="20" t="s">
         <v>135</v>
@@ -5511,10 +5508,10 @@
         <v>507</v>
       </c>
       <c r="F59" s="20" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="G59" s="20" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H59" s="20"/>
       <c r="I59" s="20"/>
@@ -5522,7 +5519,7 @@
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="20" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B60" s="20" t="s">
         <v>135</v>
@@ -5537,10 +5534,10 @@
         <v>507</v>
       </c>
       <c r="F60" s="20" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G60" s="20" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H60" s="20"/>
       <c r="I60" s="20"/>
@@ -5548,7 +5545,7 @@
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="20" t="s">
-        <v>266</v>
+        <v>511</v>
       </c>
       <c r="B61" s="20" t="s">
         <v>135</v>
@@ -5560,13 +5557,13 @@
         <v>707</v>
       </c>
       <c r="E61" s="20" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="F61" s="20" t="s">
-        <v>505</v>
+        <v>512</v>
       </c>
       <c r="G61" s="20" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="H61" s="20"/>
       <c r="I61" s="20"/>
@@ -5574,7 +5571,7 @@
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="20" t="s">
-        <v>528</v>
+        <v>266</v>
       </c>
       <c r="B62" s="20" t="s">
         <v>135</v>
@@ -5586,13 +5583,13 @@
         <v>707</v>
       </c>
       <c r="E62" s="20" t="s">
-        <v>517</v>
+        <v>503</v>
       </c>
       <c r="F62" s="20" t="s">
-        <v>529</v>
+        <v>505</v>
       </c>
       <c r="G62" s="20" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="H62" s="20"/>
       <c r="I62" s="20"/>
@@ -5600,7 +5597,7 @@
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="20" t="s">
-        <v>513</v>
+        <v>528</v>
       </c>
       <c r="B63" s="20" t="s">
         <v>135</v>
@@ -5612,13 +5609,13 @@
         <v>707</v>
       </c>
       <c r="E63" s="20" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="F63" s="20" t="s">
-        <v>515</v>
+        <v>529</v>
       </c>
       <c r="G63" s="20" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="H63" s="20"/>
       <c r="I63" s="20"/>
@@ -5626,7 +5623,7 @@
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="20" t="s">
-        <v>530</v>
+        <v>513</v>
       </c>
       <c r="B64" s="20" t="s">
         <v>135</v>
@@ -5638,51 +5635,47 @@
         <v>707</v>
       </c>
       <c r="E64" s="20" t="s">
-        <v>531</v>
+        <v>514</v>
       </c>
       <c r="F64" s="20" t="s">
-        <v>532</v>
+        <v>515</v>
       </c>
       <c r="G64" s="20" t="s">
-        <v>533</v>
+        <v>295</v>
       </c>
       <c r="H64" s="20"/>
       <c r="I64" s="20"/>
       <c r="J64" s="20"/>
     </row>
     <row r="65" spans="1:10">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="20" t="s">
+        <v>530</v>
+      </c>
+      <c r="B65" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="C65" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D65" s="20" t="s">
+        <v>707</v>
+      </c>
+      <c r="E65" s="20" t="s">
+        <v>531</v>
+      </c>
+      <c r="F65" s="20" t="s">
+        <v>532</v>
+      </c>
+      <c r="G65" s="20" t="s">
+        <v>533</v>
+      </c>
+      <c r="H65" s="20"/>
+      <c r="I65" s="20"/>
+      <c r="J65" s="20"/>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="3" t="s">
         <v>371</v>
-      </c>
-      <c r="B65" t="s">
-        <v>135</v>
-      </c>
-      <c r="C65" t="s">
-        <v>26</v>
-      </c>
-      <c r="D65" t="s">
-        <v>708</v>
-      </c>
-      <c r="E65" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="H65" t="s">
-        <v>261</v>
-      </c>
-      <c r="I65" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
-      <c r="A66" t="s">
-        <v>251</v>
       </c>
       <c r="B66" t="s">
         <v>135</v>
@@ -5694,16 +5687,16 @@
         <v>708</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>249</v>
+        <v>177</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="H66" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="I66" t="e">
         <f>NA()</f>
@@ -5712,7 +5705,7 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67" t="s">
-        <v>493</v>
+        <v>251</v>
       </c>
       <c r="B67" t="s">
         <v>135</v>
@@ -5723,17 +5716,17 @@
       <c r="D67" t="s">
         <v>708</v>
       </c>
-      <c r="E67" s="12" t="s">
-        <v>268</v>
+      <c r="E67" s="7" t="s">
+        <v>249</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="G67" s="11" t="s">
-        <v>303</v>
+        <v>250</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>302</v>
       </c>
       <c r="H67" t="s">
-        <v>501</v>
+        <v>252</v>
       </c>
       <c r="I67" t="e">
         <f>NA()</f>
@@ -5742,7 +5735,7 @@
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>269</v>
+        <v>493</v>
       </c>
       <c r="B68" t="s">
         <v>135</v>
@@ -5757,13 +5750,13 @@
         <v>268</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H68" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="I68" t="e">
         <f>NA()</f>
@@ -5772,7 +5765,7 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B69" t="s">
         <v>135</v>
@@ -5787,13 +5780,13 @@
         <v>268</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="G69" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H69" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I69" t="e">
         <f>NA()</f>
@@ -5802,7 +5795,7 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>588</v>
+        <v>270</v>
       </c>
       <c r="B70" t="s">
         <v>135</v>
@@ -5816,14 +5809,14 @@
       <c r="E70" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F70" s="10" t="s">
-        <v>494</v>
+      <c r="F70" s="3" t="s">
+        <v>497</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="H70" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="I70" t="e">
         <f>NA()</f>
@@ -5832,7 +5825,7 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>226</v>
+        <v>588</v>
       </c>
       <c r="B71" t="s">
         <v>135</v>
@@ -5841,19 +5834,19 @@
         <v>26</v>
       </c>
       <c r="D71" t="s">
-        <v>705</v>
-      </c>
-      <c r="E71" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="G71" s="3" t="s">
-        <v>306</v>
+        <v>708</v>
+      </c>
+      <c r="E71" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="F71" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="G71" s="11" t="s">
+        <v>301</v>
       </c>
       <c r="H71" t="s">
-        <v>228</v>
+        <v>498</v>
       </c>
       <c r="I71" t="e">
         <f>NA()</f>
@@ -5862,7 +5855,7 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B72" t="s">
         <v>135</v>
@@ -5877,13 +5870,13 @@
         <v>177</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>438</v>
+        <v>306</v>
       </c>
       <c r="H72" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I72" t="e">
         <f>NA()</f>
@@ -5892,7 +5885,7 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="B73" t="s">
         <v>135</v>
@@ -5903,29 +5896,26 @@
       <c r="D73" t="s">
         <v>705</v>
       </c>
-      <c r="E73" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="F73" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="G73" s="18" t="s">
-        <v>439</v>
+      <c r="E73" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="H73" t="s">
-        <v>216</v>
+        <v>229</v>
       </c>
       <c r="I73" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="J73" t="s">
-        <v>469</v>
-      </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="B74" t="s">
         <v>135</v>
@@ -5936,29 +5926,29 @@
       <c r="D74" t="s">
         <v>705</v>
       </c>
-      <c r="E74" t="s">
-        <v>15</v>
+      <c r="E74" s="9" t="s">
+        <v>217</v>
       </c>
       <c r="F74" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="G74" s="11" t="s">
-        <v>440</v>
+        <v>213</v>
+      </c>
+      <c r="G74" s="18" t="s">
+        <v>439</v>
       </c>
       <c r="H74" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I74" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
       <c r="J74" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75" t="s">
-        <v>271</v>
+        <v>212</v>
       </c>
       <c r="B75" t="s">
         <v>135</v>
@@ -5969,20 +5959,29 @@
       <c r="D75" t="s">
         <v>705</v>
       </c>
-      <c r="E75" s="12" t="s">
-        <v>268</v>
-      </c>
-      <c r="G75" s="3" t="s">
-        <v>307</v>
+      <c r="E75" t="s">
+        <v>15</v>
+      </c>
+      <c r="F75" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="G75" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="H75" t="s">
+        <v>215</v>
       </c>
       <c r="I75" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
+      <c r="J75" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="76" spans="1:10">
       <c r="A76" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B76" t="s">
         <v>135</v>
@@ -5997,19 +5996,16 @@
         <v>268</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I76" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="J76" t="s">
-        <v>471</v>
-      </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B77" t="s">
         <v>135</v>
@@ -6020,26 +6016,23 @@
       <c r="D77" t="s">
         <v>705</v>
       </c>
-      <c r="E77" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>219</v>
+      <c r="E77" s="12" t="s">
+        <v>268</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>434</v>
-      </c>
-      <c r="H77" s="3" t="s">
-        <v>219</v>
+        <v>308</v>
       </c>
       <c r="I77" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
+      <c r="J77" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" t="s">
-        <v>241</v>
+        <v>273</v>
       </c>
       <c r="B78" t="s">
         <v>135</v>
@@ -6051,16 +6044,16 @@
         <v>705</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>242</v>
+        <v>220</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="H78" t="s">
-        <v>243</v>
+        <v>434</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="I78" t="e">
         <f>NA()</f>
@@ -6069,7 +6062,7 @@
     </row>
     <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>208</v>
+        <v>241</v>
       </c>
       <c r="B79" t="s">
         <v>135</v>
@@ -6081,16 +6074,16 @@
         <v>705</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>206</v>
+        <v>242</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>205</v>
+        <v>239</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>309</v>
+        <v>240</v>
       </c>
       <c r="H79" t="s">
-        <v>210</v>
+        <v>243</v>
       </c>
       <c r="I79" t="e">
         <f>NA()</f>
@@ -6099,7 +6092,7 @@
     </row>
     <row r="80" spans="1:10">
       <c r="A80" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B80" t="s">
         <v>135</v>
@@ -6114,13 +6107,13 @@
         <v>206</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H80" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I80" t="e">
         <f>NA()</f>
@@ -6129,7 +6122,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>735</v>
+        <v>209</v>
       </c>
       <c r="B81" t="s">
         <v>135</v>
@@ -6138,21 +6131,22 @@
         <v>26</v>
       </c>
       <c r="D81" t="s">
-        <v>426</v>
-      </c>
-      <c r="E81" t="s">
-        <v>716</v>
-      </c>
-      <c r="F81" t="s">
-        <v>736</v>
-      </c>
-      <c r="G81" t="s">
-        <v>734</v>
+        <v>705</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>310</v>
       </c>
       <c r="H81" t="s">
-        <v>737</v>
+        <v>211</v>
       </c>
       <c r="I81" t="e">
+        <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -6717,7 +6711,7 @@
     </row>
     <row r="101" spans="1:10">
       <c r="A101" t="s">
-        <v>244</v>
+        <v>646</v>
       </c>
       <c r="B101" t="s">
         <v>41</v>
@@ -6726,57 +6720,57 @@
         <v>26</v>
       </c>
       <c r="D101" t="s">
+        <v>426</v>
+      </c>
+      <c r="E101" t="s">
+        <v>112</v>
+      </c>
+      <c r="F101" t="s">
+        <v>648</v>
+      </c>
+      <c r="G101" s="22" t="s">
+        <v>647</v>
+      </c>
+      <c r="H101" t="s">
+        <v>648</v>
+      </c>
+      <c r="I101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102" t="s">
+        <v>244</v>
+      </c>
+      <c r="B102" t="s">
+        <v>41</v>
+      </c>
+      <c r="C102" t="s">
+        <v>26</v>
+      </c>
+      <c r="D102" t="s">
         <v>32</v>
       </c>
-      <c r="E101" s="7" t="s">
+      <c r="E102" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="F101" s="3" t="s">
+      <c r="F102" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="G101" s="3" t="s">
+      <c r="G102" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="H101" t="s">
+      <c r="H102" t="s">
         <v>247</v>
       </c>
-      <c r="I101" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10">
-      <c r="A102" s="20" t="s">
-        <v>571</v>
-      </c>
-      <c r="B102" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C102" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D102" s="20" t="s">
-        <v>707</v>
-      </c>
-      <c r="E102" s="20" t="s">
-        <v>546</v>
-      </c>
-      <c r="F102" s="20" t="s">
-        <v>572</v>
-      </c>
-      <c r="G102" s="20" t="s">
-        <v>573</v>
-      </c>
-      <c r="H102" s="20"/>
       <c r="I102" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="J102" s="20"/>
     </row>
     <row r="103" spans="1:10">
       <c r="A103" s="20" t="s">
-        <v>559</v>
+        <v>571</v>
       </c>
       <c r="B103" s="20" t="s">
         <v>41</v>
@@ -6788,25 +6782,24 @@
         <v>707</v>
       </c>
       <c r="E103" s="20" t="s">
-        <v>534</v>
+        <v>546</v>
       </c>
       <c r="F103" s="20" t="s">
-        <v>560</v>
+        <v>572</v>
       </c>
       <c r="G103" s="20" t="s">
-        <v>561</v>
+        <v>573</v>
       </c>
       <c r="H103" s="20"/>
-      <c r="I103" s="20">
-        <v>0</v>
-      </c>
-      <c r="J103" s="20" t="s">
-        <v>555</v>
-      </c>
+      <c r="I103" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J103" s="20"/>
     </row>
     <row r="104" spans="1:10">
       <c r="A104" s="20" t="s">
-        <v>552</v>
+        <v>559</v>
       </c>
       <c r="B104" s="20" t="s">
         <v>41</v>
@@ -6818,13 +6811,13 @@
         <v>707</v>
       </c>
       <c r="E104" s="20" t="s">
-        <v>546</v>
+        <v>534</v>
       </c>
       <c r="F104" s="20" t="s">
-        <v>553</v>
+        <v>560</v>
       </c>
       <c r="G104" s="20" t="s">
-        <v>554</v>
+        <v>561</v>
       </c>
       <c r="H104" s="20"/>
       <c r="I104" s="20">
@@ -6836,7 +6829,7 @@
     </row>
     <row r="105" spans="1:10">
       <c r="A105" s="20" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="B105" s="20" t="s">
         <v>41</v>
@@ -6851,22 +6844,22 @@
         <v>546</v>
       </c>
       <c r="F105" s="20" t="s">
-        <v>550</v>
-      </c>
-      <c r="G105" s="2" t="s">
-        <v>551</v>
+        <v>553</v>
+      </c>
+      <c r="G105" s="20" t="s">
+        <v>554</v>
       </c>
       <c r="H105" s="20"/>
       <c r="I105" s="20">
         <v>0</v>
       </c>
       <c r="J105" s="20" t="s">
-        <v>548</v>
+        <v>555</v>
       </c>
     </row>
     <row r="106" spans="1:10">
       <c r="A106" s="20" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="B106" s="20" t="s">
         <v>41</v>
@@ -6878,25 +6871,25 @@
         <v>707</v>
       </c>
       <c r="E106" s="20" t="s">
-        <v>507</v>
+        <v>546</v>
       </c>
       <c r="F106" s="20" t="s">
-        <v>581</v>
-      </c>
-      <c r="G106" s="20" t="s">
-        <v>557</v>
+        <v>550</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>551</v>
       </c>
       <c r="H106" s="20"/>
       <c r="I106" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J106" s="20" t="s">
-        <v>558</v>
+        <v>548</v>
       </c>
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="20" t="s">
-        <v>568</v>
+        <v>556</v>
       </c>
       <c r="B107" s="20" t="s">
         <v>41</v>
@@ -6908,25 +6901,25 @@
         <v>707</v>
       </c>
       <c r="E107" s="20" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="F107" s="20" t="s">
-        <v>569</v>
+        <v>581</v>
       </c>
       <c r="G107" s="20" t="s">
-        <v>570</v>
+        <v>557</v>
       </c>
       <c r="H107" s="20"/>
       <c r="I107" s="20">
         <v>1</v>
       </c>
       <c r="J107" s="20" t="s">
-        <v>582</v>
+        <v>558</v>
       </c>
     </row>
     <row r="108" spans="1:10">
       <c r="A108" s="20" t="s">
-        <v>446</v>
+        <v>568</v>
       </c>
       <c r="B108" s="20" t="s">
         <v>41</v>
@@ -6938,87 +6931,85 @@
         <v>707</v>
       </c>
       <c r="E108" s="20" t="s">
-        <v>546</v>
+        <v>503</v>
       </c>
       <c r="F108" s="20" t="s">
-        <v>547</v>
-      </c>
-      <c r="G108" s="2" t="s">
-        <v>283</v>
+        <v>569</v>
+      </c>
+      <c r="G108" s="20" t="s">
+        <v>570</v>
       </c>
       <c r="H108" s="20"/>
       <c r="I108" s="20">
+        <v>1</v>
+      </c>
+      <c r="J108" s="20" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10">
+      <c r="A109" s="20" t="s">
+        <v>446</v>
+      </c>
+      <c r="B109" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C109" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D109" s="20" t="s">
+        <v>707</v>
+      </c>
+      <c r="E109" s="20" t="s">
+        <v>546</v>
+      </c>
+      <c r="F109" s="20" t="s">
+        <v>547</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="H109" s="20"/>
+      <c r="I109" s="20">
         <v>0</v>
       </c>
-      <c r="J108" s="20" t="s">
+      <c r="J109" s="20" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
-      <c r="A109" t="s">
+    <row r="110" spans="1:10">
+      <c r="A110" t="s">
         <v>480</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B110" t="s">
         <v>41</v>
       </c>
-      <c r="C109" t="s">
-        <v>26</v>
-      </c>
-      <c r="D109" t="s">
+      <c r="C110" t="s">
+        <v>26</v>
+      </c>
+      <c r="D110" t="s">
         <v>708</v>
       </c>
-      <c r="E109" s="7" t="s">
+      <c r="E110" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="F109" s="3" t="s">
+      <c r="F110" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="G109" s="3" t="s">
+      <c r="G110" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="H109" t="s">
+      <c r="H110" t="s">
         <v>255</v>
       </c>
-      <c r="I109" t="e">
+      <c r="I110" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
-      <c r="A110" t="s">
-        <v>263</v>
-      </c>
-      <c r="B110" t="s">
-        <v>41</v>
-      </c>
-      <c r="C110" t="s">
-        <v>26</v>
-      </c>
-      <c r="D110" t="s">
-        <v>708</v>
-      </c>
-      <c r="E110" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="F110" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="G110" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="H110" t="s">
-        <v>264</v>
-      </c>
-      <c r="I110">
-        <v>0</v>
-      </c>
-      <c r="J110" t="s">
-        <v>583</v>
-      </c>
-    </row>
     <row r="111" spans="1:10">
       <c r="A111" t="s">
-        <v>481</v>
+        <v>263</v>
       </c>
       <c r="B111" t="s">
         <v>41</v>
@@ -7030,57 +7021,57 @@
         <v>708</v>
       </c>
       <c r="E111" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="G111" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="H111" t="s">
+        <v>264</v>
+      </c>
+      <c r="I111">
+        <v>0</v>
+      </c>
+      <c r="J111" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10">
+      <c r="A112" t="s">
+        <v>481</v>
+      </c>
+      <c r="B112" t="s">
+        <v>41</v>
+      </c>
+      <c r="C112" t="s">
+        <v>26</v>
+      </c>
+      <c r="D112" t="s">
+        <v>708</v>
+      </c>
+      <c r="E112" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="F111" s="3" t="s">
+      <c r="F112" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="G111" s="3" t="s">
+      <c r="G112" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="H111" t="s">
+      <c r="H112" t="s">
         <v>257</v>
       </c>
-      <c r="I111" t="e">
+      <c r="I112" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
-      <c r="A112" t="s">
-        <v>201</v>
-      </c>
-      <c r="B112" t="s">
-        <v>41</v>
-      </c>
-      <c r="C112" t="s">
-        <v>26</v>
-      </c>
-      <c r="D112" t="s">
-        <v>705</v>
-      </c>
-      <c r="E112" t="s">
-        <v>195</v>
-      </c>
-      <c r="F112" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="G112" t="s">
-        <v>192</v>
-      </c>
-      <c r="H112" t="s">
-        <v>200</v>
-      </c>
-      <c r="I112">
-        <v>0</v>
-      </c>
-      <c r="J112" t="s">
-        <v>584</v>
-      </c>
-    </row>
     <row r="113" spans="1:10">
       <c r="A113" t="s">
-        <v>472</v>
+        <v>201</v>
       </c>
       <c r="B113" t="s">
         <v>41</v>
@@ -7092,25 +7083,27 @@
         <v>705</v>
       </c>
       <c r="E113" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>474</v>
+        <v>198</v>
       </c>
       <c r="G113" t="s">
-        <v>476</v>
+        <v>192</v>
       </c>
       <c r="H113" t="s">
-        <v>478</v>
-      </c>
-      <c r="I113" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+        <v>200</v>
+      </c>
+      <c r="I113">
+        <v>0</v>
+      </c>
+      <c r="J113" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="114" spans="1:10">
       <c r="A114" t="s">
-        <v>197</v>
+        <v>472</v>
       </c>
       <c r="B114" t="s">
         <v>41</v>
@@ -7122,16 +7115,16 @@
         <v>705</v>
       </c>
       <c r="E114" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>196</v>
+        <v>474</v>
       </c>
       <c r="G114" t="s">
-        <v>191</v>
+        <v>476</v>
       </c>
       <c r="H114" t="s">
-        <v>199</v>
+        <v>478</v>
       </c>
       <c r="I114" t="e">
         <f>NA()</f>
@@ -7140,7 +7133,7 @@
     </row>
     <row r="115" spans="1:10">
       <c r="A115" t="s">
-        <v>473</v>
+        <v>197</v>
       </c>
       <c r="B115" t="s">
         <v>41</v>
@@ -7152,16 +7145,16 @@
         <v>705</v>
       </c>
       <c r="E115" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>475</v>
+        <v>196</v>
       </c>
       <c r="G115" t="s">
-        <v>477</v>
+        <v>191</v>
       </c>
       <c r="H115" t="s">
-        <v>479</v>
+        <v>199</v>
       </c>
       <c r="I115" t="e">
         <f>NA()</f>
@@ -7170,7 +7163,7 @@
     </row>
     <row r="116" spans="1:10">
       <c r="A116" t="s">
-        <v>646</v>
+        <v>473</v>
       </c>
       <c r="B116" t="s">
         <v>41</v>
@@ -7179,22 +7172,23 @@
         <v>26</v>
       </c>
       <c r="D116" t="s">
-        <v>426</v>
+        <v>705</v>
       </c>
       <c r="E116" t="s">
-        <v>112</v>
-      </c>
-      <c r="F116" t="s">
-        <v>648</v>
-      </c>
-      <c r="G116" s="22" t="s">
-        <v>647</v>
+        <v>193</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="G116" t="s">
+        <v>477</v>
       </c>
       <c r="H116" t="s">
-        <v>648</v>
-      </c>
-      <c r="I116">
-        <v>0</v>
+        <v>479</v>
+      </c>
+      <c r="I116" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="117" spans="1:10">
@@ -7627,7 +7621,7 @@
     </row>
     <row r="131" spans="1:10">
       <c r="A131" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="B131" t="s">
         <v>41</v>
@@ -7642,13 +7636,13 @@
         <v>160</v>
       </c>
       <c r="F131" s="2" t="s">
+        <v>745</v>
+      </c>
+      <c r="G131" t="s">
+        <v>746</v>
+      </c>
+      <c r="H131" t="s">
         <v>747</v>
-      </c>
-      <c r="G131" t="s">
-        <v>748</v>
-      </c>
-      <c r="H131" t="s">
-        <v>749</v>
       </c>
       <c r="I131" t="e">
         <f>NA()</f>
@@ -8232,10 +8226,10 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J152">
-    <sortCondition descending="1" ref="B2:B152"/>
-    <sortCondition ref="D2:D152"/>
-    <sortCondition ref="A2:A152"/>
+  <sortState ref="A2:J153">
+    <sortCondition descending="1" ref="B2:B153"/>
+    <sortCondition ref="D2:D153"/>
+    <sortCondition ref="A2:A153"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
update reading files from platform
</commit_message>
<xml_diff>
--- a/allvariables.xlsx
+++ b/allvariables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="560" windowWidth="24480" windowHeight="12100" tabRatio="652" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="21800" yWindow="6780" windowWidth="24480" windowHeight="12100" tabRatio="652" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="nomenclature" sheetId="5" r:id="rId1"/>
@@ -1969,9 +1969,6 @@
     <t>pOrganicN</t>
   </si>
   <si>
-    <t>PFractionMineralizableN</t>
-  </si>
-  <si>
     <t>pStones</t>
   </si>
   <si>
@@ -2342,6 +2339,9 @@
   </si>
   <si>
     <t>cCycleEndType</t>
+  </si>
+  <si>
+    <t>pFractionMineralizableN</t>
   </si>
 </sst>
 </file>
@@ -2457,8 +2457,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="481">
+  <cellStyleXfs count="489">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2976,7 +2984,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="481">
+  <cellStyles count="489">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -3217,6 +3225,10 @@
     <cellStyle name="Lien hypertexte" xfId="475" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="477" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="479" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="481" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="483" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="485" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="487" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -3457,6 +3469,10 @@
     <cellStyle name="Lien hypertexte visité" xfId="476" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="478" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="480" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="482" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="484" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="486" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="488" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3823,8 +3839,8 @@
   <sheetPr codeName="Feuil2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B141" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
@@ -3897,7 +3913,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B3" t="s">
         <v>423</v>
@@ -3912,10 +3928,10 @@
         <v>177</v>
       </c>
       <c r="F3" t="s">
+        <v>700</v>
+      </c>
+      <c r="H3" t="s">
         <v>701</v>
-      </c>
-      <c r="H3" t="s">
-        <v>702</v>
       </c>
       <c r="I3" t="e">
         <f>NA()</f>
@@ -3924,7 +3940,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B4" t="s">
         <v>423</v>
@@ -3939,10 +3955,10 @@
         <v>177</v>
       </c>
       <c r="F4" t="s">
+        <v>741</v>
+      </c>
+      <c r="H4" t="s">
         <v>742</v>
-      </c>
-      <c r="H4" t="s">
-        <v>743</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -3974,13 +3990,13 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B6" t="s">
         <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D6" t="s">
         <v>426</v>
@@ -3989,13 +4005,13 @@
         <v>177</v>
       </c>
       <c r="F6" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="G6" t="s">
         <v>246</v>
       </c>
       <c r="H6" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="I6" t="e">
         <v>#N/A</v>
@@ -4027,7 +4043,7 @@
         <v>-5</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -4056,12 +4072,12 @@
         <v>-10</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B9" t="s">
         <v>423</v>
@@ -4076,10 +4092,10 @@
         <v>177</v>
       </c>
       <c r="F9" t="s">
+        <v>702</v>
+      </c>
+      <c r="H9" t="s">
         <v>703</v>
-      </c>
-      <c r="H9" t="s">
-        <v>704</v>
       </c>
       <c r="I9" t="e">
         <f>NA()</f>
@@ -4158,7 +4174,7 @@
         <v>26</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>534</v>
@@ -4186,7 +4202,7 @@
         <v>26</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>534</v>
@@ -4214,7 +4230,7 @@
         <v>26</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>534</v>
@@ -4242,7 +4258,7 @@
         <v>26</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E15" s="20" t="s">
         <v>534</v>
@@ -4270,7 +4286,7 @@
         <v>26</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>534</v>
@@ -4298,7 +4314,7 @@
         <v>26</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>575</v>
@@ -4326,7 +4342,7 @@
         <v>26</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>534</v>
@@ -4354,7 +4370,7 @@
         <v>26</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>177</v>
@@ -4382,7 +4398,7 @@
         <v>26</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E20" s="20" t="s">
         <v>534</v>
@@ -4410,7 +4426,7 @@
         <v>26</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E21" t="s">
         <v>466</v>
@@ -4439,7 +4455,7 @@
         <v>26</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>193</v>
@@ -4451,7 +4467,7 @@
         <v>190</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -4459,7 +4475,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="14" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B23" t="s">
         <v>423</v>
@@ -4468,19 +4484,19 @@
         <v>26</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>193</v>
       </c>
       <c r="F23" s="15" t="s">
+        <v>643</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>642</v>
+      </c>
+      <c r="H23" s="14" t="s">
         <v>644</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>643</v>
-      </c>
-      <c r="H23" s="14" t="s">
-        <v>645</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -4497,7 +4513,7 @@
         <v>26</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>177</v>
@@ -4526,7 +4542,7 @@
         <v>26</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>230</v>
@@ -4555,7 +4571,7 @@
         <v>26</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>237</v>
@@ -4587,7 +4603,7 @@
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E27" t="s">
         <v>97</v>
@@ -4616,7 +4632,7 @@
         <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E28" t="s">
         <v>97</v>
@@ -4645,7 +4661,7 @@
         <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E29" t="s">
         <v>97</v>
@@ -4678,7 +4694,7 @@
         <v>163</v>
       </c>
       <c r="D30" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E30" t="s">
         <v>161</v>
@@ -4705,7 +4721,7 @@
         <v>26</v>
       </c>
       <c r="D31" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>177</v>
@@ -4731,7 +4747,7 @@
         <v>26</v>
       </c>
       <c r="D32" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E32" t="s">
         <v>118</v>
@@ -4760,7 +4776,7 @@
         <v>26</v>
       </c>
       <c r="D33" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E33" t="s">
         <v>118</v>
@@ -4789,7 +4805,7 @@
         <v>26</v>
       </c>
       <c r="D34" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="E34" t="s">
         <v>112</v>
@@ -4809,7 +4825,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B35" t="s">
         <v>423</v>
@@ -4818,19 +4834,19 @@
         <v>26</v>
       </c>
       <c r="D35" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E35" t="s">
+        <v>715</v>
+      </c>
+      <c r="F35" t="s">
         <v>716</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>717</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>718</v>
-      </c>
-      <c r="H35" t="s">
-        <v>719</v>
       </c>
       <c r="I35">
         <v>0</v>
@@ -4838,7 +4854,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B36" s="13" t="s">
         <v>423</v>
@@ -4847,19 +4863,19 @@
         <v>26</v>
       </c>
       <c r="D36" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E36" t="s">
         <v>177</v>
       </c>
       <c r="F36" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G36" t="s">
         <v>397</v>
       </c>
       <c r="H36" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="I36">
         <v>0</v>
@@ -4876,7 +4892,7 @@
         <v>26</v>
       </c>
       <c r="D37" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E37" t="s">
         <v>322</v>
@@ -4905,7 +4921,7 @@
         <v>26</v>
       </c>
       <c r="D38" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E38" t="s">
         <v>322</v>
@@ -4934,7 +4950,7 @@
         <v>26</v>
       </c>
       <c r="D39" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E39" t="s">
         <v>322</v>
@@ -4963,7 +4979,7 @@
         <v>26</v>
       </c>
       <c r="D40" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E40" t="s">
         <v>322</v>
@@ -4992,7 +5008,7 @@
         <v>26</v>
       </c>
       <c r="D41" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E41" t="s">
         <v>322</v>
@@ -5021,7 +5037,7 @@
         <v>26</v>
       </c>
       <c r="D42" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E42" t="s">
         <v>322</v>
@@ -5050,7 +5066,7 @@
         <v>26</v>
       </c>
       <c r="D43" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E43" t="s">
         <v>322</v>
@@ -5079,7 +5095,7 @@
         <v>26</v>
       </c>
       <c r="D44" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E44" t="s">
         <v>322</v>
@@ -5108,7 +5124,7 @@
         <v>26</v>
       </c>
       <c r="D45" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E45" t="s">
         <v>322</v>
@@ -5137,7 +5153,7 @@
         <v>26</v>
       </c>
       <c r="D46" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E46" t="s">
         <v>322</v>
@@ -5166,7 +5182,7 @@
         <v>26</v>
       </c>
       <c r="D47" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E47" t="s">
         <v>104</v>
@@ -5223,7 +5239,7 @@
         <v>26</v>
       </c>
       <c r="D49" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E49" t="s">
         <v>14</v>
@@ -5253,7 +5269,7 @@
         <v>26</v>
       </c>
       <c r="D50" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E50" t="s">
         <v>16</v>
@@ -5283,7 +5299,7 @@
         <v>26</v>
       </c>
       <c r="D51" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E51" t="s">
         <v>15</v>
@@ -5313,7 +5329,7 @@
         <v>26</v>
       </c>
       <c r="D52" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E52" t="s">
         <v>15</v>
@@ -5334,7 +5350,7 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B53" t="s">
         <v>135</v>
@@ -5346,16 +5362,16 @@
         <v>426</v>
       </c>
       <c r="E53" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="F53" t="s">
+        <v>735</v>
+      </c>
+      <c r="G53" t="s">
+        <v>733</v>
+      </c>
+      <c r="H53" t="s">
         <v>736</v>
-      </c>
-      <c r="G53" t="s">
-        <v>734</v>
-      </c>
-      <c r="H53" t="s">
-        <v>737</v>
       </c>
       <c r="I53" t="e">
         <v>#N/A</v>
@@ -5372,7 +5388,7 @@
         <v>26</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E54" s="20" t="s">
         <v>517</v>
@@ -5398,7 +5414,7 @@
         <v>26</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E55" s="20" t="s">
         <v>520</v>
@@ -5424,7 +5440,7 @@
         <v>26</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E56" s="20" t="s">
         <v>523</v>
@@ -5450,7 +5466,7 @@
         <v>26</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E57" s="20" t="s">
         <v>526</v>
@@ -5476,7 +5492,7 @@
         <v>26</v>
       </c>
       <c r="D58" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E58" s="20" t="s">
         <v>503</v>
@@ -5502,7 +5518,7 @@
         <v>26</v>
       </c>
       <c r="D59" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E59" s="20" t="s">
         <v>507</v>
@@ -5528,7 +5544,7 @@
         <v>26</v>
       </c>
       <c r="D60" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E60" s="20" t="s">
         <v>507</v>
@@ -5554,7 +5570,7 @@
         <v>26</v>
       </c>
       <c r="D61" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E61" s="20" t="s">
         <v>507</v>
@@ -5580,7 +5596,7 @@
         <v>26</v>
       </c>
       <c r="D62" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E62" s="20" t="s">
         <v>503</v>
@@ -5606,7 +5622,7 @@
         <v>26</v>
       </c>
       <c r="D63" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E63" s="20" t="s">
         <v>517</v>
@@ -5632,7 +5648,7 @@
         <v>26</v>
       </c>
       <c r="D64" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E64" s="20" t="s">
         <v>514</v>
@@ -5658,7 +5674,7 @@
         <v>26</v>
       </c>
       <c r="D65" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E65" s="20" t="s">
         <v>531</v>
@@ -5684,7 +5700,7 @@
         <v>26</v>
       </c>
       <c r="D66" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E66" s="7" t="s">
         <v>177</v>
@@ -5714,7 +5730,7 @@
         <v>26</v>
       </c>
       <c r="D67" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E67" s="7" t="s">
         <v>249</v>
@@ -5744,7 +5760,7 @@
         <v>26</v>
       </c>
       <c r="D68" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E68" s="12" t="s">
         <v>268</v>
@@ -5774,7 +5790,7 @@
         <v>26</v>
       </c>
       <c r="D69" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E69" s="12" t="s">
         <v>268</v>
@@ -5804,7 +5820,7 @@
         <v>26</v>
       </c>
       <c r="D70" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E70" s="12" t="s">
         <v>268</v>
@@ -5834,7 +5850,7 @@
         <v>26</v>
       </c>
       <c r="D71" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E71" s="12" t="s">
         <v>268</v>
@@ -5864,7 +5880,7 @@
         <v>26</v>
       </c>
       <c r="D72" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E72" s="7" t="s">
         <v>177</v>
@@ -5894,7 +5910,7 @@
         <v>26</v>
       </c>
       <c r="D73" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E73" s="7" t="s">
         <v>177</v>
@@ -5924,7 +5940,7 @@
         <v>26</v>
       </c>
       <c r="D74" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E74" s="9" t="s">
         <v>217</v>
@@ -5957,7 +5973,7 @@
         <v>26</v>
       </c>
       <c r="D75" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E75" t="s">
         <v>15</v>
@@ -5990,7 +6006,7 @@
         <v>26</v>
       </c>
       <c r="D76" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E76" s="12" t="s">
         <v>268</v>
@@ -6014,7 +6030,7 @@
         <v>26</v>
       </c>
       <c r="D77" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E77" s="12" t="s">
         <v>268</v>
@@ -6041,7 +6057,7 @@
         <v>26</v>
       </c>
       <c r="D78" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E78" s="7" t="s">
         <v>220</v>
@@ -6071,7 +6087,7 @@
         <v>26</v>
       </c>
       <c r="D79" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E79" s="7" t="s">
         <v>242</v>
@@ -6101,7 +6117,7 @@
         <v>26</v>
       </c>
       <c r="D80" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E80" s="7" t="s">
         <v>206</v>
@@ -6131,7 +6147,7 @@
         <v>26</v>
       </c>
       <c r="D81" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E81" s="7" t="s">
         <v>206</v>
@@ -6161,7 +6177,7 @@
         <v>26</v>
       </c>
       <c r="D82" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E82" t="s">
         <v>176</v>
@@ -6191,7 +6207,7 @@
         <v>163</v>
       </c>
       <c r="D83" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F83" t="s">
         <v>449</v>
@@ -6215,7 +6231,7 @@
         <v>26</v>
       </c>
       <c r="D84" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E84" t="s">
         <v>177</v>
@@ -6245,7 +6261,7 @@
         <v>26</v>
       </c>
       <c r="D85" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E85" t="s">
         <v>15</v>
@@ -6275,7 +6291,7 @@
         <v>26</v>
       </c>
       <c r="D86" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E86" t="s">
         <v>15</v>
@@ -6305,7 +6321,7 @@
         <v>26</v>
       </c>
       <c r="D87" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E87" t="s">
         <v>15</v>
@@ -6335,7 +6351,7 @@
         <v>26</v>
       </c>
       <c r="D88" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E88" t="s">
         <v>15</v>
@@ -6365,7 +6381,7 @@
         <v>26</v>
       </c>
       <c r="D89" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E89" t="s">
         <v>15</v>
@@ -6395,7 +6411,7 @@
         <v>26</v>
       </c>
       <c r="D90" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E90" t="s">
         <v>15</v>
@@ -6425,7 +6441,7 @@
         <v>26</v>
       </c>
       <c r="D91" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E91" t="s">
         <v>15</v>
@@ -6455,7 +6471,7 @@
         <v>26</v>
       </c>
       <c r="D92" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E92" t="s">
         <v>15</v>
@@ -6485,7 +6501,7 @@
         <v>26</v>
       </c>
       <c r="D93" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E93" s="4"/>
       <c r="F93" s="5" t="s">
@@ -6513,7 +6529,7 @@
         <v>26</v>
       </c>
       <c r="D94" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F94" s="3" t="s">
         <v>139</v>
@@ -6540,7 +6556,7 @@
         <v>26</v>
       </c>
       <c r="D95" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="E95" t="s">
         <v>112</v>
@@ -6570,7 +6586,7 @@
         <v>26</v>
       </c>
       <c r="D96" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="E96" s="7" t="s">
         <v>351</v>
@@ -6591,7 +6607,7 @@
     </row>
     <row r="97" spans="1:10">
       <c r="A97" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B97" t="s">
         <v>135</v>
@@ -6600,19 +6616,19 @@
         <v>26</v>
       </c>
       <c r="D97" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E97" s="7" t="s">
         <v>177</v>
       </c>
       <c r="F97" t="s">
+        <v>668</v>
+      </c>
+      <c r="G97" t="s">
+        <v>652</v>
+      </c>
+      <c r="H97" t="s">
         <v>669</v>
-      </c>
-      <c r="G97" t="s">
-        <v>653</v>
-      </c>
-      <c r="H97" t="s">
-        <v>670</v>
       </c>
       <c r="I97" t="e">
         <f>NA()</f>
@@ -6621,7 +6637,7 @@
     </row>
     <row r="98" spans="1:10">
       <c r="A98" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B98" t="s">
         <v>135</v>
@@ -6630,19 +6646,19 @@
         <v>26</v>
       </c>
       <c r="D98" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E98" s="7" t="s">
         <v>177</v>
       </c>
       <c r="F98" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G98" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="H98" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="I98" t="e">
         <f>NA()</f>
@@ -6651,7 +6667,7 @@
     </row>
     <row r="99" spans="1:10">
       <c r="A99" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B99" t="s">
         <v>135</v>
@@ -6660,19 +6676,19 @@
         <v>26</v>
       </c>
       <c r="D99" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E99" s="7" t="s">
         <v>177</v>
       </c>
       <c r="F99" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="G99" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="H99" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="I99" t="e">
         <f>NA()</f>
@@ -6690,7 +6706,7 @@
         <v>26</v>
       </c>
       <c r="D100" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E100" t="s">
         <v>177</v>
@@ -6711,7 +6727,7 @@
     </row>
     <row r="101" spans="1:10">
       <c r="A101" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B101" t="s">
         <v>41</v>
@@ -6726,13 +6742,13 @@
         <v>112</v>
       </c>
       <c r="F101" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G101" s="22" t="s">
+        <v>646</v>
+      </c>
+      <c r="H101" t="s">
         <v>647</v>
-      </c>
-      <c r="H101" t="s">
-        <v>648</v>
       </c>
       <c r="I101">
         <v>0</v>
@@ -6779,7 +6795,7 @@
         <v>26</v>
       </c>
       <c r="D103" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E103" s="20" t="s">
         <v>546</v>
@@ -6808,7 +6824,7 @@
         <v>26</v>
       </c>
       <c r="D104" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E104" s="20" t="s">
         <v>534</v>
@@ -6838,7 +6854,7 @@
         <v>26</v>
       </c>
       <c r="D105" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E105" s="20" t="s">
         <v>546</v>
@@ -6868,7 +6884,7 @@
         <v>26</v>
       </c>
       <c r="D106" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E106" s="20" t="s">
         <v>546</v>
@@ -6898,7 +6914,7 @@
         <v>26</v>
       </c>
       <c r="D107" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E107" s="20" t="s">
         <v>507</v>
@@ -6928,7 +6944,7 @@
         <v>26</v>
       </c>
       <c r="D108" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E108" s="20" t="s">
         <v>503</v>
@@ -6958,7 +6974,7 @@
         <v>26</v>
       </c>
       <c r="D109" s="20" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E109" s="20" t="s">
         <v>546</v>
@@ -6988,7 +7004,7 @@
         <v>26</v>
       </c>
       <c r="D110" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E110" s="7" t="s">
         <v>253</v>
@@ -7018,7 +7034,7 @@
         <v>26</v>
       </c>
       <c r="D111" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E111" s="7" t="s">
         <v>238</v>
@@ -7050,7 +7066,7 @@
         <v>26</v>
       </c>
       <c r="D112" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E112" s="7" t="s">
         <v>249</v>
@@ -7080,7 +7096,7 @@
         <v>26</v>
       </c>
       <c r="D113" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E113" t="s">
         <v>195</v>
@@ -7112,7 +7128,7 @@
         <v>26</v>
       </c>
       <c r="D114" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E114" t="s">
         <v>193</v>
@@ -7142,7 +7158,7 @@
         <v>26</v>
       </c>
       <c r="D115" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E115" t="s">
         <v>195</v>
@@ -7172,7 +7188,7 @@
         <v>26</v>
       </c>
       <c r="D116" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E116" t="s">
         <v>193</v>
@@ -7202,7 +7218,7 @@
         <v>26</v>
       </c>
       <c r="D117" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E117" t="s">
         <v>160</v>
@@ -7231,7 +7247,7 @@
         <v>26</v>
       </c>
       <c r="D118" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E118" t="s">
         <v>160</v>
@@ -7263,7 +7279,7 @@
         <v>26</v>
       </c>
       <c r="D119" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E119" t="s">
         <v>160</v>
@@ -7295,7 +7311,7 @@
         <v>26</v>
       </c>
       <c r="D120" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E120" t="s">
         <v>160</v>
@@ -7327,7 +7343,7 @@
         <v>26</v>
       </c>
       <c r="D121" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E121" t="s">
         <v>15</v>
@@ -7357,7 +7373,7 @@
         <v>26</v>
       </c>
       <c r="D122" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E122" t="s">
         <v>160</v>
@@ -7389,7 +7405,7 @@
         <v>26</v>
       </c>
       <c r="D123" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E123" t="s">
         <v>15</v>
@@ -7421,7 +7437,7 @@
         <v>26</v>
       </c>
       <c r="D124" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E124" t="s">
         <v>15</v>
@@ -7451,7 +7467,7 @@
         <v>163</v>
       </c>
       <c r="D125" s="16" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E125" s="16" t="s">
         <v>171</v>
@@ -7477,7 +7493,7 @@
         <v>26</v>
       </c>
       <c r="D126" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E126" s="4" t="s">
         <v>176</v>
@@ -7507,7 +7523,7 @@
         <v>26</v>
       </c>
       <c r="D127" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E127" t="s">
         <v>15</v>
@@ -7537,7 +7553,7 @@
         <v>26</v>
       </c>
       <c r="D128" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E128" t="s">
         <v>160</v>
@@ -7559,7 +7575,7 @@
     </row>
     <row r="129" spans="1:10">
       <c r="A129" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B129" t="s">
         <v>41</v>
@@ -7568,7 +7584,7 @@
         <v>26</v>
       </c>
       <c r="D129" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E129" s="7" t="s">
         <v>177</v>
@@ -7590,7 +7606,7 @@
     </row>
     <row r="130" spans="1:10">
       <c r="A130" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B130" t="s">
         <v>41</v>
@@ -7599,7 +7615,7 @@
         <v>26</v>
       </c>
       <c r="D130" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E130" t="s">
         <v>160</v>
@@ -7621,7 +7637,7 @@
     </row>
     <row r="131" spans="1:10">
       <c r="A131" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B131" t="s">
         <v>41</v>
@@ -7630,19 +7646,19 @@
         <v>26</v>
       </c>
       <c r="D131" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E131" t="s">
         <v>160</v>
       </c>
       <c r="F131" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="G131" t="s">
         <v>745</v>
       </c>
-      <c r="G131" t="s">
+      <c r="H131" t="s">
         <v>746</v>
-      </c>
-      <c r="H131" t="s">
-        <v>747</v>
       </c>
       <c r="I131" t="e">
         <f>NA()</f>
@@ -7652,7 +7668,7 @@
     </row>
     <row r="132" spans="1:10">
       <c r="A132" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B132" t="s">
         <v>41</v>
@@ -7661,19 +7677,19 @@
         <v>26</v>
       </c>
       <c r="D132" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E132" t="s">
         <v>112</v>
       </c>
       <c r="F132" t="s">
+        <v>672</v>
+      </c>
+      <c r="G132" t="s">
+        <v>671</v>
+      </c>
+      <c r="H132" t="s">
         <v>673</v>
-      </c>
-      <c r="G132" t="s">
-        <v>672</v>
-      </c>
-      <c r="H132" t="s">
-        <v>674</v>
       </c>
       <c r="I132" t="e">
         <f>NA()</f>
@@ -7682,7 +7698,7 @@
     </row>
     <row r="133" spans="1:10">
       <c r="A133" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B133" t="s">
         <v>41</v>
@@ -7691,19 +7707,19 @@
         <v>26</v>
       </c>
       <c r="D133" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E133" t="s">
         <v>160</v>
       </c>
       <c r="F133" t="s">
+        <v>664</v>
+      </c>
+      <c r="G133" t="s">
         <v>665</v>
       </c>
-      <c r="G133" t="s">
+      <c r="H133" t="s">
         <v>666</v>
-      </c>
-      <c r="H133" t="s">
-        <v>667</v>
       </c>
       <c r="I133" t="e">
         <f>NA()</f>
@@ -7712,7 +7728,7 @@
     </row>
     <row r="134" spans="1:10">
       <c r="A134" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B134" t="s">
         <v>41</v>
@@ -7721,19 +7737,19 @@
         <v>26</v>
       </c>
       <c r="D134" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E134" t="s">
         <v>112</v>
       </c>
       <c r="F134" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="G134" t="s">
         <v>400</v>
       </c>
       <c r="H134" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="I134" t="e">
         <f>NA()</f>
@@ -7751,7 +7767,7 @@
         <v>26</v>
       </c>
       <c r="D135" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E135" t="s">
         <v>112</v>
@@ -7775,7 +7791,7 @@
         <v>26</v>
       </c>
       <c r="D136" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E136" t="s">
         <v>112</v>
@@ -7796,7 +7812,7 @@
         <v>26</v>
       </c>
       <c r="D137" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E137" t="s">
         <v>112</v>
@@ -7817,7 +7833,7 @@
         <v>26</v>
       </c>
       <c r="D138" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E138" t="s">
         <v>112</v>
@@ -7838,7 +7854,7 @@
         <v>26</v>
       </c>
       <c r="D139" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E139" t="s">
         <v>112</v>
@@ -7859,7 +7875,7 @@
         <v>26</v>
       </c>
       <c r="D140" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E140" t="s">
         <v>112</v>
@@ -7880,7 +7896,7 @@
         <v>26</v>
       </c>
       <c r="D141" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E141" t="s">
         <v>112</v>
@@ -7901,7 +7917,7 @@
         <v>26</v>
       </c>
       <c r="D142" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E142" t="s">
         <v>112</v>
@@ -7922,7 +7938,7 @@
         <v>26</v>
       </c>
       <c r="D143" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E143" t="s">
         <v>112</v>
@@ -7943,7 +7959,7 @@
         <v>26</v>
       </c>
       <c r="D144" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E144" t="s">
         <v>112</v>
@@ -7955,7 +7971,7 @@
     </row>
     <row r="145" spans="1:10">
       <c r="A145" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B145" t="s">
         <v>41</v>
@@ -7964,19 +7980,19 @@
         <v>26</v>
       </c>
       <c r="D145" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E145" t="s">
         <v>112</v>
       </c>
       <c r="F145" t="s">
+        <v>694</v>
+      </c>
+      <c r="G145" t="s">
+        <v>693</v>
+      </c>
+      <c r="H145" t="s">
         <v>695</v>
-      </c>
-      <c r="G145" t="s">
-        <v>694</v>
-      </c>
-      <c r="H145" t="s">
-        <v>696</v>
       </c>
       <c r="I145" t="e">
         <f>NA()</f>
@@ -7985,7 +8001,7 @@
     </row>
     <row r="146" spans="1:10">
       <c r="A146" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B146" t="s">
         <v>41</v>
@@ -7994,19 +8010,19 @@
         <v>26</v>
       </c>
       <c r="D146" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E146" t="s">
         <v>112</v>
       </c>
       <c r="F146" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="G146" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H146" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="I146" t="e">
         <f>NA()</f>
@@ -8015,7 +8031,7 @@
     </row>
     <row r="147" spans="1:10">
       <c r="A147" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B147" t="s">
         <v>41</v>
@@ -8024,19 +8040,19 @@
         <v>26</v>
       </c>
       <c r="D147" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E147" t="s">
         <v>112</v>
       </c>
       <c r="F147" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="G147" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="H147" s="13" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="I147" t="e">
         <f>NA()</f>
@@ -8045,7 +8061,7 @@
     </row>
     <row r="148" spans="1:10">
       <c r="A148" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B148" t="s">
         <v>41</v>
@@ -8054,19 +8070,19 @@
         <v>26</v>
       </c>
       <c r="D148" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E148" t="s">
         <v>112</v>
       </c>
       <c r="F148" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="G148" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="H148" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="I148" t="e">
         <f>NA()</f>
@@ -8084,7 +8100,7 @@
         <v>26</v>
       </c>
       <c r="D149" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E149" t="s">
         <v>112</v>
@@ -8105,7 +8121,7 @@
     </row>
     <row r="150" spans="1:10">
       <c r="A150" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B150" t="s">
         <v>41</v>
@@ -8114,25 +8130,25 @@
         <v>26</v>
       </c>
       <c r="D150" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E150" t="s">
         <v>112</v>
       </c>
       <c r="F150" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="G150" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="H150" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="I150">
         <v>0</v>
       </c>
       <c r="J150" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="151" spans="1:10">
@@ -8146,7 +8162,7 @@
         <v>26</v>
       </c>
       <c r="D151" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E151" t="s">
         <v>16</v>
@@ -8176,7 +8192,7 @@
         <v>26</v>
       </c>
       <c r="D152" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E152" t="s">
         <v>112</v>
@@ -8206,7 +8222,7 @@
         <v>26</v>
       </c>
       <c r="D153" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E153" t="s">
         <v>112</v>
@@ -8246,8 +8262,8 @@
   <sheetPr codeName="Feuil3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8304,7 +8320,7 @@
         <v>363</v>
       </c>
       <c r="G2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="H2" t="s">
         <v>364</v>
@@ -8327,13 +8343,13 @@
         <v>346</v>
       </c>
       <c r="F3" t="s">
+        <v>719</v>
+      </c>
+      <c r="G3" t="s">
+        <v>634</v>
+      </c>
+      <c r="H3" t="s">
         <v>720</v>
-      </c>
-      <c r="G3" t="s">
-        <v>635</v>
-      </c>
-      <c r="H3" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -8356,10 +8372,10 @@
         <v>392</v>
       </c>
       <c r="G4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="H4" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -8382,10 +8398,10 @@
         <v>393</v>
       </c>
       <c r="G5" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="H5" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -8408,10 +8424,10 @@
         <v>394</v>
       </c>
       <c r="G6" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="H6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -8434,10 +8450,10 @@
         <v>395</v>
       </c>
       <c r="G7" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="H7" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -8526,13 +8542,13 @@
         <v>362</v>
       </c>
       <c r="F11" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="G11" t="s">
         <v>597</v>
       </c>
       <c r="H11" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -8555,7 +8571,7 @@
         <v>595</v>
       </c>
       <c r="H12" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -8612,7 +8628,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B15" t="s">
         <v>344</v>
@@ -8621,7 +8637,7 @@
         <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>619</v>
@@ -8630,7 +8646,7 @@
         <v>606</v>
       </c>
       <c r="H15" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -8644,7 +8660,7 @@
         <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E16" t="s">
         <v>616</v>
@@ -8656,7 +8672,7 @@
         <v>607</v>
       </c>
       <c r="H16" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -8670,7 +8686,7 @@
         <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E17" t="s">
         <v>618</v>
@@ -8682,12 +8698,12 @@
         <v>608</v>
       </c>
       <c r="H17" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>624</v>
+        <v>748</v>
       </c>
       <c r="B18" t="s">
         <v>344</v>
@@ -8696,7 +8712,7 @@
         <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F18" s="22" t="s">
         <v>621</v>
@@ -8705,12 +8721,12 @@
         <v>609</v>
       </c>
       <c r="H18" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B19" t="s">
         <v>344</v>
@@ -8719,24 +8735,24 @@
         <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E19" s="22" t="s">
         <v>617</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G19" t="s">
         <v>610</v>
       </c>
       <c r="H19" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B20" t="s">
         <v>344</v>
@@ -8745,19 +8761,19 @@
         <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E20" s="22" t="s">
         <v>617</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G20" t="s">
         <v>611</v>
       </c>
       <c r="H20" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
   </sheetData>
@@ -9437,7 +9453,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B7" t="s">
         <v>36</v>
@@ -9449,13 +9465,13 @@
         <v>426</v>
       </c>
       <c r="F7" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="G7" t="e">
         <v>#N/A</v>
       </c>
       <c r="H7" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="I7">
         <v>0.05</v>
@@ -9463,7 +9479,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B8" t="s">
         <v>36</v>
@@ -9472,16 +9488,16 @@
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="F8" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="G8" t="e">
         <v>#N/A</v>
       </c>
       <c r="H8" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="I8">
         <v>0.02</v>

</xml_diff>

<commit_message>
renaming variables (closing issue #3)
renaming cEfficientRootLength and cFTSWweightedByRoots into cAvailableWaterInRootZone and cFTSWrootZone
</commit_message>
<xml_diff>
--- a/allvariables.xlsx
+++ b/allvariables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32240" windowHeight="16200" tabRatio="652" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="5440" yWindow="3260" windowWidth="32240" windowHeight="16200" tabRatio="652" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="nomenclature" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="756">
   <si>
     <t>name</t>
   </si>
@@ -2086,12 +2086,6 @@
     <t>rUpdateStresses</t>
   </si>
   <si>
-    <t>cFTSWweightedByRoots</t>
-  </si>
-  <si>
-    <t>FTSW of the whole soil weighted by rooted length in each layer</t>
-  </si>
-  <si>
     <t>FTSWRZ</t>
   </si>
   <si>
@@ -2107,18 +2101,9 @@
     <t>coefficient pour passer du stress hydrique pour la croissance au stress hydrique pour le développement</t>
   </si>
   <si>
-    <t>cEfficientRootLength</t>
-  </si>
-  <si>
     <t>AROOT</t>
   </si>
   <si>
-    <t>root length weighted by effect of water stress on transpiration</t>
-  </si>
-  <si>
-    <t>longueur de racines pondérée par effet du stress hydrique sur la transpiration</t>
-  </si>
-  <si>
     <t>cCoefWaterstressLeafArea</t>
   </si>
   <si>
@@ -2357,6 +2342,27 @@
   </si>
   <si>
     <t>factor levels: 1 "normal", 2 "low LAI", 3 "not sowed", 4 "stopDAP", 5 "killed by flood", 6 "not yet"</t>
+  </si>
+  <si>
+    <t>cAvailableWaterInRootZone</t>
+  </si>
+  <si>
+    <t>cAvailableWaterInRootZone was cEfficientRootLength (root length weighted by effect of water stress on transpiration)</t>
+  </si>
+  <si>
+    <t>available water in root zone</t>
+  </si>
+  <si>
+    <t>eau disponible dans la zone racinée</t>
+  </si>
+  <si>
+    <t>cFTSWrootZone</t>
+  </si>
+  <si>
+    <t>cFTSWrootZone was cFTSWweightedByRoots (FTSW of the whole soil weighted by rooted length in each layer)</t>
+  </si>
+  <si>
+    <t>FTSW in the root zone</t>
   </si>
 </sst>
 </file>
@@ -2472,8 +2478,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="497">
+  <cellStyleXfs count="505">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3007,7 +3021,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="497">
+  <cellStyles count="505">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -3256,6 +3270,10 @@
     <cellStyle name="Lien hypertexte" xfId="491" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="493" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="495" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="497" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="499" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="501" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="503" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -3504,6 +3522,10 @@
     <cellStyle name="Lien hypertexte visité" xfId="492" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="494" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="496" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="498" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="500" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="502" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="504" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3871,10 +3893,10 @@
   <dimension ref="A1:J154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B114" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomRight" activeCell="J135" sqref="J135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3944,7 +3966,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="B3" t="s">
         <v>423</v>
@@ -3959,10 +3981,10 @@
         <v>177</v>
       </c>
       <c r="F3" t="s">
-        <v>700</v>
+        <v>695</v>
       </c>
       <c r="H3" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="I3" t="e">
         <f>NA()</f>
@@ -3971,7 +3993,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="B4" t="s">
         <v>423</v>
@@ -3986,10 +4008,10 @@
         <v>177</v>
       </c>
       <c r="F4" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="H4" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -4021,13 +4043,13 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>747</v>
+        <v>742</v>
       </c>
       <c r="B6" t="s">
         <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="D6" t="s">
         <v>426</v>
@@ -4036,19 +4058,19 @@
         <v>177</v>
       </c>
       <c r="F6" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="G6" t="s">
         <v>246</v>
       </c>
       <c r="H6" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="I6" t="e">
         <v>#N/A</v>
       </c>
       <c r="J6" t="s">
-        <v>753</v>
+        <v>748</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -4077,7 +4099,7 @@
         <v>-5</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -4106,12 +4128,12 @@
         <v>-10</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
       <c r="B9" t="s">
         <v>423</v>
@@ -4126,10 +4148,10 @@
         <v>177</v>
       </c>
       <c r="F9" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="H9" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="I9" t="e">
         <f>NA()</f>
@@ -4167,7 +4189,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
       <c r="B11" t="s">
         <v>423</v>
@@ -4182,13 +4204,13 @@
         <v>177</v>
       </c>
       <c r="F11" t="s">
-        <v>750</v>
+        <v>745</v>
       </c>
       <c r="G11" t="s">
-        <v>751</v>
+        <v>746</v>
       </c>
       <c r="H11" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -4237,7 +4259,7 @@
         <v>26</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>534</v>
@@ -4265,7 +4287,7 @@
         <v>26</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>534</v>
@@ -4293,7 +4315,7 @@
         <v>26</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E15" s="20" t="s">
         <v>534</v>
@@ -4321,7 +4343,7 @@
         <v>26</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>534</v>
@@ -4349,7 +4371,7 @@
         <v>26</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>534</v>
@@ -4377,7 +4399,7 @@
         <v>26</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>575</v>
@@ -4405,7 +4427,7 @@
         <v>26</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>534</v>
@@ -4433,7 +4455,7 @@
         <v>26</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>177</v>
@@ -4461,7 +4483,7 @@
         <v>26</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E21" s="20" t="s">
         <v>534</v>
@@ -4489,7 +4511,7 @@
         <v>26</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="E22" t="s">
         <v>466</v>
@@ -4518,7 +4540,7 @@
         <v>26</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>193</v>
@@ -4547,7 +4569,7 @@
         <v>26</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>193</v>
@@ -4576,7 +4598,7 @@
         <v>26</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>177</v>
@@ -4605,7 +4627,7 @@
         <v>26</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>230</v>
@@ -4634,7 +4656,7 @@
         <v>26</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>237</v>
@@ -4868,7 +4890,7 @@
         <v>26</v>
       </c>
       <c r="D35" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="E35" t="s">
         <v>112</v>
@@ -4888,7 +4910,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="B36" t="s">
         <v>423</v>
@@ -4900,16 +4922,16 @@
         <v>662</v>
       </c>
       <c r="E36" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="F36" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="G36" t="s">
-        <v>717</v>
+        <v>712</v>
       </c>
       <c r="H36" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="I36">
         <v>0</v>
@@ -4926,7 +4948,7 @@
         <v>26</v>
       </c>
       <c r="D37" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E37" t="s">
         <v>177</v>
@@ -4955,7 +4977,7 @@
         <v>26</v>
       </c>
       <c r="D38" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E38" t="s">
         <v>322</v>
@@ -4984,7 +5006,7 @@
         <v>26</v>
       </c>
       <c r="D39" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E39" t="s">
         <v>322</v>
@@ -5013,7 +5035,7 @@
         <v>26</v>
       </c>
       <c r="D40" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E40" t="s">
         <v>322</v>
@@ -5042,7 +5064,7 @@
         <v>26</v>
       </c>
       <c r="D41" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E41" t="s">
         <v>322</v>
@@ -5071,7 +5093,7 @@
         <v>26</v>
       </c>
       <c r="D42" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E42" t="s">
         <v>322</v>
@@ -5100,7 +5122,7 @@
         <v>26</v>
       </c>
       <c r="D43" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E43" t="s">
         <v>322</v>
@@ -5129,7 +5151,7 @@
         <v>26</v>
       </c>
       <c r="D44" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E44" t="s">
         <v>322</v>
@@ -5158,7 +5180,7 @@
         <v>26</v>
       </c>
       <c r="D45" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E45" t="s">
         <v>322</v>
@@ -5187,7 +5209,7 @@
         <v>26</v>
       </c>
       <c r="D46" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E46" t="s">
         <v>322</v>
@@ -5216,7 +5238,7 @@
         <v>26</v>
       </c>
       <c r="D47" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E47" t="s">
         <v>322</v>
@@ -5245,7 +5267,7 @@
         <v>26</v>
       </c>
       <c r="D48" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="E48" t="s">
         <v>104</v>
@@ -5302,7 +5324,7 @@
         <v>26</v>
       </c>
       <c r="D50" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="E50" t="s">
         <v>14</v>
@@ -5332,7 +5354,7 @@
         <v>26</v>
       </c>
       <c r="D51" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="E51" t="s">
         <v>16</v>
@@ -5362,7 +5384,7 @@
         <v>26</v>
       </c>
       <c r="D52" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="E52" t="s">
         <v>15</v>
@@ -5392,7 +5414,7 @@
         <v>26</v>
       </c>
       <c r="D53" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="E53" t="s">
         <v>15</v>
@@ -5413,7 +5435,7 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="B54" t="s">
         <v>135</v>
@@ -5425,16 +5447,16 @@
         <v>426</v>
       </c>
       <c r="E54" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="F54" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="G54" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
       <c r="H54" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="I54" t="e">
         <v>#N/A</v>
@@ -5451,7 +5473,7 @@
         <v>26</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E55" s="20" t="s">
         <v>517</v>
@@ -5477,7 +5499,7 @@
         <v>26</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E56" s="20" t="s">
         <v>520</v>
@@ -5503,7 +5525,7 @@
         <v>26</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E57" s="20" t="s">
         <v>523</v>
@@ -5529,7 +5551,7 @@
         <v>26</v>
       </c>
       <c r="D58" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E58" s="20" t="s">
         <v>526</v>
@@ -5555,7 +5577,7 @@
         <v>26</v>
       </c>
       <c r="D59" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E59" s="20" t="s">
         <v>503</v>
@@ -5581,7 +5603,7 @@
         <v>26</v>
       </c>
       <c r="D60" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E60" s="20" t="s">
         <v>507</v>
@@ -5607,7 +5629,7 @@
         <v>26</v>
       </c>
       <c r="D61" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E61" s="20" t="s">
         <v>507</v>
@@ -5633,7 +5655,7 @@
         <v>26</v>
       </c>
       <c r="D62" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E62" s="20" t="s">
         <v>507</v>
@@ -5659,7 +5681,7 @@
         <v>26</v>
       </c>
       <c r="D63" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E63" s="20" t="s">
         <v>503</v>
@@ -5685,7 +5707,7 @@
         <v>26</v>
       </c>
       <c r="D64" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E64" s="20" t="s">
         <v>517</v>
@@ -5711,7 +5733,7 @@
         <v>26</v>
       </c>
       <c r="D65" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E65" s="20" t="s">
         <v>514</v>
@@ -5737,7 +5759,7 @@
         <v>26</v>
       </c>
       <c r="D66" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E66" s="20" t="s">
         <v>531</v>
@@ -5763,7 +5785,7 @@
         <v>26</v>
       </c>
       <c r="D67" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="E67" s="7" t="s">
         <v>177</v>
@@ -5793,7 +5815,7 @@
         <v>26</v>
       </c>
       <c r="D68" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="E68" s="7" t="s">
         <v>249</v>
@@ -5823,7 +5845,7 @@
         <v>26</v>
       </c>
       <c r="D69" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="E69" s="12" t="s">
         <v>268</v>
@@ -5853,7 +5875,7 @@
         <v>26</v>
       </c>
       <c r="D70" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="E70" s="12" t="s">
         <v>268</v>
@@ -5883,7 +5905,7 @@
         <v>26</v>
       </c>
       <c r="D71" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="E71" s="12" t="s">
         <v>268</v>
@@ -5913,7 +5935,7 @@
         <v>26</v>
       </c>
       <c r="D72" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="E72" s="12" t="s">
         <v>268</v>
@@ -5943,7 +5965,7 @@
         <v>26</v>
       </c>
       <c r="D73" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="E73" s="7" t="s">
         <v>177</v>
@@ -5973,7 +5995,7 @@
         <v>26</v>
       </c>
       <c r="D74" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="E74" s="7" t="s">
         <v>177</v>
@@ -6003,7 +6025,7 @@
         <v>26</v>
       </c>
       <c r="D75" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="E75" s="9" t="s">
         <v>217</v>
@@ -6036,7 +6058,7 @@
         <v>26</v>
       </c>
       <c r="D76" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="E76" t="s">
         <v>15</v>
@@ -6069,7 +6091,7 @@
         <v>26</v>
       </c>
       <c r="D77" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="E77" s="12" t="s">
         <v>268</v>
@@ -6093,7 +6115,7 @@
         <v>26</v>
       </c>
       <c r="D78" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="E78" s="12" t="s">
         <v>268</v>
@@ -6120,7 +6142,7 @@
         <v>26</v>
       </c>
       <c r="D79" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="E79" s="7" t="s">
         <v>220</v>
@@ -6150,7 +6172,7 @@
         <v>26</v>
       </c>
       <c r="D80" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="E80" s="7" t="s">
         <v>242</v>
@@ -6180,7 +6202,7 @@
         <v>26</v>
       </c>
       <c r="D81" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="E81" s="7" t="s">
         <v>206</v>
@@ -6210,7 +6232,7 @@
         <v>26</v>
       </c>
       <c r="D82" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="E82" s="7" t="s">
         <v>206</v>
@@ -6619,7 +6641,7 @@
         <v>26</v>
       </c>
       <c r="D96" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="E96" t="s">
         <v>112</v>
@@ -6649,7 +6671,7 @@
         <v>26</v>
       </c>
       <c r="D97" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="E97" s="7" t="s">
         <v>351</v>
@@ -6670,7 +6692,7 @@
     </row>
     <row r="98" spans="1:10">
       <c r="A98" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B98" t="s">
         <v>135</v>
@@ -6685,13 +6707,13 @@
         <v>177</v>
       </c>
       <c r="F98" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="G98" t="s">
         <v>652</v>
       </c>
       <c r="H98" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="I98" t="e">
         <f>NA()</f>
@@ -6769,7 +6791,7 @@
         <v>26</v>
       </c>
       <c r="D101" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E101" t="s">
         <v>177</v>
@@ -6858,7 +6880,7 @@
         <v>26</v>
       </c>
       <c r="D104" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E104" s="20" t="s">
         <v>546</v>
@@ -6887,7 +6909,7 @@
         <v>26</v>
       </c>
       <c r="D105" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E105" s="20" t="s">
         <v>534</v>
@@ -6917,7 +6939,7 @@
         <v>26</v>
       </c>
       <c r="D106" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E106" s="20" t="s">
         <v>546</v>
@@ -6947,7 +6969,7 @@
         <v>26</v>
       </c>
       <c r="D107" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E107" s="20" t="s">
         <v>546</v>
@@ -6977,7 +6999,7 @@
         <v>26</v>
       </c>
       <c r="D108" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E108" s="20" t="s">
         <v>507</v>
@@ -7007,7 +7029,7 @@
         <v>26</v>
       </c>
       <c r="D109" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E109" s="20" t="s">
         <v>503</v>
@@ -7037,7 +7059,7 @@
         <v>26</v>
       </c>
       <c r="D110" s="20" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="E110" s="20" t="s">
         <v>546</v>
@@ -7067,7 +7089,7 @@
         <v>26</v>
       </c>
       <c r="D111" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="E111" s="7" t="s">
         <v>253</v>
@@ -7097,7 +7119,7 @@
         <v>26</v>
       </c>
       <c r="D112" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="E112" s="7" t="s">
         <v>238</v>
@@ -7129,7 +7151,7 @@
         <v>26</v>
       </c>
       <c r="D113" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="E113" s="7" t="s">
         <v>249</v>
@@ -7159,7 +7181,7 @@
         <v>26</v>
       </c>
       <c r="D114" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="E114" t="s">
         <v>195</v>
@@ -7191,7 +7213,7 @@
         <v>26</v>
       </c>
       <c r="D115" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="E115" t="s">
         <v>193</v>
@@ -7221,7 +7243,7 @@
         <v>26</v>
       </c>
       <c r="D116" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="E116" t="s">
         <v>195</v>
@@ -7251,7 +7273,7 @@
         <v>26</v>
       </c>
       <c r="D117" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="E117" t="s">
         <v>193</v>
@@ -7669,7 +7691,7 @@
     </row>
     <row r="131" spans="1:10">
       <c r="A131" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="B131" t="s">
         <v>41</v>
@@ -7700,7 +7722,7 @@
     </row>
     <row r="132" spans="1:10">
       <c r="A132" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="B132" t="s">
         <v>41</v>
@@ -7715,13 +7737,13 @@
         <v>160</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>744</v>
+        <v>739</v>
       </c>
       <c r="G132" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="H132" t="s">
-        <v>746</v>
+        <v>741</v>
       </c>
       <c r="I132" t="e">
         <f>NA()</f>
@@ -7731,7 +7753,7 @@
     </row>
     <row r="133" spans="1:10">
       <c r="A133" t="s">
-        <v>670</v>
+        <v>749</v>
       </c>
       <c r="B133" t="s">
         <v>41</v>
@@ -7746,22 +7768,25 @@
         <v>112</v>
       </c>
       <c r="F133" t="s">
-        <v>672</v>
+        <v>751</v>
       </c>
       <c r="G133" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="H133" t="s">
-        <v>673</v>
+        <v>752</v>
       </c>
       <c r="I133" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
+      <c r="J133" t="s">
+        <v>750</v>
+      </c>
     </row>
     <row r="134" spans="1:10">
       <c r="A134" t="s">
-        <v>663</v>
+        <v>753</v>
       </c>
       <c r="B134" t="s">
         <v>41</v>
@@ -7776,22 +7801,25 @@
         <v>160</v>
       </c>
       <c r="F134" t="s">
+        <v>755</v>
+      </c>
+      <c r="G134" t="s">
+        <v>663</v>
+      </c>
+      <c r="H134" t="s">
         <v>664</v>
-      </c>
-      <c r="G134" t="s">
-        <v>665</v>
-      </c>
-      <c r="H134" t="s">
-        <v>666</v>
       </c>
       <c r="I134" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
+      <c r="J134" t="s">
+        <v>754</v>
+      </c>
     </row>
     <row r="135" spans="1:10">
       <c r="A135" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="B135" t="s">
         <v>41</v>
@@ -7800,19 +7828,19 @@
         <v>26</v>
       </c>
       <c r="D135" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E135" t="s">
         <v>112</v>
       </c>
       <c r="F135" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="G135" t="s">
         <v>400</v>
       </c>
       <c r="H135" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="I135" t="e">
         <f>NA()</f>
@@ -7830,7 +7858,7 @@
         <v>26</v>
       </c>
       <c r="D136" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E136" t="s">
         <v>112</v>
@@ -7854,7 +7882,7 @@
         <v>26</v>
       </c>
       <c r="D137" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E137" t="s">
         <v>112</v>
@@ -7875,7 +7903,7 @@
         <v>26</v>
       </c>
       <c r="D138" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E138" t="s">
         <v>112</v>
@@ -7896,7 +7924,7 @@
         <v>26</v>
       </c>
       <c r="D139" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E139" t="s">
         <v>112</v>
@@ -7917,7 +7945,7 @@
         <v>26</v>
       </c>
       <c r="D140" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E140" t="s">
         <v>112</v>
@@ -7938,7 +7966,7 @@
         <v>26</v>
       </c>
       <c r="D141" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E141" t="s">
         <v>112</v>
@@ -7959,7 +7987,7 @@
         <v>26</v>
       </c>
       <c r="D142" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E142" t="s">
         <v>112</v>
@@ -7980,7 +8008,7 @@
         <v>26</v>
       </c>
       <c r="D143" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E143" t="s">
         <v>112</v>
@@ -8001,7 +8029,7 @@
         <v>26</v>
       </c>
       <c r="D144" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E144" t="s">
         <v>112</v>
@@ -8022,7 +8050,7 @@
         <v>26</v>
       </c>
       <c r="D145" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E145" t="s">
         <v>112</v>
@@ -8034,7 +8062,7 @@
     </row>
     <row r="146" spans="1:10">
       <c r="A146" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
       <c r="B146" t="s">
         <v>41</v>
@@ -8043,19 +8071,19 @@
         <v>26</v>
       </c>
       <c r="D146" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E146" t="s">
         <v>112</v>
       </c>
       <c r="F146" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="G146" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="H146" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
       <c r="I146" t="e">
         <f>NA()</f>
@@ -8064,7 +8092,7 @@
     </row>
     <row r="147" spans="1:10">
       <c r="A147" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="B147" t="s">
         <v>41</v>
@@ -8073,19 +8101,19 @@
         <v>26</v>
       </c>
       <c r="D147" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E147" t="s">
         <v>112</v>
       </c>
       <c r="F147" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="G147" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="H147" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="I147" t="e">
         <f>NA()</f>
@@ -8094,7 +8122,7 @@
     </row>
     <row r="148" spans="1:10">
       <c r="A148" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="B148" t="s">
         <v>41</v>
@@ -8103,19 +8131,19 @@
         <v>26</v>
       </c>
       <c r="D148" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E148" t="s">
         <v>112</v>
       </c>
       <c r="F148" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="G148" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="H148" s="13" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="I148" t="e">
         <f>NA()</f>
@@ -8124,7 +8152,7 @@
     </row>
     <row r="149" spans="1:10">
       <c r="A149" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="B149" t="s">
         <v>41</v>
@@ -8133,19 +8161,19 @@
         <v>26</v>
       </c>
       <c r="D149" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E149" t="s">
         <v>112</v>
       </c>
       <c r="F149" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="G149" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="H149" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="I149" t="e">
         <f>NA()</f>
@@ -8163,7 +8191,7 @@
         <v>26</v>
       </c>
       <c r="D150" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E150" t="s">
         <v>112</v>
@@ -8184,7 +8212,7 @@
     </row>
     <row r="151" spans="1:10">
       <c r="A151" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="B151" t="s">
         <v>41</v>
@@ -8193,25 +8221,25 @@
         <v>26</v>
       </c>
       <c r="D151" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="E151" t="s">
         <v>112</v>
       </c>
       <c r="F151" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="G151" t="s">
+        <v>678</v>
+      </c>
+      <c r="H151" t="s">
         <v>683</v>
-      </c>
-      <c r="H151" t="s">
-        <v>688</v>
       </c>
       <c r="I151">
         <v>0</v>
       </c>
       <c r="J151" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
     </row>
     <row r="152" spans="1:10">
@@ -8225,7 +8253,7 @@
         <v>26</v>
       </c>
       <c r="D152" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="E152" t="s">
         <v>16</v>
@@ -8255,7 +8283,7 @@
         <v>26</v>
       </c>
       <c r="D153" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="E153" t="s">
         <v>112</v>
@@ -8285,7 +8313,7 @@
         <v>26</v>
       </c>
       <c r="D154" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="E154" t="s">
         <v>112</v>
@@ -8406,13 +8434,13 @@
         <v>346</v>
       </c>
       <c r="F3" t="s">
-        <v>719</v>
+        <v>714</v>
       </c>
       <c r="G3" t="s">
         <v>634</v>
       </c>
       <c r="H3" t="s">
-        <v>720</v>
+        <v>715</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -8438,7 +8466,7 @@
         <v>635</v>
       </c>
       <c r="H4" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -8464,7 +8492,7 @@
         <v>636</v>
       </c>
       <c r="H5" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -8490,7 +8518,7 @@
         <v>639</v>
       </c>
       <c r="H6" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -8516,7 +8544,7 @@
         <v>637</v>
       </c>
       <c r="H7" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -8605,13 +8633,13 @@
         <v>362</v>
       </c>
       <c r="F11" t="s">
-        <v>726</v>
+        <v>721</v>
       </c>
       <c r="G11" t="s">
         <v>597</v>
       </c>
       <c r="H11" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -8634,7 +8662,7 @@
         <v>595</v>
       </c>
       <c r="H12" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -8766,7 +8794,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>748</v>
+        <v>743</v>
       </c>
       <c r="B18" t="s">
         <v>344</v>
@@ -8804,7 +8832,7 @@
         <v>617</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>728</v>
+        <v>723</v>
       </c>
       <c r="G19" t="s">
         <v>610</v>
@@ -8830,7 +8858,7 @@
         <v>617</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="G20" t="s">
         <v>611</v>
@@ -9516,7 +9544,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
       <c r="B7" t="s">
         <v>36</v>
@@ -9528,13 +9556,13 @@
         <v>426</v>
       </c>
       <c r="F7" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="G7" t="e">
         <v>#N/A</v>
       </c>
       <c r="H7" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
       <c r="I7">
         <v>0.05</v>
@@ -9542,7 +9570,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>730</v>
+        <v>725</v>
       </c>
       <c r="B8" t="s">
         <v>36</v>
@@ -9554,13 +9582,13 @@
         <v>662</v>
       </c>
       <c r="F8" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
       <c r="G8" t="e">
         <v>#N/A</v>
       </c>
       <c r="H8" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
       <c r="I8">
         <v>0.02</v>

</xml_diff>

<commit_message>
update N applications and changelog
</commit_message>
<xml_diff>
--- a/allvariables.xlsx
+++ b/allvariables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Achille\Documents\GitHub\SSM.R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713A1245-1CC3-4EFD-8BC4-53D921659107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D88732-FF43-45B4-9E2D-BE47F50A019F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="790" windowWidth="10400" windowHeight="9410" tabRatio="652" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8800" yWindow="790" windowWidth="10400" windowHeight="9410" tabRatio="652" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nomenclature" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2939" uniqueCount="1364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3019" uniqueCount="1394">
   <si>
     <t>name</t>
   </si>
@@ -4203,6 +4203,96 @@
   </si>
   <si>
     <t>N application number</t>
+  </si>
+  <si>
+    <t>cFractionTranspirableWater.1</t>
+  </si>
+  <si>
+    <t>Quantité effective d'eau accessible pour absorption dans la couche 11</t>
+  </si>
+  <si>
+    <t>Fraction transpirable soil water in layer 1</t>
+  </si>
+  <si>
+    <t>cFractionTranspirableWater.2</t>
+  </si>
+  <si>
+    <t>Fraction transpirable soil water in layer 2</t>
+  </si>
+  <si>
+    <t>Quantité effective d'eau accessible pour absorption dans la couche 12</t>
+  </si>
+  <si>
+    <t>cFractionTranspirableWater.3</t>
+  </si>
+  <si>
+    <t>Fraction transpirable soil water in layer 3</t>
+  </si>
+  <si>
+    <t>Quantité effective d'eau accessible pour absorption dans la couche 13</t>
+  </si>
+  <si>
+    <t>cFractionTranspirableWater.4</t>
+  </si>
+  <si>
+    <t>Fraction transpirable soil water in layer 4</t>
+  </si>
+  <si>
+    <t>Quantité effective d'eau accessible pour absorption dans la couche 14</t>
+  </si>
+  <si>
+    <t>cFractionTranspirableWater.5</t>
+  </si>
+  <si>
+    <t>Fraction transpirable soil water in layer 5</t>
+  </si>
+  <si>
+    <t>Quantité effective d'eau accessible pour absorption dans la couche 15</t>
+  </si>
+  <si>
+    <t>cFractionTranspirableWater.6</t>
+  </si>
+  <si>
+    <t>Fraction transpirable soil water in layer 6</t>
+  </si>
+  <si>
+    <t>Quantité effective d'eau accessible pour absorption dans la couche 16</t>
+  </si>
+  <si>
+    <t>cFractionTranspirableWater.7</t>
+  </si>
+  <si>
+    <t>Fraction transpirable soil water in layer 7</t>
+  </si>
+  <si>
+    <t>Quantité effective d'eau accessible pour absorption dans la couche 17</t>
+  </si>
+  <si>
+    <t>cFractionTranspirableWater.8</t>
+  </si>
+  <si>
+    <t>Fraction transpirable soil water in layer 8</t>
+  </si>
+  <si>
+    <t>Quantité effective d'eau accessible pour absorption dans la couche 18</t>
+  </si>
+  <si>
+    <t>cFractionTranspirableWater.9</t>
+  </si>
+  <si>
+    <t>Fraction transpirable soil water in layer 9</t>
+  </si>
+  <si>
+    <t>Quantité effective d'eau accessible pour absorption dans la couche 19</t>
+  </si>
+  <si>
+    <t>cFractionTranspirableWater.10</t>
+  </si>
+  <si>
+    <t>Fraction transpirable soil water in layer 10</t>
+  </si>
+  <si>
+    <t>Quantité effective d'eau accessible pour absorption dans la couche 20</t>
   </si>
 </sst>
 </file>
@@ -5923,13 +6013,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:T291"/>
+  <dimension ref="A1:T301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B134" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F279" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A293" sqref="A293"/>
+      <selection pane="bottomRight" activeCell="F300" sqref="F300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -14798,35 +14888,325 @@
       </c>
     </row>
     <row r="291" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A291" s="30" t="s">
+      <c r="A291" s="80" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B291" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="C291" s="84" t="s">
+        <v>26</v>
+      </c>
+      <c r="D291" s="84" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E291" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="F291" s="84" t="s">
+        <v>1366</v>
+      </c>
+      <c r="G291" s="84" t="s">
+        <v>771</v>
+      </c>
+      <c r="H291" s="84" t="s">
+        <v>1365</v>
+      </c>
+      <c r="I291" s="85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A292" s="80" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B292" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="C292" s="84" t="s">
+        <v>26</v>
+      </c>
+      <c r="D292" s="84" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E292" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="F292" s="84" t="s">
+        <v>1368</v>
+      </c>
+      <c r="G292" s="84" t="s">
+        <v>771</v>
+      </c>
+      <c r="H292" s="84" t="s">
+        <v>1369</v>
+      </c>
+      <c r="I292" s="85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A293" s="80" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B293" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="C293" s="84" t="s">
+        <v>26</v>
+      </c>
+      <c r="D293" s="84" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E293" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="F293" s="84" t="s">
+        <v>1371</v>
+      </c>
+      <c r="G293" s="84" t="s">
+        <v>771</v>
+      </c>
+      <c r="H293" s="84" t="s">
+        <v>1372</v>
+      </c>
+      <c r="I293" s="85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A294" s="80" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B294" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="C294" s="84" t="s">
+        <v>26</v>
+      </c>
+      <c r="D294" s="84" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E294" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="F294" s="84" t="s">
+        <v>1374</v>
+      </c>
+      <c r="G294" s="84" t="s">
+        <v>771</v>
+      </c>
+      <c r="H294" s="84" t="s">
+        <v>1375</v>
+      </c>
+      <c r="I294" s="85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A295" s="80" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B295" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="C295" s="84" t="s">
+        <v>26</v>
+      </c>
+      <c r="D295" s="84" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E295" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="F295" s="84" t="s">
+        <v>1377</v>
+      </c>
+      <c r="G295" s="84" t="s">
+        <v>771</v>
+      </c>
+      <c r="H295" s="84" t="s">
+        <v>1378</v>
+      </c>
+      <c r="I295" s="85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A296" s="80" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B296" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="C296" s="84" t="s">
+        <v>26</v>
+      </c>
+      <c r="D296" s="84" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E296" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="F296" s="84" t="s">
+        <v>1380</v>
+      </c>
+      <c r="G296" s="84" t="s">
+        <v>771</v>
+      </c>
+      <c r="H296" s="84" t="s">
+        <v>1381</v>
+      </c>
+      <c r="I296" s="85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A297" s="80" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B297" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="C297" s="84" t="s">
+        <v>26</v>
+      </c>
+      <c r="D297" s="84" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E297" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="F297" s="84" t="s">
+        <v>1383</v>
+      </c>
+      <c r="G297" s="84" t="s">
+        <v>771</v>
+      </c>
+      <c r="H297" s="84" t="s">
+        <v>1384</v>
+      </c>
+      <c r="I297" s="85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A298" s="80" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B298" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="C298" s="84" t="s">
+        <v>26</v>
+      </c>
+      <c r="D298" s="84" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E298" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="F298" s="84" t="s">
+        <v>1386</v>
+      </c>
+      <c r="G298" s="84" t="s">
+        <v>771</v>
+      </c>
+      <c r="H298" s="84" t="s">
+        <v>1387</v>
+      </c>
+      <c r="I298" s="85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A299" s="80" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B299" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="C299" s="84" t="s">
+        <v>26</v>
+      </c>
+      <c r="D299" s="84" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E299" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="F299" s="84" t="s">
+        <v>1389</v>
+      </c>
+      <c r="G299" s="84" t="s">
+        <v>771</v>
+      </c>
+      <c r="H299" s="84" t="s">
+        <v>1390</v>
+      </c>
+      <c r="I299" s="85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A300" s="80" t="s">
+        <v>1391</v>
+      </c>
+      <c r="B300" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="C300" s="84" t="s">
+        <v>26</v>
+      </c>
+      <c r="D300" s="84" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E300" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="F300" s="84" t="s">
+        <v>1392</v>
+      </c>
+      <c r="G300" s="84" t="s">
+        <v>771</v>
+      </c>
+      <c r="H300" s="84" t="s">
+        <v>1393</v>
+      </c>
+      <c r="I300" s="85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A301" s="30" t="s">
         <v>1299</v>
       </c>
-      <c r="B291" s="30" t="s">
+      <c r="B301" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="C291" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="D291" s="30" t="s">
+      <c r="C301" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D301" s="30" t="s">
         <v>1213</v>
       </c>
-      <c r="E291" s="30" t="s">
+      <c r="E301" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="F291" s="30" t="s">
+      <c r="F301" s="30" t="s">
         <v>1300</v>
       </c>
-      <c r="G291" s="30" t="s">
+      <c r="G301" s="30" t="s">
         <v>767</v>
       </c>
-      <c r="H291" s="30" t="s">
+      <c r="H301" s="30" t="s">
         <v>1301</v>
       </c>
-      <c r="I291" s="30" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J291" s="23" t="s">
+      <c r="I301" s="30" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J301" s="23" t="s">
         <v>1286</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Started adding gaetan's work
</commit_message>
<xml_diff>
--- a/allvariables.xlsx
+++ b/allvariables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Achille\Documents\GitHub\SSM.R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B8A182-16CC-4441-A665-4E60FA2FCC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E133246-77BF-4022-8D08-45B3ADC74972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="652" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9030" yWindow="400" windowWidth="10400" windowHeight="9410" tabRatio="652" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nomenclature" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3024" uniqueCount="1396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3277" uniqueCount="1536">
   <si>
     <t>name</t>
   </si>
@@ -4300,12 +4300,540 @@
   <si>
     <t>rIrrigation</t>
   </si>
+  <si>
+    <t>cDemandNAccumulation</t>
+  </si>
+  <si>
+    <t>rUpdatePlantNitrogen</t>
+  </si>
+  <si>
+    <t>g m−2 day−1</t>
+  </si>
+  <si>
+    <t>Daily demand for N accumulation</t>
+  </si>
+  <si>
+    <t>NUP</t>
+  </si>
+  <si>
+    <t>Besoin quotidien pour accumulation d’Azote</t>
+  </si>
+  <si>
+    <t>cBiologicalNFixation</t>
+  </si>
+  <si>
+    <t>Biological nitrogen Fixation</t>
+  </si>
+  <si>
+    <t>BNF</t>
+  </si>
+  <si>
+    <t>Fixation de l’azote de l’air</t>
+  </si>
+  <si>
+    <t>NUP2</t>
+  </si>
+  <si>
+    <t>g m−2 day−2</t>
+  </si>
+  <si>
+    <t>Adjusted NUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nup ajusté </t>
+  </si>
+  <si>
+    <t>sAccumulatedAboveGroundN</t>
+  </si>
+  <si>
+    <t>Accumulated nitrogen in above-ground crop organs</t>
+  </si>
+  <si>
+    <t>CNUP</t>
+  </si>
+  <si>
+    <t>Azote accumulé dans les organes plein air de la plante</t>
+  </si>
+  <si>
+    <t>pSNCG</t>
+  </si>
+  <si>
+    <t>g N g-1</t>
+  </si>
+  <si>
+    <t>N content per unit stem weight</t>
+  </si>
+  <si>
+    <t>SNCG</t>
+  </si>
+  <si>
+    <t>Teneur en azote par masse de tige</t>
+  </si>
+  <si>
+    <t>cDemandResultDeficiencies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">daily N demand as a result of N deficiencies in the plant that developed early in the season 
+</t>
+  </si>
+  <si>
+    <t>NSTDF</t>
+  </si>
+  <si>
+    <t>Demande quotidienne en N dû aux carences des précédentes plantes</t>
+  </si>
+  <si>
+    <t>pNUPmax</t>
+  </si>
+  <si>
+    <t>NUP maximum rate</t>
+  </si>
+  <si>
+    <t>MXNUP</t>
+  </si>
+  <si>
+    <t>Taux maximum d’NUP</t>
+  </si>
+  <si>
+    <t>cDailySeedsNDemands</t>
+  </si>
+  <si>
+    <t>G m-2 d-1</t>
+  </si>
+  <si>
+    <t>Daily N demand by the seeds</t>
+  </si>
+  <si>
+    <t>INGRN</t>
+  </si>
+  <si>
+    <t>Besoin quotidien en N par les graines</t>
+  </si>
+  <si>
+    <t>sGrainConcentrationN</t>
+  </si>
+  <si>
+    <t>G N g-1</t>
+  </si>
+  <si>
+    <t>Grain N concentration</t>
+  </si>
+  <si>
+    <t>GNC</t>
+  </si>
+  <si>
+    <t>Concentration en N des graines</t>
+  </si>
+  <si>
+    <t>pGrainMinConcentrationN</t>
+  </si>
+  <si>
+    <t>Grain min N concentration</t>
+  </si>
+  <si>
+    <t>GNCmin</t>
+  </si>
+  <si>
+    <t>Concentration minimum en N des graines</t>
+  </si>
+  <si>
+    <t>pGrainMaxConcentrationN</t>
+  </si>
+  <si>
+    <t>Grain max N concentration</t>
+  </si>
+  <si>
+    <t>GNCmax</t>
+  </si>
+  <si>
+    <t>Concentration maximum en N des graines</t>
+  </si>
+  <si>
+    <t>cTotalMobilizable</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="17"/>
+        <rFont val="Trebuchet MS"/>
+      </rPr>
+      <t xml:space="preserve">Total mobilizable N available in the plant at the beginning of seed fill </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="17"/>
+        <rFont val="Times"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>TRLN</t>
+  </si>
+  <si>
+    <t>Quantité totale d’azote disponible dans la plante au début du remplissage des semences</t>
+  </si>
+  <si>
+    <t>cBSGMobilizable</t>
+  </si>
+  <si>
+    <t>G N m-2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="17"/>
+        <rFont val="Trebuchet MS"/>
+      </rPr>
+      <t>Total mobilizable N available in the plant before seed growth</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="17"/>
+        <rFont val="Times"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>TRLNBSG</t>
+  </si>
+  <si>
+    <t>Quantité totale d’azote disponible dans la plante avant la croissance des graines</t>
+  </si>
+  <si>
+    <t>cProportionDailyFromLeaves</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="17"/>
+        <rFont val="Trebuchet MS"/>
+      </rPr>
+      <t xml:space="preserve">proportion of the daily N transfer from the leaves </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="17"/>
+        <rFont val="Times"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>FXLF</t>
+  </si>
+  <si>
+    <t>Proportion quotidienne d’azote transférée des feuilles</t>
+  </si>
+  <si>
+    <t>sDailyRateNFromStem</t>
+  </si>
+  <si>
+    <t>rUpdatePlantNitrogeng N m-2 d-1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="17"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">Daily rate of nitrogen mobilized from stems </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="17"/>
+        <rFont val="Times"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="17"/>
+        <rFont val="Times"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>XNST</t>
+  </si>
+  <si>
+    <t>Taux quotidien d’azote mobilisé dans la tige</t>
+  </si>
+  <si>
+    <t>cEstimateSupplyVeg</t>
+  </si>
+  <si>
+    <t>Estimate of supply from veg</t>
+  </si>
+  <si>
+    <t>XNVEG</t>
+  </si>
+  <si>
+    <t>Estimation de l’approvisionnement en légumes</t>
+  </si>
+  <si>
+    <t>sDailyAccumulationStemN</t>
+  </si>
+  <si>
+    <t>G N m-2 d-1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="17"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">Daily rate of nitrogen accumulation in stems
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="17"/>
+        <rFont val="Times"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>INST</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Taux quotidien d’accumulation d’azote dans la tige</t>
+  </si>
+  <si>
+    <t>sDailyAccumulationLeavesN</t>
+  </si>
+  <si>
+    <t>G N m-2 d0</t>
+  </si>
+  <si>
+    <t>Daily rate of nitrogen accumulation in leaves</t>
+  </si>
+  <si>
+    <t>INLF</t>
+  </si>
+  <si>
+    <t>Augmentation quotidienne en azote dans les feuilles</t>
+  </si>
+  <si>
+    <t>sBdFromSowingToEmerge</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Biological day form sowing to emergence</t>
+  </si>
+  <si>
+    <t>bdEMR</t>
+  </si>
+  <si>
+    <t>Nombre de jours biologiques de la semis à l’émergence des feuilles</t>
+  </si>
+  <si>
+    <t>sBdFromSowingToTerminationLeaf</t>
+  </si>
+  <si>
+    <t>Biological day from sowing to termination leaf growth</t>
+  </si>
+  <si>
+    <t>bdTSG</t>
+  </si>
+  <si>
+    <t>Nombre de jours biologiques de la semis à la croissance des feuilles de terminaison</t>
+  </si>
+  <si>
+    <t>sBdFromSowingToFixation</t>
+  </si>
+  <si>
+    <t>Biological day from sowing to biological nitrogen fixation</t>
+  </si>
+  <si>
+    <t>bdBNF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre de jours biologiques de la semis au début de la fixation d’azote </t>
+  </si>
+  <si>
+    <t>sBdFromSowingToSeedGrowth</t>
+  </si>
+  <si>
+    <t>Biological day from sowing to beginning seed growth</t>
+  </si>
+  <si>
+    <t>bdBSG</t>
+  </si>
+  <si>
+    <t>Nombre de jours biologiques de la semis à la croissance des graines</t>
+  </si>
+  <si>
+    <t>sNitrogenAccumulation</t>
+  </si>
+  <si>
+    <t>Nitrogen Accumulation</t>
+  </si>
+  <si>
+    <t>WSFN</t>
+  </si>
+  <si>
+    <t>Accumulation d’azote (dans WSF)</t>
+  </si>
+  <si>
+    <t>Process of WSF</t>
+  </si>
+  <si>
+    <t>sNitrogenContent</t>
+  </si>
+  <si>
+    <t>Cumulative Nitrogen Fixation day</t>
+  </si>
+  <si>
+    <t>CUMBNF</t>
+  </si>
+  <si>
+    <t>Nombre de jours cumulés pour la fixation de l’azote sur les plantes</t>
+  </si>
+  <si>
+    <t>sPotentielRateNitrogenFixation</t>
+  </si>
+  <si>
+    <t>Potential rate of biological nitrogen fixation</t>
+  </si>
+  <si>
+    <t>PDNF</t>
+  </si>
+  <si>
+    <t>Taux potentiel de fixation biologique de l’azote</t>
+  </si>
+  <si>
+    <t>cUptakeNGrain</t>
+  </si>
+  <si>
+    <t>N uptake fraction of grain</t>
+  </si>
+  <si>
+    <t>nup_fr_grn</t>
+  </si>
+  <si>
+    <t>Fraction d’absorption d’azote par les grains</t>
+  </si>
+  <si>
+    <t>sAccumulatedLeafNitrogen</t>
+  </si>
+  <si>
+    <t>Accumulated Nitrogen in leaf</t>
+  </si>
+  <si>
+    <t>NLF</t>
+  </si>
+  <si>
+    <t>Azote accumulé dans les feuilles</t>
+  </si>
+  <si>
+    <t>sAccumulatedNStem</t>
+  </si>
+  <si>
+    <t>G N m-1</t>
+  </si>
+  <si>
+    <t>Accumulated Nitrogen in Stem</t>
+  </si>
+  <si>
+    <t>NST</t>
+  </si>
+  <si>
+    <t>Azote accumulé dans la tige</t>
+  </si>
+  <si>
+    <t>Coefficient of biological nitrogen fixation per unit mass</t>
+  </si>
+  <si>
+    <t>NFC</t>
+  </si>
+  <si>
+    <t>Coefficient de fixation biologique de l’azote par unité de masse végétative</t>
+  </si>
+  <si>
+    <t>cRateBiologicalNFix</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="18"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">Actual rate of biological nitrogen fixation
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="18"/>
+        <rFont val="Times"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>DNF</t>
+  </si>
+  <si>
+    <t>Taux de fixation biologique de l’azote</t>
+  </si>
+  <si>
+    <t>sTotalAccumulatedNitrogen</t>
+  </si>
+  <si>
+    <t>Total Accumulated Nitrogen</t>
+  </si>
+  <si>
+    <t>NVEG</t>
+  </si>
+  <si>
+    <t>Nitrogen totale fixé (Tige + Feuilles)</t>
+  </si>
+  <si>
+    <t>sAccumulatedNGrain</t>
+  </si>
+  <si>
+    <t>Accumulated Nitrogen in grains</t>
+  </si>
+  <si>
+    <t>NGRN</t>
+  </si>
+  <si>
+    <t>Azote accumulé dans les graines</t>
+  </si>
+  <si>
+    <t>cCoefBiologicalNFixation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4402,8 +4930,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color indexed="17"/>
+      <name val="Trebuchet MS"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="17"/>
+      <name val="Trebuchet MS"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="17"/>
+      <name val="Times"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="17"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="18"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="18"/>
+      <name val="Times"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4440,8 +5009,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -4538,6 +5119,81 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="505">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -5046,7 +5702,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5146,6 +5802,21 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="15" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="505">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -6019,13 +6690,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:T302"/>
+  <dimension ref="A1:T334"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B164" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H302" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A180" sqref="A1:A1048576"/>
+      <selection pane="bottomRight" activeCell="I307" sqref="I307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -14835,7 +15506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A289" s="87" t="s">
         <v>1318</v>
       </c>
@@ -14864,7 +15535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A290" s="88" t="s">
         <v>1319</v>
       </c>
@@ -14893,7 +15564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A291" s="80" t="s">
         <v>1362</v>
       </c>
@@ -14922,7 +15593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A292" s="80" t="s">
         <v>1365</v>
       </c>
@@ -14951,7 +15622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A293" s="80" t="s">
         <v>1368</v>
       </c>
@@ -14980,7 +15651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A294" s="80" t="s">
         <v>1371</v>
       </c>
@@ -15009,7 +15680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A295" s="80" t="s">
         <v>1374</v>
       </c>
@@ -15038,7 +15709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A296" s="80" t="s">
         <v>1377</v>
       </c>
@@ -15067,7 +15738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A297" s="80" t="s">
         <v>1380</v>
       </c>
@@ -15096,7 +15767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A298" s="80" t="s">
         <v>1383</v>
       </c>
@@ -15125,7 +15796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A299" s="80" t="s">
         <v>1386</v>
       </c>
@@ -15154,7 +15825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A300" s="80" t="s">
         <v>1389</v>
       </c>
@@ -15183,7 +15854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A301" s="30" t="s">
         <v>1297</v>
       </c>
@@ -15216,7 +15887,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>1392</v>
       </c>
@@ -15235,6 +15906,1288 @@
       <c r="I302" t="e">
         <v>#N/A</v>
       </c>
+    </row>
+    <row r="303" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A303" s="89" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B303" s="89" t="s">
+        <v>41</v>
+      </c>
+      <c r="C303" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D303" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E303" s="89" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F303" s="89" t="s">
+        <v>1399</v>
+      </c>
+      <c r="G303" s="89" t="s">
+        <v>1400</v>
+      </c>
+      <c r="H303" s="89" t="s">
+        <v>1401</v>
+      </c>
+      <c r="I303" s="90" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J303" s="90"/>
+      <c r="K303" s="90"/>
+      <c r="L303" s="90"/>
+      <c r="M303" s="91"/>
+      <c r="N303" s="92"/>
+      <c r="O303" s="92"/>
+      <c r="P303" s="92"/>
+      <c r="Q303" s="92"/>
+      <c r="R303" s="92"/>
+      <c r="S303" s="92"/>
+      <c r="T303" s="92"/>
+    </row>
+    <row r="304" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A304" s="89" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B304" s="89" t="s">
+        <v>41</v>
+      </c>
+      <c r="C304" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D304" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E304" s="90"/>
+      <c r="F304" s="89" t="s">
+        <v>1403</v>
+      </c>
+      <c r="G304" s="89" t="s">
+        <v>1404</v>
+      </c>
+      <c r="H304" s="89" t="s">
+        <v>1405</v>
+      </c>
+      <c r="I304" s="90" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J304" s="90"/>
+      <c r="K304" s="90"/>
+      <c r="L304" s="90"/>
+      <c r="M304" s="91"/>
+      <c r="N304" s="92"/>
+      <c r="O304" s="92"/>
+      <c r="P304" s="92"/>
+      <c r="Q304" s="92"/>
+      <c r="R304" s="92"/>
+      <c r="S304" s="92"/>
+      <c r="T304" s="92"/>
+    </row>
+    <row r="305" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A305" s="89" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B305" s="89" t="s">
+        <v>41</v>
+      </c>
+      <c r="C305" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D305" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E305" s="89" t="s">
+        <v>1407</v>
+      </c>
+      <c r="F305" s="89" t="s">
+        <v>1408</v>
+      </c>
+      <c r="G305" s="89" t="s">
+        <v>1406</v>
+      </c>
+      <c r="H305" s="89" t="s">
+        <v>1409</v>
+      </c>
+      <c r="I305" s="90" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J305" s="90"/>
+      <c r="K305" s="90"/>
+      <c r="L305" s="90"/>
+      <c r="M305" s="91"/>
+      <c r="N305" s="92"/>
+      <c r="O305" s="92"/>
+      <c r="P305" s="92"/>
+      <c r="Q305" s="92"/>
+      <c r="R305" s="92"/>
+      <c r="S305" s="92"/>
+      <c r="T305" s="92"/>
+    </row>
+    <row r="306" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A306" s="89" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B306" s="89" t="s">
+        <v>418</v>
+      </c>
+      <c r="C306" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D306" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E306" s="89" t="s">
+        <v>206</v>
+      </c>
+      <c r="F306" s="89" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G306" s="89" t="s">
+        <v>1412</v>
+      </c>
+      <c r="H306" s="89" t="s">
+        <v>1413</v>
+      </c>
+      <c r="I306" s="90">
+        <v>0</v>
+      </c>
+      <c r="J306" s="90"/>
+      <c r="K306" s="90"/>
+      <c r="L306" s="90"/>
+      <c r="M306" s="91"/>
+      <c r="N306" s="92"/>
+      <c r="O306" s="92"/>
+      <c r="P306" s="92"/>
+      <c r="Q306" s="92"/>
+      <c r="R306" s="92"/>
+      <c r="S306" s="92"/>
+      <c r="T306" s="92"/>
+    </row>
+    <row r="307" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A307" s="89" t="s">
+        <v>1414</v>
+      </c>
+      <c r="B307" s="89" t="s">
+        <v>135</v>
+      </c>
+      <c r="C307" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D307" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E307" s="89" t="s">
+        <v>1415</v>
+      </c>
+      <c r="F307" s="93" t="s">
+        <v>1416</v>
+      </c>
+      <c r="G307" s="94" t="s">
+        <v>1417</v>
+      </c>
+      <c r="H307" s="89" t="s">
+        <v>1418</v>
+      </c>
+      <c r="I307" s="90" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J307" s="90"/>
+      <c r="K307" s="90"/>
+      <c r="L307" s="90"/>
+      <c r="M307" s="91"/>
+      <c r="N307" s="92"/>
+      <c r="O307" s="92"/>
+      <c r="P307" s="92"/>
+      <c r="Q307" s="92"/>
+      <c r="R307" s="92"/>
+      <c r="S307" s="92"/>
+      <c r="T307" s="92"/>
+    </row>
+    <row r="308" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A308" s="89" t="s">
+        <v>1419</v>
+      </c>
+      <c r="B308" s="89" t="s">
+        <v>41</v>
+      </c>
+      <c r="C308" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D308" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E308" s="89" t="s">
+        <v>770</v>
+      </c>
+      <c r="F308" s="95" t="s">
+        <v>1420</v>
+      </c>
+      <c r="G308" s="89" t="s">
+        <v>1421</v>
+      </c>
+      <c r="H308" s="89" t="s">
+        <v>1422</v>
+      </c>
+      <c r="I308" s="90" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J308" s="90"/>
+      <c r="K308" s="90"/>
+      <c r="L308" s="90"/>
+      <c r="M308" s="91"/>
+      <c r="N308" s="92"/>
+      <c r="O308" s="92"/>
+      <c r="P308" s="92"/>
+      <c r="Q308" s="92"/>
+      <c r="R308" s="92"/>
+      <c r="S308" s="92"/>
+      <c r="T308" s="92"/>
+    </row>
+    <row r="309" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A309" s="89" t="s">
+        <v>1423</v>
+      </c>
+      <c r="B309" s="89" t="s">
+        <v>135</v>
+      </c>
+      <c r="C309" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D309" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E309" s="89" t="s">
+        <v>203</v>
+      </c>
+      <c r="F309" s="89" t="s">
+        <v>1424</v>
+      </c>
+      <c r="G309" s="89" t="s">
+        <v>1425</v>
+      </c>
+      <c r="H309" s="89" t="s">
+        <v>1426</v>
+      </c>
+      <c r="I309" s="90" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J309" s="90"/>
+      <c r="K309" s="90"/>
+      <c r="L309" s="90"/>
+      <c r="M309" s="91"/>
+      <c r="N309" s="92"/>
+      <c r="O309" s="92"/>
+      <c r="P309" s="92"/>
+      <c r="Q309" s="92"/>
+      <c r="R309" s="92"/>
+      <c r="S309" s="92"/>
+      <c r="T309" s="92"/>
+    </row>
+    <row r="310" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A310" s="89" t="s">
+        <v>1427</v>
+      </c>
+      <c r="B310" s="89" t="s">
+        <v>41</v>
+      </c>
+      <c r="C310" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D310" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E310" s="89" t="s">
+        <v>1428</v>
+      </c>
+      <c r="F310" s="89" t="s">
+        <v>1429</v>
+      </c>
+      <c r="G310" s="89" t="s">
+        <v>1430</v>
+      </c>
+      <c r="H310" s="89" t="s">
+        <v>1431</v>
+      </c>
+      <c r="I310" s="90" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J310" s="90"/>
+      <c r="K310" s="90"/>
+      <c r="L310" s="90"/>
+      <c r="M310" s="91"/>
+      <c r="N310" s="92"/>
+      <c r="O310" s="92"/>
+      <c r="P310" s="92"/>
+      <c r="Q310" s="92"/>
+      <c r="R310" s="92"/>
+      <c r="S310" s="92"/>
+      <c r="T310" s="92"/>
+    </row>
+    <row r="311" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A311" s="89" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B311" s="89" t="s">
+        <v>418</v>
+      </c>
+      <c r="C311" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D311" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E311" s="89" t="s">
+        <v>1433</v>
+      </c>
+      <c r="F311" s="89" t="s">
+        <v>1434</v>
+      </c>
+      <c r="G311" s="96" t="s">
+        <v>1435</v>
+      </c>
+      <c r="H311" s="89" t="s">
+        <v>1436</v>
+      </c>
+      <c r="I311" s="90">
+        <v>0</v>
+      </c>
+      <c r="J311" s="90"/>
+      <c r="K311" s="90"/>
+      <c r="L311" s="90"/>
+      <c r="M311" s="91"/>
+      <c r="N311" s="92"/>
+      <c r="O311" s="92"/>
+      <c r="P311" s="92"/>
+      <c r="Q311" s="92"/>
+      <c r="R311" s="92"/>
+      <c r="S311" s="92"/>
+      <c r="T311" s="92"/>
+    </row>
+    <row r="312" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A312" s="89" t="s">
+        <v>1437</v>
+      </c>
+      <c r="B312" s="89" t="s">
+        <v>135</v>
+      </c>
+      <c r="C312" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D312" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E312" s="89" t="s">
+        <v>1433</v>
+      </c>
+      <c r="F312" s="89" t="s">
+        <v>1438</v>
+      </c>
+      <c r="G312" s="96" t="s">
+        <v>1439</v>
+      </c>
+      <c r="H312" s="89" t="s">
+        <v>1440</v>
+      </c>
+      <c r="I312" s="90" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J312" s="90"/>
+      <c r="K312" s="90"/>
+      <c r="L312" s="90"/>
+      <c r="M312" s="91"/>
+      <c r="N312" s="92"/>
+      <c r="O312" s="92"/>
+      <c r="P312" s="92"/>
+      <c r="Q312" s="92"/>
+      <c r="R312" s="92"/>
+      <c r="S312" s="92"/>
+      <c r="T312" s="92"/>
+    </row>
+    <row r="313" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A313" s="89" t="s">
+        <v>1441</v>
+      </c>
+      <c r="B313" s="89" t="s">
+        <v>135</v>
+      </c>
+      <c r="C313" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D313" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E313" s="89" t="s">
+        <v>1433</v>
+      </c>
+      <c r="F313" s="89" t="s">
+        <v>1442</v>
+      </c>
+      <c r="G313" s="96" t="s">
+        <v>1443</v>
+      </c>
+      <c r="H313" s="89" t="s">
+        <v>1444</v>
+      </c>
+      <c r="I313" s="90" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J313" s="90"/>
+      <c r="K313" s="90"/>
+      <c r="L313" s="90"/>
+      <c r="M313" s="91"/>
+      <c r="N313" s="92"/>
+      <c r="O313" s="92"/>
+      <c r="P313" s="92"/>
+      <c r="Q313" s="92"/>
+      <c r="R313" s="92"/>
+      <c r="S313" s="92"/>
+      <c r="T313" s="92"/>
+    </row>
+    <row r="314" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A314" s="89" t="s">
+        <v>1445</v>
+      </c>
+      <c r="B314" s="89" t="s">
+        <v>41</v>
+      </c>
+      <c r="C314" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D314" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E314" s="89" t="s">
+        <v>206</v>
+      </c>
+      <c r="F314" s="95" t="s">
+        <v>1446</v>
+      </c>
+      <c r="G314" s="89" t="s">
+        <v>1447</v>
+      </c>
+      <c r="H314" s="89" t="s">
+        <v>1448</v>
+      </c>
+      <c r="I314" s="90" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J314" s="90"/>
+      <c r="K314" s="90"/>
+      <c r="L314" s="90"/>
+      <c r="M314" s="91"/>
+      <c r="N314" s="92"/>
+      <c r="O314" s="92"/>
+      <c r="P314" s="92"/>
+      <c r="Q314" s="92"/>
+      <c r="R314" s="92"/>
+      <c r="S314" s="92"/>
+      <c r="T314" s="92"/>
+    </row>
+    <row r="315" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A315" s="89" t="s">
+        <v>1449</v>
+      </c>
+      <c r="B315" s="89" t="s">
+        <v>41</v>
+      </c>
+      <c r="C315" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D315" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E315" s="89" t="s">
+        <v>1450</v>
+      </c>
+      <c r="F315" s="95" t="s">
+        <v>1451</v>
+      </c>
+      <c r="G315" s="89" t="s">
+        <v>1452</v>
+      </c>
+      <c r="H315" s="89" t="s">
+        <v>1453</v>
+      </c>
+      <c r="I315" s="90" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J315" s="90"/>
+      <c r="K315" s="90"/>
+      <c r="L315" s="90"/>
+      <c r="M315" s="91"/>
+      <c r="N315" s="92"/>
+      <c r="O315" s="92"/>
+      <c r="P315" s="92"/>
+      <c r="Q315" s="92"/>
+      <c r="R315" s="92"/>
+      <c r="S315" s="92"/>
+      <c r="T315" s="92"/>
+    </row>
+    <row r="316" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A316" s="89" t="s">
+        <v>1454</v>
+      </c>
+      <c r="B316" s="89" t="s">
+        <v>41</v>
+      </c>
+      <c r="C316" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D316" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E316" s="89" t="s">
+        <v>830</v>
+      </c>
+      <c r="F316" s="95" t="s">
+        <v>1455</v>
+      </c>
+      <c r="G316" s="89" t="s">
+        <v>1456</v>
+      </c>
+      <c r="H316" s="89" t="s">
+        <v>1457</v>
+      </c>
+      <c r="I316" s="90" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J316" s="90"/>
+      <c r="K316" s="90"/>
+      <c r="L316" s="90"/>
+      <c r="M316" s="91"/>
+      <c r="N316" s="92"/>
+      <c r="O316" s="92"/>
+      <c r="P316" s="92"/>
+      <c r="Q316" s="92"/>
+      <c r="R316" s="92"/>
+      <c r="S316" s="92"/>
+      <c r="T316" s="92"/>
+    </row>
+    <row r="317" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A317" s="89" t="s">
+        <v>1458</v>
+      </c>
+      <c r="B317" s="89" t="s">
+        <v>418</v>
+      </c>
+      <c r="C317" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D317" s="89" t="s">
+        <v>1459</v>
+      </c>
+      <c r="E317" s="90"/>
+      <c r="F317" s="95" t="s">
+        <v>1460</v>
+      </c>
+      <c r="G317" s="89" t="s">
+        <v>1461</v>
+      </c>
+      <c r="H317" s="89" t="s">
+        <v>1462</v>
+      </c>
+      <c r="I317" s="90">
+        <v>0</v>
+      </c>
+      <c r="J317" s="90"/>
+      <c r="K317" s="90"/>
+      <c r="L317" s="90"/>
+      <c r="M317" s="91"/>
+      <c r="N317" s="92"/>
+      <c r="O317" s="92"/>
+      <c r="P317" s="92"/>
+      <c r="Q317" s="92"/>
+      <c r="R317" s="92"/>
+      <c r="S317" s="92"/>
+      <c r="T317" s="92"/>
+    </row>
+    <row r="318" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A318" s="89" t="s">
+        <v>1463</v>
+      </c>
+      <c r="B318" s="89" t="s">
+        <v>41</v>
+      </c>
+      <c r="C318" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D318" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E318" s="89" t="s">
+        <v>1428</v>
+      </c>
+      <c r="F318" s="89" t="s">
+        <v>1464</v>
+      </c>
+      <c r="G318" s="89" t="s">
+        <v>1465</v>
+      </c>
+      <c r="H318" s="89" t="s">
+        <v>1466</v>
+      </c>
+      <c r="I318" s="90" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J318" s="90"/>
+      <c r="K318" s="90"/>
+      <c r="L318" s="90"/>
+      <c r="M318" s="91"/>
+      <c r="N318" s="92"/>
+      <c r="O318" s="92"/>
+      <c r="P318" s="92"/>
+      <c r="Q318" s="92"/>
+      <c r="R318" s="92"/>
+      <c r="S318" s="92"/>
+      <c r="T318" s="92"/>
+    </row>
+    <row r="319" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A319" s="89" t="s">
+        <v>1467</v>
+      </c>
+      <c r="B319" s="89" t="s">
+        <v>418</v>
+      </c>
+      <c r="C319" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D319" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E319" s="89" t="s">
+        <v>1468</v>
+      </c>
+      <c r="F319" s="95" t="s">
+        <v>1469</v>
+      </c>
+      <c r="G319" s="89" t="s">
+        <v>1470</v>
+      </c>
+      <c r="H319" s="89" t="s">
+        <v>1471</v>
+      </c>
+      <c r="I319" s="90">
+        <v>0</v>
+      </c>
+      <c r="J319" s="90"/>
+      <c r="K319" s="90"/>
+      <c r="L319" s="90"/>
+      <c r="M319" s="91"/>
+      <c r="N319" s="92"/>
+      <c r="O319" s="92"/>
+      <c r="P319" s="92"/>
+      <c r="Q319" s="92"/>
+      <c r="R319" s="92"/>
+      <c r="S319" s="92"/>
+      <c r="T319" s="92"/>
+    </row>
+    <row r="320" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A320" s="89" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B320" s="89" t="s">
+        <v>418</v>
+      </c>
+      <c r="C320" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D320" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E320" s="89" t="s">
+        <v>1473</v>
+      </c>
+      <c r="F320" s="97" t="s">
+        <v>1474</v>
+      </c>
+      <c r="G320" s="89" t="s">
+        <v>1475</v>
+      </c>
+      <c r="H320" s="89" t="s">
+        <v>1476</v>
+      </c>
+      <c r="I320" s="90">
+        <v>0</v>
+      </c>
+      <c r="J320" s="90"/>
+      <c r="K320" s="90"/>
+      <c r="L320" s="90"/>
+      <c r="M320" s="91"/>
+      <c r="N320" s="92"/>
+      <c r="O320" s="92"/>
+      <c r="P320" s="92"/>
+      <c r="Q320" s="92"/>
+      <c r="R320" s="92"/>
+      <c r="S320" s="92"/>
+      <c r="T320" s="92"/>
+    </row>
+    <row r="321" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A321" s="89" t="s">
+        <v>1477</v>
+      </c>
+      <c r="B321" s="89" t="s">
+        <v>418</v>
+      </c>
+      <c r="C321" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D321" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E321" s="89" t="s">
+        <v>1478</v>
+      </c>
+      <c r="F321" s="89" t="s">
+        <v>1479</v>
+      </c>
+      <c r="G321" s="89" t="s">
+        <v>1480</v>
+      </c>
+      <c r="H321" s="89" t="s">
+        <v>1481</v>
+      </c>
+      <c r="I321" s="90"/>
+      <c r="J321" s="90"/>
+      <c r="K321" s="90"/>
+      <c r="L321" s="90"/>
+      <c r="M321" s="91"/>
+      <c r="N321" s="92"/>
+      <c r="O321" s="92"/>
+      <c r="P321" s="92"/>
+      <c r="Q321" s="92"/>
+      <c r="R321" s="92"/>
+      <c r="S321" s="92"/>
+      <c r="T321" s="92"/>
+    </row>
+    <row r="322" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A322" s="89" t="s">
+        <v>1482</v>
+      </c>
+      <c r="B322" s="89" t="s">
+        <v>418</v>
+      </c>
+      <c r="C322" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D322" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E322" s="89" t="s">
+        <v>1478</v>
+      </c>
+      <c r="F322" s="89" t="s">
+        <v>1483</v>
+      </c>
+      <c r="G322" s="89" t="s">
+        <v>1484</v>
+      </c>
+      <c r="H322" s="89" t="s">
+        <v>1485</v>
+      </c>
+      <c r="I322" s="90"/>
+      <c r="J322" s="90"/>
+      <c r="K322" s="90"/>
+      <c r="L322" s="90"/>
+      <c r="M322" s="91"/>
+      <c r="N322" s="92"/>
+      <c r="O322" s="92"/>
+      <c r="P322" s="92"/>
+      <c r="Q322" s="92"/>
+      <c r="R322" s="92"/>
+      <c r="S322" s="92"/>
+      <c r="T322" s="92"/>
+    </row>
+    <row r="323" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A323" s="89" t="s">
+        <v>1486</v>
+      </c>
+      <c r="B323" s="89" t="s">
+        <v>418</v>
+      </c>
+      <c r="C323" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D323" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E323" s="89" t="s">
+        <v>1478</v>
+      </c>
+      <c r="F323" s="89" t="s">
+        <v>1487</v>
+      </c>
+      <c r="G323" s="89" t="s">
+        <v>1488</v>
+      </c>
+      <c r="H323" s="89" t="s">
+        <v>1489</v>
+      </c>
+      <c r="I323" s="90"/>
+      <c r="J323" s="90"/>
+      <c r="K323" s="90"/>
+      <c r="L323" s="90"/>
+      <c r="M323" s="91"/>
+      <c r="N323" s="92"/>
+      <c r="O323" s="92"/>
+      <c r="P323" s="92"/>
+      <c r="Q323" s="92"/>
+      <c r="R323" s="92"/>
+      <c r="S323" s="92"/>
+      <c r="T323" s="92"/>
+    </row>
+    <row r="324" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A324" s="89" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B324" s="89" t="s">
+        <v>418</v>
+      </c>
+      <c r="C324" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D324" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E324" s="89" t="s">
+        <v>1478</v>
+      </c>
+      <c r="F324" s="89" t="s">
+        <v>1491</v>
+      </c>
+      <c r="G324" s="89" t="s">
+        <v>1492</v>
+      </c>
+      <c r="H324" s="89" t="s">
+        <v>1493</v>
+      </c>
+      <c r="I324" s="90"/>
+      <c r="J324" s="90"/>
+      <c r="K324" s="90"/>
+      <c r="L324" s="90"/>
+      <c r="M324" s="91"/>
+      <c r="N324" s="92"/>
+      <c r="O324" s="92"/>
+      <c r="P324" s="92"/>
+      <c r="Q324" s="92"/>
+      <c r="R324" s="92"/>
+      <c r="S324" s="92"/>
+      <c r="T324" s="92"/>
+    </row>
+    <row r="325" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A325" s="89" t="s">
+        <v>1494</v>
+      </c>
+      <c r="B325" s="89" t="s">
+        <v>418</v>
+      </c>
+      <c r="C325" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D325" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E325" s="90"/>
+      <c r="F325" s="89" t="s">
+        <v>1495</v>
+      </c>
+      <c r="G325" s="89" t="s">
+        <v>1496</v>
+      </c>
+      <c r="H325" s="89" t="s">
+        <v>1497</v>
+      </c>
+      <c r="I325" s="90">
+        <v>1</v>
+      </c>
+      <c r="J325" s="89" t="s">
+        <v>1498</v>
+      </c>
+      <c r="K325" s="90"/>
+      <c r="L325" s="90"/>
+      <c r="M325" s="91"/>
+      <c r="N325" s="92"/>
+      <c r="O325" s="92"/>
+      <c r="P325" s="92"/>
+      <c r="Q325" s="92"/>
+      <c r="R325" s="92"/>
+      <c r="S325" s="92"/>
+      <c r="T325" s="92"/>
+    </row>
+    <row r="326" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A326" s="89" t="s">
+        <v>1499</v>
+      </c>
+      <c r="B326" s="89" t="s">
+        <v>418</v>
+      </c>
+      <c r="C326" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D326" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E326" s="89" t="s">
+        <v>1478</v>
+      </c>
+      <c r="F326" s="89" t="s">
+        <v>1500</v>
+      </c>
+      <c r="G326" s="89" t="s">
+        <v>1501</v>
+      </c>
+      <c r="H326" s="89" t="s">
+        <v>1502</v>
+      </c>
+      <c r="I326" s="90">
+        <v>0</v>
+      </c>
+      <c r="J326" s="90"/>
+      <c r="K326" s="90"/>
+      <c r="L326" s="90"/>
+      <c r="M326" s="91"/>
+      <c r="N326" s="92"/>
+      <c r="O326" s="92"/>
+      <c r="P326" s="92"/>
+      <c r="Q326" s="92"/>
+      <c r="R326" s="92"/>
+      <c r="S326" s="92"/>
+      <c r="T326" s="92"/>
+    </row>
+    <row r="327" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A327" s="89" t="s">
+        <v>1503</v>
+      </c>
+      <c r="B327" s="89" t="s">
+        <v>418</v>
+      </c>
+      <c r="C327" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D327" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E327" s="89" t="s">
+        <v>1450</v>
+      </c>
+      <c r="F327" s="89" t="s">
+        <v>1504</v>
+      </c>
+      <c r="G327" s="89" t="s">
+        <v>1505</v>
+      </c>
+      <c r="H327" s="89" t="s">
+        <v>1506</v>
+      </c>
+      <c r="I327" s="90">
+        <v>0</v>
+      </c>
+      <c r="J327" s="90"/>
+      <c r="K327" s="90"/>
+      <c r="L327" s="90"/>
+      <c r="M327" s="91"/>
+      <c r="N327" s="92"/>
+      <c r="O327" s="92"/>
+      <c r="P327" s="92"/>
+      <c r="Q327" s="92"/>
+      <c r="R327" s="92"/>
+      <c r="S327" s="92"/>
+      <c r="T327" s="92"/>
+    </row>
+    <row r="328" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A328" s="89" t="s">
+        <v>1507</v>
+      </c>
+      <c r="B328" s="89" t="s">
+        <v>41</v>
+      </c>
+      <c r="C328" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D328" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E328" s="89" t="s">
+        <v>830</v>
+      </c>
+      <c r="F328" s="89" t="s">
+        <v>1508</v>
+      </c>
+      <c r="G328" s="89" t="s">
+        <v>1509</v>
+      </c>
+      <c r="H328" s="89" t="s">
+        <v>1510</v>
+      </c>
+      <c r="I328" s="90" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J328" s="90"/>
+      <c r="K328" s="90"/>
+      <c r="L328" s="90"/>
+      <c r="M328" s="91"/>
+      <c r="N328" s="92"/>
+      <c r="O328" s="92"/>
+      <c r="P328" s="92"/>
+      <c r="Q328" s="92"/>
+      <c r="R328" s="92"/>
+      <c r="S328" s="92"/>
+      <c r="T328" s="92"/>
+    </row>
+    <row r="329" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A329" s="89" t="s">
+        <v>1511</v>
+      </c>
+      <c r="B329" s="89" t="s">
+        <v>418</v>
+      </c>
+      <c r="C329" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D329" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E329" s="89" t="s">
+        <v>1450</v>
+      </c>
+      <c r="F329" s="89" t="s">
+        <v>1512</v>
+      </c>
+      <c r="G329" s="89" t="s">
+        <v>1513</v>
+      </c>
+      <c r="H329" s="89" t="s">
+        <v>1514</v>
+      </c>
+      <c r="I329" s="90">
+        <v>0</v>
+      </c>
+      <c r="J329" s="90"/>
+      <c r="K329" s="90"/>
+      <c r="L329" s="90"/>
+      <c r="M329" s="91"/>
+      <c r="N329" s="92"/>
+      <c r="O329" s="92"/>
+      <c r="P329" s="92"/>
+      <c r="Q329" s="92"/>
+      <c r="R329" s="92"/>
+      <c r="S329" s="92"/>
+      <c r="T329" s="92"/>
+    </row>
+    <row r="330" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A330" s="89" t="s">
+        <v>1515</v>
+      </c>
+      <c r="B330" s="89" t="s">
+        <v>418</v>
+      </c>
+      <c r="C330" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D330" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E330" s="89" t="s">
+        <v>1516</v>
+      </c>
+      <c r="F330" s="89" t="s">
+        <v>1517</v>
+      </c>
+      <c r="G330" s="89" t="s">
+        <v>1518</v>
+      </c>
+      <c r="H330" s="89" t="s">
+        <v>1519</v>
+      </c>
+      <c r="I330" s="90">
+        <v>0</v>
+      </c>
+      <c r="J330" s="90"/>
+      <c r="K330" s="90"/>
+      <c r="L330" s="90"/>
+      <c r="M330" s="91"/>
+      <c r="N330" s="92"/>
+      <c r="O330" s="92"/>
+      <c r="P330" s="92"/>
+      <c r="Q330" s="92"/>
+      <c r="R330" s="92"/>
+      <c r="S330" s="92"/>
+      <c r="T330" s="92"/>
+    </row>
+    <row r="331" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A331" s="89" t="s">
+        <v>1535</v>
+      </c>
+      <c r="B331" s="89" t="s">
+        <v>418</v>
+      </c>
+      <c r="C331" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D331" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E331" s="89" t="s">
+        <v>1415</v>
+      </c>
+      <c r="F331" s="89" t="s">
+        <v>1520</v>
+      </c>
+      <c r="G331" s="89" t="s">
+        <v>1521</v>
+      </c>
+      <c r="H331" s="89" t="s">
+        <v>1522</v>
+      </c>
+      <c r="I331" s="90" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J331" s="90"/>
+      <c r="K331" s="90"/>
+      <c r="L331" s="90"/>
+      <c r="M331" s="91"/>
+      <c r="N331" s="92"/>
+      <c r="O331" s="92"/>
+      <c r="P331" s="92"/>
+      <c r="Q331" s="92"/>
+      <c r="R331" s="92"/>
+      <c r="S331" s="92"/>
+      <c r="T331" s="92"/>
+    </row>
+    <row r="332" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A332" s="89" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B332" s="89" t="s">
+        <v>41</v>
+      </c>
+      <c r="C332" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D332" s="89" t="s">
+        <v>1459</v>
+      </c>
+      <c r="E332" s="90"/>
+      <c r="F332" s="95" t="s">
+        <v>1524</v>
+      </c>
+      <c r="G332" s="89" t="s">
+        <v>1525</v>
+      </c>
+      <c r="H332" s="89" t="s">
+        <v>1526</v>
+      </c>
+      <c r="I332" s="90" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J332" s="90"/>
+      <c r="K332" s="90"/>
+      <c r="L332" s="90"/>
+      <c r="M332" s="91"/>
+      <c r="N332" s="92"/>
+      <c r="O332" s="92"/>
+      <c r="P332" s="92"/>
+      <c r="Q332" s="92"/>
+      <c r="R332" s="92"/>
+      <c r="S332" s="92"/>
+      <c r="T332" s="92"/>
+    </row>
+    <row r="333" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A333" s="89" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B333" s="89" t="s">
+        <v>418</v>
+      </c>
+      <c r="C333" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D333" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E333" s="89" t="s">
+        <v>1450</v>
+      </c>
+      <c r="F333" s="89" t="s">
+        <v>1528</v>
+      </c>
+      <c r="G333" s="89" t="s">
+        <v>1529</v>
+      </c>
+      <c r="H333" s="89" t="s">
+        <v>1530</v>
+      </c>
+      <c r="I333" s="90">
+        <v>0</v>
+      </c>
+      <c r="J333" s="90"/>
+      <c r="K333" s="90"/>
+      <c r="L333" s="90"/>
+      <c r="M333" s="91"/>
+      <c r="N333" s="92"/>
+      <c r="O333" s="92"/>
+      <c r="P333" s="92"/>
+      <c r="Q333" s="92"/>
+      <c r="R333" s="92"/>
+      <c r="S333" s="92"/>
+      <c r="T333" s="92"/>
+    </row>
+    <row r="334" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A334" s="89" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B334" s="89" t="s">
+        <v>418</v>
+      </c>
+      <c r="C334" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D334" s="89" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E334" s="89" t="s">
+        <v>1450</v>
+      </c>
+      <c r="F334" s="89" t="s">
+        <v>1532</v>
+      </c>
+      <c r="G334" s="89" t="s">
+        <v>1533</v>
+      </c>
+      <c r="H334" s="89" t="s">
+        <v>1534</v>
+      </c>
+      <c r="I334" s="90">
+        <v>0</v>
+      </c>
+      <c r="J334" s="90"/>
+      <c r="K334" s="90"/>
+      <c r="L334" s="90"/>
+      <c r="M334" s="91"/>
+      <c r="N334" s="92"/>
+      <c r="O334" s="92"/>
+      <c r="P334" s="92"/>
+      <c r="Q334" s="92"/>
+      <c r="R334" s="92"/>
+      <c r="S334" s="92"/>
+      <c r="T334" s="92"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J153">

</xml_diff>